<commit_message>
Conduct the sim of 16ggq-1-2
</commit_message>
<xml_diff>
--- a/bin/2d_s_cc/reorganized exp.data.xlsx
+++ b/bin/2d_s_cc/reorganized exp.data.xlsx
@@ -653,9 +653,9 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.000E+00"/>
+    <numFmt numFmtId="166" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -765,8 +765,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -803,8 +820,18 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -827,8 +854,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -851,8 +908,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -952,21 +1011,29 @@
     <xf numFmtId="165" fontId="12" fillId="5" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="12" fillId="6" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="12" fillId="6" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="2" xfId="8" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="3" xfId="9" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="10">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
     <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
     <cellStyle name="20% - Accent3" xfId="4" builtinId="38"/>
     <cellStyle name="20% - Accent4" xfId="5" builtinId="42"/>
     <cellStyle name="20% - Accent6" xfId="7" builtinId="50"/>
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
+    <cellStyle name="Input" xfId="8" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="9" builtinId="21"/>
     <cellStyle name="Style 1" xfId="6"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1637,14 +1704,15 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.28515625" style="18" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" style="18" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="18"/>
+    <col min="3" max="4" width="9.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -2244,23 +2312,23 @@
       <c r="B40" t="s">
         <v>99</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="35">
         <f>C24/1000000/60/(C16*C17/10000)</f>
         <v>8.4395555555555543E-3</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="35">
         <f>C40</f>
         <v>8.4395555555555543E-3</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="35">
         <f t="shared" ref="E40:G40" si="0">D40</f>
         <v>8.4395555555555543E-3</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="35">
         <f t="shared" si="0"/>
         <v>8.4395555555555543E-3</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="35">
         <f t="shared" si="0"/>
         <v>8.4395555555555543E-3</v>
       </c>
@@ -2272,23 +2340,23 @@
       <c r="B41" t="s">
         <v>104</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="35">
         <f>C26+273.15</f>
         <v>305.95490858938018</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="35">
         <f>D26+273.15</f>
         <v>310.69592116787919</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="35">
         <f>E26+273.15</f>
         <v>313.61279404111355</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="35">
         <f>F26+273.15</f>
         <v>319.9632722324157</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="35">
         <f>G26+273.15</f>
         <v>325.43803056208191</v>
       </c>
@@ -2300,23 +2368,23 @@
       <c r="B42" t="s">
         <v>104</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="36">
         <f>C33+273.15</f>
         <v>305.35915961980555</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="36">
         <f>D33+273.15</f>
         <v>309.79188253593401</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="36">
         <f>E33+273.15</f>
         <v>312.35623159324001</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="36">
         <f>F33+273.15</f>
         <v>318.26500700465544</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="36">
         <f>G33+273.15</f>
         <v>323.63862859035953</v>
       </c>
@@ -2333,23 +2401,23 @@
       <c r="B44" t="s">
         <v>99</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="35">
         <f>C29/1000000/60/(C16*C17/10000)</f>
         <v>8.7448888888888889E-3</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="35">
         <f>C44</f>
         <v>8.7448888888888889E-3</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="35">
         <f t="shared" ref="E44:G44" si="1">D44</f>
         <v>8.7448888888888889E-3</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="35">
         <f t="shared" si="1"/>
         <v>8.7448888888888889E-3</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="35">
         <f t="shared" si="1"/>
         <v>8.7448888888888889E-3</v>
       </c>
@@ -2358,23 +2426,23 @@
       <c r="B45" t="s">
         <v>104</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="35">
         <f>C31+273.15</f>
         <v>293.17058482349387</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="35">
         <f>D31+273.15</f>
         <v>293.16399690708016</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="35">
         <f>E31+273.15</f>
         <v>293.19055520526842</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="35">
         <f>F31+273.15</f>
         <v>293.11519271759857</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="35">
         <f>G31+273.15</f>
         <v>293.68159105444261</v>
       </c>
@@ -2383,23 +2451,23 @@
       <c r="B46" t="s">
         <v>104</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="36">
         <f>C34+273.15</f>
         <v>294.29682689366177</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="36">
         <f>D34+273.15</f>
         <v>294.21664608339694</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="36">
         <f>E34+273.15</f>
         <v>294.35225488233681</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="36">
         <f>F34+273.15</f>
         <v>294.57886130730265</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="36">
         <f>G34+273.15</f>
         <v>295.14325006184663</v>
       </c>
@@ -2411,23 +2479,23 @@
       <c r="B47" t="s">
         <v>103</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="36">
         <f>C35/3600</f>
         <v>1.0791274666666665E-3</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="36">
         <f>D35/3600</f>
         <v>1.5744281599999997E-3</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="36">
         <f>E35/3600</f>
         <v>1.9465498666666667E-3</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="36">
         <f>F35/3600</f>
         <v>2.9802457599999999E-3</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="36">
         <f>G35/3600</f>
         <v>3.9183833599999995E-3</v>
       </c>
@@ -2437,7 +2505,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="16" customFormat="1">
+    <row r="49" spans="1:7" s="16" customFormat="1">
       <c r="A49" s="16" t="s">
         <v>102</v>
       </c>
@@ -2447,8 +2515,11 @@
       <c r="C49" s="16">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" s="16" customFormat="1">
+      <c r="D49" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" s="16" customFormat="1">
       <c r="A50" s="34" t="s">
         <v>118</v>
       </c>
@@ -2458,8 +2529,11 @@
       <c r="C50" s="16">
         <v>304.49</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" s="16" customFormat="1">
+      <c r="D50" s="16">
+        <v>308.7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" s="16" customFormat="1">
       <c r="A51" s="34" t="s">
         <v>119</v>
       </c>
@@ -2469,8 +2543,11 @@
       <c r="C51" s="16">
         <v>294.58999999999997</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" s="16" customFormat="1">
+      <c r="D51" s="16">
+        <v>295.12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" s="16" customFormat="1">
       <c r="A52" s="16" t="s">
         <v>72</v>
       </c>
@@ -2480,6 +2557,12 @@
       <c r="C52" s="33">
         <v>9.6889999999999997E-4</v>
       </c>
+      <c r="D52" s="33">
+        <v>1.387E-3</v>
+      </c>
+      <c r="E52" s="33"/>
+      <c r="F52" s="33"/>
+      <c r="G52" s="33"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
Add the case of 16ggq-1-3.cas
</commit_message>
<xml_diff>
--- a/bin/2d_s_cc/reorganized exp.data.xlsx
+++ b/bin/2d_s_cc/reorganized exp.data.xlsx
@@ -218,7 +218,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="123">
   <si>
     <t>Wang K Y, Chung T S, Gryta M. Chem. Eng. Sci., 2008, 63: 2587-2594</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -645,6 +645,9 @@
   <si>
     <t>16GGQ-1-</t>
   </si>
+  <si>
+    <t>Divergence</t>
+  </si>
 </sst>
 </file>
 
@@ -655,7 +658,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -782,6 +785,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -911,7 +921,7 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1021,6 +1031,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="3" xfId="9" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1701,10 +1714,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2518,6 +2531,9 @@
       <c r="D49" s="16">
         <v>2</v>
       </c>
+      <c r="E49" s="16">
+        <v>3</v>
+      </c>
     </row>
     <row r="50" spans="1:7" s="16" customFormat="1">
       <c r="A50" s="34" t="s">
@@ -2563,6 +2579,11 @@
       <c r="E52" s="33"/>
       <c r="F52" s="33"/>
       <c r="G52" s="33"/>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="E53" s="37" t="s">
+        <v>122</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
Complete the case of 16ggq-1-3
</commit_message>
<xml_diff>
--- a/bin/2d_s_cc/reorganized exp.data.xlsx
+++ b/bin/2d_s_cc/reorganized exp.data.xlsx
@@ -218,7 +218,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="122">
   <si>
     <t>Wang K Y, Chung T S, Gryta M. Chem. Eng. Sci., 2008, 63: 2587-2594</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -644,9 +644,6 @@
   </si>
   <si>
     <t>16GGQ-1-</t>
-  </si>
-  <si>
-    <t>Divergence</t>
   </si>
 </sst>
 </file>
@@ -1717,15 +1714,15 @@
   <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.28515625" style="18" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" style="18" customWidth="1"/>
-    <col min="3" max="4" width="9.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="18"/>
+    <col min="3" max="5" width="9.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -2548,6 +2545,9 @@
       <c r="D50" s="16">
         <v>308.7</v>
       </c>
+      <c r="E50" s="16">
+        <v>311.29000000000002</v>
+      </c>
     </row>
     <row r="51" spans="1:7" s="16" customFormat="1">
       <c r="A51" s="34" t="s">
@@ -2562,6 +2562,9 @@
       <c r="D51" s="16">
         <v>295.12</v>
       </c>
+      <c r="E51" s="16">
+        <v>295.47000000000003</v>
+      </c>
     </row>
     <row r="52" spans="1:7" s="16" customFormat="1">
       <c r="A52" s="16" t="s">
@@ -2576,14 +2579,14 @@
       <c r="D52" s="33">
         <v>1.387E-3</v>
       </c>
-      <c r="E52" s="33"/>
+      <c r="E52" s="33">
+        <v>1.7049999999999999E-3</v>
+      </c>
       <c r="F52" s="33"/>
       <c r="G52" s="33"/>
     </row>
     <row r="53" spans="1:7">
-      <c r="E53" s="37" t="s">
-        <v>122</v>
-      </c>
+      <c r="E53" s="37"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
Conduct the sim for the case of 16ggq-1-4 The case can be done when the relax factor of momentum is changed from 0.7 to 0.4. It looks the new code has a little improvement.
</commit_message>
<xml_diff>
--- a/bin/2d_s_cc/reorganized exp.data.xlsx
+++ b/bin/2d_s_cc/reorganized exp.data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="17235" windowHeight="8955" activeTab="1"/>
@@ -1713,16 +1713,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.28515625" style="18" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" style="18" customWidth="1"/>
-    <col min="3" max="5" width="9.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="18"/>
+    <col min="3" max="6" width="9.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -2531,6 +2531,9 @@
       <c r="E49" s="16">
         <v>3</v>
       </c>
+      <c r="F49" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="50" spans="1:7" s="16" customFormat="1">
       <c r="A50" s="34" t="s">
@@ -2548,6 +2551,9 @@
       <c r="E50" s="16">
         <v>311.29000000000002</v>
       </c>
+      <c r="F50" s="16">
+        <v>316.98</v>
+      </c>
     </row>
     <row r="51" spans="1:7" s="16" customFormat="1">
       <c r="A51" s="34" t="s">
@@ -2565,6 +2571,9 @@
       <c r="E51" s="16">
         <v>295.47000000000003</v>
       </c>
+      <c r="F51" s="16">
+        <v>296.06</v>
+      </c>
     </row>
     <row r="52" spans="1:7" s="16" customFormat="1">
       <c r="A52" s="16" t="s">
@@ -2582,7 +2591,9 @@
       <c r="E52" s="33">
         <v>1.7049999999999999E-3</v>
       </c>
-      <c r="F52" s="33"/>
+      <c r="F52" s="33">
+        <v>2.317E-3</v>
+      </c>
       <c r="G52" s="33"/>
     </row>
     <row r="53" spans="1:7">

</xml_diff>

<commit_message>
Set the relax factor of momentum from 0.7 to 0.4 Conduct the sim for the case of 16ggq-1-4
</commit_message>
<xml_diff>
--- a/bin/2d_s_cc/reorganized exp.data.xlsx
+++ b/bin/2d_s_cc/reorganized exp.data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="17235" windowHeight="8955" activeTab="1"/>
@@ -1713,16 +1713,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.28515625" style="18" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" style="18" customWidth="1"/>
-    <col min="3" max="5" width="9.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="18"/>
+    <col min="3" max="6" width="9.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -2531,6 +2531,9 @@
       <c r="E49" s="16">
         <v>3</v>
       </c>
+      <c r="F49" s="16">
+        <v>4</v>
+      </c>
     </row>
     <row r="50" spans="1:7" s="16" customFormat="1">
       <c r="A50" s="34" t="s">
@@ -2548,6 +2551,9 @@
       <c r="E50" s="16">
         <v>311.29000000000002</v>
       </c>
+      <c r="F50" s="16">
+        <v>316.91000000000003</v>
+      </c>
     </row>
     <row r="51" spans="1:7" s="16" customFormat="1">
       <c r="A51" s="34" t="s">
@@ -2565,6 +2571,9 @@
       <c r="E51" s="16">
         <v>295.47000000000003</v>
       </c>
+      <c r="F51" s="16">
+        <v>296.13</v>
+      </c>
     </row>
     <row r="52" spans="1:7" s="16" customFormat="1">
       <c r="A52" s="16" t="s">
@@ -2582,7 +2591,9 @@
       <c r="E52" s="33">
         <v>1.7049999999999999E-3</v>
       </c>
-      <c r="F52" s="33"/>
+      <c r="F52" s="33">
+        <v>2.3280000000000002E-3</v>
+      </c>
       <c r="G52" s="33"/>
     </row>
     <row r="53" spans="1:7">

</xml_diff>

<commit_message>
Add a switch in the function of HeatFlux to output the preferred heat flux
</commit_message>
<xml_diff>
--- a/bin/2d_s_cc/reorganized exp.data.xlsx
+++ b/bin/2d_s_cc/reorganized exp.data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="17235" windowHeight="8955" activeTab="1"/>
@@ -218,7 +218,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="122">
   <si>
     <t>Wang K Y, Chung T S, Gryta M. Chem. Eng. Sci., 2008, 63: 2587-2594</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -1713,8 +1713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2433,6 +2433,9 @@
       </c>
     </row>
     <row r="45" spans="1:7" customFormat="1">
+      <c r="A45" t="s">
+        <v>116</v>
+      </c>
       <c r="B45" t="s">
         <v>104</v>
       </c>
@@ -2458,6 +2461,9 @@
       </c>
     </row>
     <row r="46" spans="1:7" customFormat="1">
+      <c r="A46" t="s">
+        <v>115</v>
+      </c>
       <c r="B46" t="s">
         <v>104</v>
       </c>
@@ -2552,7 +2558,7 @@
         <v>311.29000000000002</v>
       </c>
       <c r="F50" s="16">
-        <v>316.91000000000003</v>
+        <v>317.02</v>
       </c>
     </row>
     <row r="51" spans="1:7" s="16" customFormat="1">
@@ -2572,7 +2578,7 @@
         <v>295.47000000000003</v>
       </c>
       <c r="F51" s="16">
-        <v>296.13</v>
+        <v>296.02</v>
       </c>
     </row>
     <row r="52" spans="1:7" s="16" customFormat="1">
@@ -2592,7 +2598,7 @@
         <v>1.7049999999999999E-3</v>
       </c>
       <c r="F52" s="33">
-        <v>2.3280000000000002E-3</v>
+        <v>2.3249999999999998E-3</v>
       </c>
       <c r="G52" s="33"/>
     </row>

</xml_diff>

<commit_message>
Set the MD coefficient as 9.5e-7
</commit_message>
<xml_diff>
--- a/bin/2d_s_cc/reorganized exp.data.xlsx
+++ b/bin/2d_s_cc/reorganized exp.data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="17235" windowHeight="8955" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="17235" windowHeight="8955" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Wang&amp;Chung2008CES" sheetId="1" r:id="rId1"/>
     <sheet name="Yao2016(preparing)" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="SimRecords" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -218,7 +219,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="135">
   <si>
     <t>Wang K Y, Chung T S, Gryta M. Chem. Eng. Sci., 2008, 63: 2587-2594</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -644,6 +645,45 @@
   </si>
   <si>
     <t>16GGQ-1-</t>
+  </si>
+  <si>
+    <t>16GGQ-2-</t>
+  </si>
+  <si>
+    <t>Calc. permeation flux</t>
+  </si>
+  <si>
+    <t>Feed-side outlet (facet avg. temp.)</t>
+  </si>
+  <si>
+    <t>Perm-side outlet (facet avg. temp.)</t>
+  </si>
+  <si>
+    <t>16GGQ-2-5</t>
+  </si>
+  <si>
+    <t>case file</t>
+  </si>
+  <si>
+    <t>Adj. Param.</t>
+  </si>
+  <si>
+    <t>MDC</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>T1out</t>
+  </si>
+  <si>
+    <t>T0out</t>
+  </si>
+  <si>
+    <t>Facet Avg. UDMI(1)</t>
+  </si>
+  <si>
+    <t>JM</t>
   </si>
 </sst>
 </file>
@@ -918,7 +958,7 @@
     <xf numFmtId="0" fontId="15" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1031,6 +1071,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="7" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1711,15 +1760,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" style="18" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" style="18" customWidth="1"/>
     <col min="3" max="6" width="9.28515625" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="18"/>
@@ -2604,6 +2653,59 @@
     </row>
     <row r="53" spans="1:7">
       <c r="E53" s="37"/>
+    </row>
+    <row r="54" spans="1:7" s="38" customFormat="1">
+      <c r="A54" s="38" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="G54" s="38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" s="38" customFormat="1">
+      <c r="A55" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="B55" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="G55" s="38">
+        <v>322.20999999999998</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" s="38" customFormat="1">
+      <c r="A56" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="B56" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="G56" s="38">
+        <v>297.17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" s="38" customFormat="1">
+      <c r="A57" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57" s="38" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" s="38" customFormat="1">
+      <c r="A58" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="B58" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="G58" s="38">
+        <f>SimRecords!B8</f>
+        <v>7.7795E-3</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -2616,7 +2718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N24" sqref="N24:R28"/>
     </sheetView>
   </sheetViews>
@@ -3244,4 +3346,84 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="40">
+        <v>2.3999999999999999E-6</v>
+      </c>
+      <c r="C3" s="40">
+        <v>4.7999999999999998E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="B5">
+        <v>322.20999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6">
+        <v>297.17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7">
+        <v>15.558999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8">
+        <f>B7*0.0005</f>
+        <v>7.7795E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add FLUENT case and date files, which produced the results in "reorganized exp.data.xlsx"
</commit_message>
<xml_diff>
--- a/bin/2d_s_cc/reorganized exp.data.xlsx
+++ b/bin/2d_s_cc/reorganized exp.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="17235" windowHeight="8955" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="17235" windowHeight="8955" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Wang&amp;Chung2008CES" sheetId="1" r:id="rId1"/>
@@ -219,7 +219,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="139">
   <si>
     <t>Wang K Y, Chung T S, Gryta M. Chem. Eng. Sci., 2008, 63: 2587-2594</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -650,9 +650,6 @@
     <t>16GGQ-2-</t>
   </si>
   <si>
-    <t>Calc. permeation flux</t>
-  </si>
-  <si>
     <t>Feed-side outlet (facet avg. temp.)</t>
   </si>
   <si>
@@ -684,6 +681,21 @@
   </si>
   <si>
     <t>JM</t>
+  </si>
+  <si>
+    <t>kg/m3-s</t>
+  </si>
+  <si>
+    <t>RSMD</t>
+  </si>
+  <si>
+    <t>dT0/T0 = (T0_exp - T0_sim)/T0_exp</t>
+  </si>
+  <si>
+    <t>dT1/T1 = (T1_exp - T1_sim)/T1_exp</t>
+  </si>
+  <si>
+    <t>dJM/JM</t>
   </si>
 </sst>
 </file>
@@ -695,7 +707,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -829,6 +841,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -932,7 +952,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -957,8 +977,9 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1082,13 +1103,23 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="2" xfId="10" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="18" fillId="8" borderId="2" xfId="10" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="11">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
     <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
     <cellStyle name="20% - Accent3" xfId="4" builtinId="38"/>
     <cellStyle name="20% - Accent4" xfId="5" builtinId="42"/>
     <cellStyle name="20% - Accent6" xfId="7" builtinId="50"/>
+    <cellStyle name="Calculation" xfId="10" builtinId="22"/>
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Input" xfId="8" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -1098,6 +1129,139 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-SG"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:xVal>
+            <c:numRef>
+              <c:f>SimRecords!$B$3:$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>9.5000000000000001E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.7999999999999998E-6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>SimRecords!$B$8:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.8479500000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5685500000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.7795E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.485995E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="91719168"/>
+        <c:axId val="91695744"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="91719168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="91695744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="91695744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="91719168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1387,8 +1551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1048576"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1760,17 +1924,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L58"/>
+  <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.7109375" style="18" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" style="18" customWidth="1"/>
-    <col min="3" max="6" width="9.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.28515625" style="18" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
@@ -2661,56 +2827,226 @@
       <c r="B54" s="38" t="s">
         <v>122</v>
       </c>
+      <c r="C54" s="38">
+        <v>1</v>
+      </c>
+      <c r="D54" s="38">
+        <v>2</v>
+      </c>
+      <c r="E54" s="38">
+        <v>3</v>
+      </c>
+      <c r="F54" s="38">
+        <v>4</v>
+      </c>
       <c r="G54" s="38">
         <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:7" s="38" customFormat="1">
       <c r="A55" s="38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B55" s="38" t="s">
         <v>104</v>
       </c>
+      <c r="C55" s="38">
+        <v>305.07</v>
+      </c>
+      <c r="D55" s="38">
+        <v>309.42</v>
+      </c>
+      <c r="E55" s="38">
+        <v>312.06</v>
+      </c>
+      <c r="F55" s="38">
+        <v>317.77999999999997</v>
+      </c>
       <c r="G55" s="38">
-        <v>322.20999999999998</v>
+        <f>SimRecords!$B$5</f>
+        <v>322.74</v>
       </c>
     </row>
     <row r="56" spans="1:7" s="38" customFormat="1">
       <c r="A56" s="38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B56" s="38" t="s">
         <v>104</v>
       </c>
+      <c r="C56" s="38">
+        <v>294.04000000000002</v>
+      </c>
+      <c r="D56" s="38">
+        <v>294.45</v>
+      </c>
+      <c r="E56" s="38">
+        <v>294.75</v>
+      </c>
+      <c r="F56" s="38">
+        <v>295.33999999999997</v>
+      </c>
       <c r="G56" s="38">
-        <v>297.17</v>
+        <f>SimRecords!$B$6</f>
+        <v>296.47000000000003</v>
       </c>
     </row>
     <row r="57" spans="1:7" s="38" customFormat="1">
       <c r="A57" s="38" t="s">
-        <v>72</v>
+        <v>132</v>
       </c>
       <c r="B57" s="38" t="s">
-        <v>103</v>
+        <v>134</v>
+      </c>
+      <c r="C57" s="38">
+        <v>2.1501100000000002</v>
+      </c>
+      <c r="D57" s="38">
+        <v>3.1509200000000002</v>
+      </c>
+      <c r="E57" s="38">
+        <v>3.8756499999999998</v>
+      </c>
+      <c r="F57" s="38">
+        <v>5.7749699999999997</v>
+      </c>
+      <c r="G57" s="38">
+        <f>SimRecords!$B$7</f>
+        <v>7.6959</v>
       </c>
     </row>
     <row r="58" spans="1:7" s="38" customFormat="1">
       <c r="A58" s="38" t="s">
-        <v>123</v>
+        <v>72</v>
       </c>
       <c r="B58" s="38" t="s">
         <v>103</v>
       </c>
+      <c r="C58" s="38">
+        <f>C57*0.0005</f>
+        <v>1.0750550000000001E-3</v>
+      </c>
+      <c r="D58" s="38">
+        <f>D57*0.0005</f>
+        <v>1.5754600000000001E-3</v>
+      </c>
+      <c r="E58" s="38">
+        <f>E57*0.0005</f>
+        <v>1.937825E-3</v>
+      </c>
+      <c r="F58" s="38">
+        <f>F57*0.0005</f>
+        <v>2.887485E-3</v>
+      </c>
       <c r="G58" s="38">
-        <f>SimRecords!B8</f>
-        <v>7.7795E-3</v>
+        <f>SimRecords!$B$8</f>
+        <v>3.8479500000000002E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="38" t="s">
+        <v>136</v>
+      </c>
+      <c r="C59" s="42">
+        <f>(C42-C55)/C42</f>
+        <v>9.4694922584141349E-4</v>
+      </c>
+      <c r="D59" s="42">
+        <f>(D42-D55)/D42</f>
+        <v>1.2004269863037987E-3</v>
+      </c>
+      <c r="E59" s="42">
+        <f t="shared" ref="E59:G59" si="2">(E42-E55)/E42</f>
+        <v>9.4837740783661011E-4</v>
+      </c>
+      <c r="F59" s="42">
+        <f t="shared" si="2"/>
+        <v>1.5239093019371039E-3</v>
+      </c>
+      <c r="G59" s="42">
+        <f t="shared" si="2"/>
+        <v>2.7766419425072604E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="C60" s="42">
+        <f>(C46-C56)/C46</f>
+        <v>8.7267979193860639E-4</v>
+      </c>
+      <c r="D60" s="42">
+        <f>(D46-D56)/D46</f>
+        <v>-7.9313634938556589E-4</v>
+      </c>
+      <c r="E60" s="42">
+        <f t="shared" ref="E60:G60" si="3">(E46-E56)/E46</f>
+        <v>-1.3512555486357143E-3</v>
+      </c>
+      <c r="F60" s="42">
+        <f t="shared" si="3"/>
+        <v>-2.5838197938558632E-3</v>
+      </c>
+      <c r="G60" s="42">
+        <f t="shared" si="3"/>
+        <v>-4.4952745416857081E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="38" t="s">
+        <v>138</v>
+      </c>
+      <c r="C61" s="43">
+        <f>(C47-C58)/C47</f>
+        <v>3.7738513683150884E-3</v>
+      </c>
+      <c r="D61" s="43">
+        <f>(D47-D58)/D47</f>
+        <v>-6.5537445671729399E-4</v>
+      </c>
+      <c r="E61" s="43">
+        <f t="shared" ref="E61:G61" si="4">(E47-E58)/E47</f>
+        <v>4.4822209880538222E-3</v>
+      </c>
+      <c r="F61" s="43">
+        <f t="shared" si="4"/>
+        <v>3.1125204922697346E-2</v>
+      </c>
+      <c r="G61" s="43">
+        <f t="shared" si="4"/>
+        <v>1.7975106958396075E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="C62" s="42">
+        <f>SQRT(C59^2+C60^2+C61^2)</f>
+        <v>3.9875101260953968E-3</v>
+      </c>
+      <c r="D62" s="42">
+        <f>SQRT(D59^2+D60^2+D61^2)</f>
+        <v>1.5810141987599514E-3</v>
+      </c>
+      <c r="E62" s="42">
+        <f t="shared" ref="E62:G62" si="5">SQRT(E59^2+E60^2+E61^2)</f>
+        <v>4.7765695065772754E-3</v>
+      </c>
+      <c r="F62" s="42">
+        <f t="shared" si="5"/>
+        <v>3.1269422856323316E-2</v>
+      </c>
+      <c r="G62" s="42">
+        <f t="shared" si="5"/>
+        <v>1.8735573219087726E-2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0.94488188976377963" bottom="0.94488188976377963" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3350,10 +3686,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3361,69 +3697,121 @@
     <col min="1" max="1" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
         <v>127</v>
       </c>
-      <c r="B1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="39" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="39" t="s">
+      <c r="B3" s="41">
+        <v>9.5000000000000001E-7</v>
+      </c>
+      <c r="C3" s="41">
+        <v>1.1999999999999999E-6</v>
+      </c>
+      <c r="D3" s="40">
+        <v>2.3999999999999999E-6</v>
+      </c>
+      <c r="E3" s="40">
+        <v>4.7999999999999998E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
         <v>129</v>
       </c>
-      <c r="B3" s="40">
-        <v>2.3999999999999999E-6</v>
-      </c>
-      <c r="C3" s="40">
-        <v>4.7999999999999998E-6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="39">
+        <v>322.74</v>
+      </c>
+      <c r="C5" s="39">
+        <v>322.64</v>
+      </c>
+      <c r="D5">
+        <v>322.20999999999998</v>
+      </c>
+      <c r="E5">
+        <v>322.27999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="39" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="39" t="s">
+      <c r="B6" s="39">
+        <v>296.47000000000003</v>
+      </c>
+      <c r="C6" s="39">
+        <v>296.60000000000002</v>
+      </c>
+      <c r="D6">
+        <v>297.17</v>
+      </c>
+      <c r="E6">
+        <v>297.38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="B5">
-        <v>322.20999999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="39" t="s">
-        <v>131</v>
-      </c>
-      <c r="B6">
-        <v>297.17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="39" t="s">
+      <c r="B7" s="39">
+        <v>7.6959</v>
+      </c>
+      <c r="C7" s="39">
+        <v>9.1371000000000002</v>
+      </c>
+      <c r="D7">
+        <v>15.558999999999999</v>
+      </c>
+      <c r="E7">
+        <v>29.719899999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="39" t="s">
         <v>133</v>
-      </c>
-      <c r="B7">
-        <v>15.558999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="39" t="s">
-        <v>134</v>
       </c>
       <c r="B8">
         <f>B7*0.0005</f>
+        <v>3.8479500000000002E-3</v>
+      </c>
+      <c r="C8">
+        <f>C7*0.0005</f>
+        <v>4.5685500000000002E-3</v>
+      </c>
+      <c r="D8">
+        <f>D7*0.0005</f>
         <v>7.7795E-3</v>
+      </c>
+      <c r="E8">
+        <f>E7*0.0005</f>
+        <v>1.485995E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="B10" s="40">
+        <f>(0.003918-C8)*(C3-D3)/(C8-D8)+C3</f>
+        <v>9.5687569099487663E-7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CFD simulation verification with Yao's experiments All results including the sims and exps are collected in the Excel file of "reorganized exp.data.xlsx".
</commit_message>
<xml_diff>
--- a/bin/2d_s_cc/reorganized exp.data.xlsx
+++ b/bin/2d_s_cc/reorganized exp.data.xlsx
@@ -1299,23 +1299,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="170538496"/>
-        <c:axId val="170540032"/>
+        <c:axId val="154027136"/>
+        <c:axId val="154028672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="170538496"/>
+        <c:axId val="154027136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170540032"/>
+        <c:crossAx val="154028672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="170540032"/>
+        <c:axId val="154028672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1323,7 +1323,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170538496"/>
+        <c:crossAx val="154027136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1335,7 +1335,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2886,8 +2886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4520,95 +4520,95 @@
         <v>86</v>
       </c>
       <c r="C41" s="24">
-        <f>C26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" ref="C41:Y41" si="10">C26/1000000/60/(MOD1W*MOD1H/10000)</f>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="D41" s="24">
-        <f>D26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" si="10"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="E41" s="24">
-        <f>E26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" si="10"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="F41" s="24">
-        <f>F26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" si="10"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="G41" s="24">
-        <f>G26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" si="10"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="H41" s="24">
-        <f>H26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" si="10"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="I41" s="24">
-        <f>I26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" si="10"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="J41" s="24">
-        <f>J26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" si="10"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="K41" s="24">
-        <f>K26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" si="10"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="L41" s="24">
-        <f>L26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" si="10"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="M41" s="24">
-        <f>M26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" si="10"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="N41" s="24">
-        <f>N26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" si="10"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="O41" s="24">
-        <f>O26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" si="10"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="P41" s="24">
-        <f>P26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" si="10"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="Q41" s="24">
-        <f>Q26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" si="10"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="R41" s="24">
-        <f>R26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" si="10"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="S41" s="24">
-        <f>S26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" si="10"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="T41" s="24">
-        <f>T26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" si="10"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="U41" s="24">
-        <f>U26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" si="10"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="V41" s="24">
-        <f>V26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" si="10"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="W41" s="24">
-        <f>W26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" si="10"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="X41" s="24">
-        <f>X26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" si="10"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="Y41" s="24">
-        <f>Y26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" si="10"/>
         <v>8.4395555555555543E-3</v>
       </c>
     </row>
@@ -4620,95 +4620,95 @@
         <v>90</v>
       </c>
       <c r="C42" s="24">
-        <f>C30+273.15</f>
+        <f t="shared" ref="C42:Y42" si="11">C30+273.15</f>
         <v>305.95490858938018</v>
       </c>
       <c r="D42" s="24">
-        <f>D30+273.15</f>
+        <f t="shared" si="11"/>
         <v>310.69592116787919</v>
       </c>
       <c r="E42" s="24">
-        <f>E30+273.15</f>
+        <f t="shared" si="11"/>
         <v>313.61279404111355</v>
       </c>
       <c r="F42" s="24">
-        <f>F30+273.15</f>
+        <f t="shared" si="11"/>
         <v>319.9632722324157</v>
       </c>
       <c r="G42" s="24">
-        <f>G30+273.15</f>
+        <f t="shared" si="11"/>
         <v>325.43803056208191</v>
       </c>
       <c r="H42" s="24">
-        <f>H30+273.15</f>
+        <f t="shared" si="11"/>
         <v>319.9632722324157</v>
       </c>
       <c r="I42" s="24">
-        <f>I30+273.15</f>
+        <f t="shared" si="11"/>
         <v>319.8855595510372</v>
       </c>
       <c r="J42" s="24">
-        <f>J30+273.15</f>
+        <f t="shared" si="11"/>
         <v>319.90637697413189</v>
       </c>
       <c r="K42" s="24">
-        <f>K30+273.15</f>
+        <f t="shared" si="11"/>
         <v>319.90971551314635</v>
       </c>
       <c r="L42" s="24">
-        <f>L30+273.15</f>
+        <f t="shared" si="11"/>
         <v>319.94575411738424</v>
       </c>
       <c r="M42" s="24">
-        <f>M30+273.15</f>
+        <f t="shared" si="11"/>
         <v>319.91596078453716</v>
       </c>
       <c r="N42" s="24">
-        <f>N30+273.15</f>
+        <f t="shared" si="11"/>
         <v>319.89779784944972</v>
       </c>
       <c r="O42" s="24">
-        <f>O30+273.15</f>
+        <f t="shared" si="11"/>
         <v>319.9632722324157</v>
       </c>
       <c r="P42" s="24">
-        <f>P30+273.15</f>
+        <f t="shared" si="11"/>
         <v>319.93013526515875</v>
       </c>
       <c r="Q42" s="24">
-        <f>Q30+273.15</f>
+        <f t="shared" si="11"/>
         <v>319.93591507034586</v>
       </c>
       <c r="R42" s="24">
-        <f>R30+273.15</f>
+        <f t="shared" si="11"/>
         <v>319.98130444404444</v>
       </c>
       <c r="S42" s="24">
-        <f>S30+273.15</f>
+        <f t="shared" si="11"/>
         <v>319.98563639027623</v>
       </c>
       <c r="T42" s="24">
-        <f>T30+273.15</f>
+        <f t="shared" si="11"/>
         <v>319.9632722324157</v>
       </c>
       <c r="U42" s="24">
-        <f>U30+273.15</f>
+        <f t="shared" si="11"/>
         <v>319.92324841993519</v>
       </c>
       <c r="V42" s="24">
-        <f>V30+273.15</f>
+        <f t="shared" si="11"/>
         <v>319.92299838980034</v>
       </c>
       <c r="W42" s="24">
-        <f>W30+273.15</f>
+        <f t="shared" si="11"/>
         <v>319.9632722324157</v>
       </c>
       <c r="X42" s="24">
-        <f>X30+273.15</f>
+        <f t="shared" si="11"/>
         <v>319.9883711327808</v>
       </c>
       <c r="Y42" s="24">
-        <f>Y30+273.15</f>
+        <f t="shared" si="11"/>
         <v>319.99352168817984</v>
       </c>
     </row>
@@ -4720,95 +4720,95 @@
         <v>90</v>
       </c>
       <c r="C43" s="24">
-        <f>C35+273.15</f>
+        <f t="shared" ref="C43:Y43" si="12">C35+273.15</f>
         <v>305.35915961980555</v>
       </c>
       <c r="D43" s="24">
-        <f>D35+273.15</f>
+        <f t="shared" si="12"/>
         <v>309.79188253593401</v>
       </c>
       <c r="E43" s="24">
-        <f>E35+273.15</f>
+        <f t="shared" si="12"/>
         <v>312.35623159324001</v>
       </c>
       <c r="F43" s="24">
-        <f>F35+273.15</f>
+        <f t="shared" si="12"/>
         <v>318.26500700465544</v>
       </c>
       <c r="G43" s="24">
-        <f>G35+273.15</f>
+        <f t="shared" si="12"/>
         <v>323.63862859035953</v>
       </c>
       <c r="H43" s="24">
-        <f>H35+273.15</f>
+        <f t="shared" si="12"/>
         <v>318.26500700465544</v>
       </c>
       <c r="I43" s="24">
-        <f>I35+273.15</f>
+        <f t="shared" si="12"/>
         <v>318.30270436408495</v>
       </c>
       <c r="J43" s="24">
-        <f>J35+273.15</f>
+        <f t="shared" si="12"/>
         <v>318.4829372796284</v>
       </c>
       <c r="K43" s="24">
-        <f>K35+273.15</f>
+        <f t="shared" si="12"/>
         <v>318.80301197436296</v>
       </c>
       <c r="L43" s="24">
-        <f>L35+273.15</f>
+        <f t="shared" si="12"/>
         <v>319.01289994963463</v>
       </c>
       <c r="M43" s="24">
-        <f>M35+273.15</f>
+        <f t="shared" si="12"/>
         <v>319.56472605071929</v>
       </c>
       <c r="N43" s="24">
-        <f>N35+273.15</f>
+        <f t="shared" si="12"/>
         <v>318.40305616471557</v>
       </c>
       <c r="O43" s="24">
-        <f>O35+273.15</f>
+        <f t="shared" si="12"/>
         <v>318.26500700465544</v>
       </c>
       <c r="P43" s="24">
-        <f>P35+273.15</f>
+        <f t="shared" si="12"/>
         <v>318.70412169546893</v>
       </c>
       <c r="Q43" s="24">
-        <f>Q35+273.15</f>
+        <f t="shared" si="12"/>
         <v>318.81776959447166</v>
       </c>
       <c r="R43" s="24">
-        <f>R35+273.15</f>
+        <f t="shared" si="12"/>
         <v>318.56053255624283</v>
       </c>
       <c r="S43" s="24">
-        <f>S35+273.15</f>
+        <f t="shared" si="12"/>
         <v>318.51664490974343</v>
       </c>
       <c r="T43" s="24">
-        <f>T35+273.15</f>
+        <f t="shared" si="12"/>
         <v>318.26500700465544</v>
       </c>
       <c r="U43" s="24">
-        <f>U35+273.15</f>
+        <f t="shared" si="12"/>
         <v>318.3348782464065</v>
       </c>
       <c r="V43" s="24">
-        <f>V35+273.15</f>
+        <f t="shared" si="12"/>
         <v>318.29827050530861</v>
       </c>
       <c r="W43" s="24">
-        <f>W35+273.15</f>
+        <f t="shared" si="12"/>
         <v>318.26500700465544</v>
       </c>
       <c r="X43" s="24">
-        <f>X35+273.15</f>
+        <f t="shared" si="12"/>
         <v>318.3938189793015</v>
       </c>
       <c r="Y43" s="24">
-        <f>Y35+273.15</f>
+        <f t="shared" si="12"/>
         <v>318.0786832403021</v>
       </c>
     </row>
@@ -4838,95 +4838,95 @@
         <v>86</v>
       </c>
       <c r="C45" s="24">
-        <f>C27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" ref="C45:Y45" si="13">C27/1000000/60/(MOD1H*MOD1W/10000)</f>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="D45" s="24">
-        <f>D27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" si="13"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="E45" s="24">
-        <f>E27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" si="13"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="F45" s="24">
-        <f>F27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" si="13"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="G45" s="24">
-        <f>G27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" si="13"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="H45" s="24">
-        <f>H27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" si="13"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="I45" s="24">
-        <f>I27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" si="13"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="J45" s="24">
-        <f>J27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" si="13"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="K45" s="24">
-        <f>K27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" si="13"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="L45" s="24">
-        <f>L27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" si="13"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="M45" s="24">
-        <f>M27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" si="13"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="N45" s="24">
-        <f>N27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" si="13"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="O45" s="24">
-        <f>O27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" si="13"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="P45" s="24">
-        <f>P27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" si="13"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="Q45" s="24">
-        <f>Q27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" si="13"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="R45" s="24">
-        <f>R27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" si="13"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="S45" s="24">
-        <f>S27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" si="13"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="T45" s="24">
-        <f>T27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" si="13"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="U45" s="24">
-        <f>U27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" si="13"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="V45" s="24">
-        <f>V27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" si="13"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="W45" s="24">
-        <f>W27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" si="13"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="X45" s="24">
-        <f>X27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" si="13"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="Y45" s="24">
-        <f>Y27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" si="13"/>
         <v>8.7448888888888889E-3</v>
       </c>
     </row>
@@ -4938,95 +4938,95 @@
         <v>90</v>
       </c>
       <c r="C46" s="24">
-        <f>C33+273.15</f>
+        <f t="shared" ref="C46:Y46" si="14">C33+273.15</f>
         <v>293.17058482349387</v>
       </c>
       <c r="D46" s="24">
-        <f>D33+273.15</f>
+        <f t="shared" si="14"/>
         <v>293.16399690708016</v>
       </c>
       <c r="E46" s="24">
-        <f>E33+273.15</f>
+        <f t="shared" si="14"/>
         <v>293.19055520526842</v>
       </c>
       <c r="F46" s="24">
-        <f>F33+273.15</f>
+        <f t="shared" si="14"/>
         <v>293.11519271759857</v>
       </c>
       <c r="G46" s="24">
-        <f>G33+273.15</f>
+        <f t="shared" si="14"/>
         <v>293.68159105444261</v>
       </c>
       <c r="H46" s="24">
-        <f>H33+273.15</f>
+        <f t="shared" si="14"/>
         <v>293.11519271759857</v>
       </c>
       <c r="I46" s="24">
-        <f>I33+273.15</f>
+        <f t="shared" si="14"/>
         <v>298.17047781625797</v>
       </c>
       <c r="J46" s="24">
-        <f>J33+273.15</f>
+        <f t="shared" si="14"/>
         <v>303.14666093734934</v>
       </c>
       <c r="K46" s="24">
-        <f>K33+273.15</f>
+        <f t="shared" si="14"/>
         <v>308.13104480298307</v>
       </c>
       <c r="L46" s="24">
-        <f>L33+273.15</f>
+        <f t="shared" si="14"/>
         <v>313.1456119665342</v>
       </c>
       <c r="M46" s="24">
-        <f>M33+273.15</f>
+        <f t="shared" si="14"/>
         <v>293.10147626262693</v>
       </c>
       <c r="N46" s="24">
-        <f>N33+273.15</f>
+        <f t="shared" si="14"/>
         <v>293.13472615642195</v>
       </c>
       <c r="O46" s="24">
-        <f>O33+273.15</f>
+        <f t="shared" si="14"/>
         <v>293.11519271759857</v>
       </c>
       <c r="P46" s="24">
-        <f>P33+273.15</f>
+        <f t="shared" si="14"/>
         <v>293.13426554012835</v>
       </c>
       <c r="Q46" s="24">
-        <f>Q33+273.15</f>
+        <f t="shared" si="14"/>
         <v>293.18355233922148</v>
       </c>
       <c r="R46" s="24">
-        <f>R33+273.15</f>
+        <f t="shared" si="14"/>
         <v>293.14611427063818</v>
       </c>
       <c r="S46" s="24">
-        <f>S33+273.15</f>
+        <f t="shared" si="14"/>
         <v>293.13525638330668</v>
       </c>
       <c r="T46" s="24">
-        <f>T33+273.15</f>
+        <f t="shared" si="14"/>
         <v>293.11519271759857</v>
       </c>
       <c r="U46" s="24">
-        <f>U33+273.15</f>
+        <f t="shared" si="14"/>
         <v>293.12888473278991</v>
       </c>
       <c r="V46" s="24">
-        <f>V33+273.15</f>
+        <f t="shared" si="14"/>
         <v>293.09014458415839</v>
       </c>
       <c r="W46" s="24">
-        <f>W33+273.15</f>
+        <f t="shared" si="14"/>
         <v>293.11519271759857</v>
       </c>
       <c r="X46" s="24">
-        <f>X33+273.15</f>
+        <f t="shared" si="14"/>
         <v>293.11284038778177</v>
       </c>
       <c r="Y46" s="24">
-        <f>Y33+273.15</f>
+        <f t="shared" si="14"/>
         <v>293.09308391529044</v>
       </c>
     </row>
@@ -5038,95 +5038,95 @@
         <v>90</v>
       </c>
       <c r="C47" s="24">
-        <f>C36+273.15</f>
+        <f t="shared" ref="C47:Y47" si="15">C36+273.15</f>
         <v>294.29682689366177</v>
       </c>
       <c r="D47" s="24">
-        <f>D36+273.15</f>
+        <f t="shared" si="15"/>
         <v>294.21664608339694</v>
       </c>
       <c r="E47" s="24">
-        <f>E36+273.15</f>
+        <f t="shared" si="15"/>
         <v>294.35225488233681</v>
       </c>
       <c r="F47" s="24">
-        <f>F36+273.15</f>
+        <f t="shared" si="15"/>
         <v>294.57886130730265</v>
       </c>
       <c r="G47" s="24">
-        <f>G36+273.15</f>
+        <f t="shared" si="15"/>
         <v>295.14325006184663</v>
       </c>
       <c r="H47" s="24">
-        <f>H36+273.15</f>
+        <f t="shared" si="15"/>
         <v>294.57886130730265</v>
       </c>
       <c r="I47" s="24">
-        <f>I36+273.15</f>
+        <f t="shared" si="15"/>
         <v>299.22168943939931</v>
       </c>
       <c r="J47" s="24">
-        <f>J36+273.15</f>
+        <f t="shared" si="15"/>
         <v>303.91148736331343</v>
       </c>
       <c r="K47" s="24">
-        <f>K36+273.15</f>
+        <f t="shared" si="15"/>
         <v>308.65229050926581</v>
       </c>
       <c r="L47" s="24">
-        <f>L36+273.15</f>
+        <f t="shared" si="15"/>
         <v>313.57345483397432</v>
       </c>
       <c r="M47" s="24">
-        <f>M36+273.15</f>
+        <f t="shared" si="15"/>
         <v>294.64494411853934</v>
       </c>
       <c r="N47" s="24">
-        <f>N36+273.15</f>
+        <f t="shared" si="15"/>
         <v>294.66788302030187</v>
       </c>
       <c r="O47" s="24">
-        <f>O36+273.15</f>
+        <f t="shared" si="15"/>
         <v>294.57886130730265</v>
       </c>
       <c r="P47" s="24">
-        <f>P36+273.15</f>
+        <f t="shared" si="15"/>
         <v>294.74539495317856</v>
       </c>
       <c r="Q47" s="24">
-        <f>Q36+273.15</f>
+        <f t="shared" si="15"/>
         <v>294.95517646294218</v>
       </c>
       <c r="R47" s="24">
-        <f>R36+273.15</f>
+        <f t="shared" si="15"/>
         <v>294.88340227697375</v>
       </c>
       <c r="S47" s="24">
-        <f>S36+273.15</f>
+        <f t="shared" si="15"/>
         <v>295.00451737531392</v>
       </c>
       <c r="T47" s="24">
-        <f>T36+273.15</f>
+        <f t="shared" si="15"/>
         <v>294.57886130730265</v>
       </c>
       <c r="U47" s="24">
-        <f>U36+273.15</f>
+        <f t="shared" si="15"/>
         <v>294.62908105804513</v>
       </c>
       <c r="V47" s="24">
-        <f>V36+273.15</f>
+        <f t="shared" si="15"/>
         <v>294.46046760050325</v>
       </c>
       <c r="W47" s="24">
-        <f>W36+273.15</f>
+        <f t="shared" si="15"/>
         <v>294.57886130730265</v>
       </c>
       <c r="X47" s="24">
-        <f>X36+273.15</f>
+        <f t="shared" si="15"/>
         <v>294.62831839055224</v>
       </c>
       <c r="Y47" s="24">
-        <f>Y36+273.15</f>
+        <f t="shared" si="15"/>
         <v>294.45689294842822</v>
       </c>
     </row>
@@ -5138,99 +5138,99 @@
         <v>89</v>
       </c>
       <c r="C48" s="24">
-        <f>C37/3600</f>
+        <f t="shared" ref="C48:Y48" si="16">C37/3600</f>
         <v>1.0791274666666665E-3</v>
       </c>
       <c r="D48" s="24">
-        <f>D37/3600</f>
+        <f t="shared" si="16"/>
         <v>1.5744281599999997E-3</v>
       </c>
       <c r="E48" s="24">
-        <f>E37/3600</f>
+        <f t="shared" si="16"/>
         <v>1.9465498666666667E-3</v>
       </c>
       <c r="F48" s="24">
-        <f>F37/3600</f>
+        <f t="shared" si="16"/>
         <v>2.9802457599999999E-3</v>
       </c>
       <c r="G48" s="24">
-        <f>G37/3600</f>
+        <f t="shared" si="16"/>
         <v>3.9183833599999995E-3</v>
       </c>
       <c r="H48" s="24">
-        <f>H37/3600</f>
+        <f t="shared" si="16"/>
         <v>2.9802457599999999E-3</v>
       </c>
       <c r="I48" s="24">
-        <f>I37/3600</f>
+        <f t="shared" si="16"/>
         <v>2.5700625066666666E-3</v>
       </c>
       <c r="J48" s="24">
-        <f>J37/3600</f>
+        <f t="shared" si="16"/>
         <v>2.1235246933333334E-3</v>
       </c>
       <c r="K48" s="24">
-        <f>K37/3600</f>
+        <f t="shared" si="16"/>
         <v>1.5609421866666663E-3</v>
       </c>
       <c r="L48" s="24">
-        <f>L37/3600</f>
+        <f t="shared" si="16"/>
         <v>9.935384533333333E-4</v>
       </c>
       <c r="M48" s="24">
-        <f>M37/3600</f>
+        <f t="shared" si="16"/>
         <v>2.9378886400000001E-3</v>
       </c>
       <c r="N48" s="24">
-        <f>N37/3600</f>
+        <f t="shared" si="16"/>
         <v>2.8567750399999996E-3</v>
       </c>
       <c r="O48" s="24">
-        <f>O37/3600</f>
+        <f t="shared" si="16"/>
         <v>2.9802457599999999E-3</v>
       </c>
       <c r="P48" s="24">
-        <f>P37/3600</f>
+        <f t="shared" si="16"/>
         <v>3.0446920533333329E-3</v>
       </c>
       <c r="Q48" s="24">
-        <f>Q37/3600</f>
+        <f t="shared" si="16"/>
         <v>3.1019777066666663E-3</v>
       </c>
       <c r="R48" s="24">
-        <f>R37/3600</f>
+        <f t="shared" si="16"/>
         <v>2.7461594666666673E-3</v>
       </c>
       <c r="S48" s="24">
-        <f>S37/3600</f>
+        <f t="shared" si="16"/>
         <v>2.8241684266666666E-3</v>
       </c>
       <c r="T48" s="24">
-        <f>T37/3600</f>
+        <f t="shared" si="16"/>
         <v>2.9802457599999999E-3</v>
       </c>
       <c r="U48" s="24">
-        <f>U37/3600</f>
+        <f t="shared" si="16"/>
         <v>3.2108769066666668E-3</v>
       </c>
       <c r="V48" s="24">
-        <f>V37/3600</f>
+        <f t="shared" si="16"/>
         <v>3.3036054400000002E-3</v>
       </c>
       <c r="W48" s="24">
-        <f>W37/3600</f>
+        <f t="shared" si="16"/>
         <v>2.9802457599999999E-3</v>
       </c>
       <c r="X48" s="24">
-        <f>X37/3600</f>
+        <f t="shared" si="16"/>
         <v>9.7313013333333309E-4</v>
       </c>
       <c r="Y48" s="24">
-        <f>Y37/3600</f>
+        <f t="shared" si="16"/>
         <v>1.3370305066666666E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:12" customFormat="1">
+    <row r="49" spans="1:25" customFormat="1">
       <c r="A49" s="18" t="s">
         <v>88</v>
       </c>
@@ -5240,7 +5240,7 @@
       <c r="K49" s="36"/>
       <c r="L49" s="36"/>
     </row>
-    <row r="50" spans="1:12" s="36" customFormat="1">
+    <row r="50" spans="1:25" s="36" customFormat="1">
       <c r="A50" s="37" t="s">
         <v>136</v>
       </c>
@@ -5260,7 +5260,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:12" s="36" customFormat="1">
+    <row r="51" spans="1:25" s="36" customFormat="1">
       <c r="A51" s="37" t="s">
         <v>104</v>
       </c>
@@ -5280,7 +5280,7 @@
         <v>317.02</v>
       </c>
     </row>
-    <row r="52" spans="1:12" s="36" customFormat="1">
+    <row r="52" spans="1:25" s="36" customFormat="1">
       <c r="A52" s="37" t="s">
         <v>105</v>
       </c>
@@ -5300,7 +5300,7 @@
         <v>296.02</v>
       </c>
     </row>
-    <row r="53" spans="1:12" s="36" customFormat="1">
+    <row r="53" spans="1:25" s="36" customFormat="1">
       <c r="A53" s="36" t="s">
         <v>71</v>
       </c>
@@ -5326,7 +5326,7 @@
       <c r="K53" s="28"/>
       <c r="L53" s="28"/>
     </row>
-    <row r="54" spans="1:12" s="28" customFormat="1">
+    <row r="54" spans="1:25" s="28" customFormat="1">
       <c r="E54" s="39"/>
       <c r="H54" s="40"/>
       <c r="I54" s="40"/>
@@ -5334,7 +5334,7 @@
       <c r="K54" s="40"/>
       <c r="L54" s="40"/>
     </row>
-    <row r="55" spans="1:12" s="40" customFormat="1">
+    <row r="55" spans="1:25" s="40" customFormat="1">
       <c r="A55" s="40" t="s">
         <v>136</v>
       </c>
@@ -5356,8 +5356,50 @@
       <c r="G55" s="40">
         <v>5</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" s="40" customFormat="1">
+      <c r="I55" s="40">
+        <v>6</v>
+      </c>
+      <c r="J55" s="40">
+        <v>7</v>
+      </c>
+      <c r="K55" s="40">
+        <v>8</v>
+      </c>
+      <c r="L55" s="40">
+        <v>9</v>
+      </c>
+      <c r="M55" s="40">
+        <v>10</v>
+      </c>
+      <c r="N55" s="40">
+        <v>11</v>
+      </c>
+      <c r="P55" s="40">
+        <v>12</v>
+      </c>
+      <c r="Q55" s="40">
+        <v>13</v>
+      </c>
+      <c r="R55" s="40">
+        <v>14</v>
+      </c>
+      <c r="S55" s="40">
+        <v>15</v>
+      </c>
+      <c r="U55" s="40">
+        <v>16</v>
+      </c>
+      <c r="V55" s="40">
+        <v>17</v>
+      </c>
+      <c r="X55" s="40">
+        <v>18</v>
+      </c>
+      <c r="Y55" s="40">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25" s="40" customFormat="1">
       <c r="A56" s="40" t="s">
         <v>108</v>
       </c>
@@ -5380,8 +5422,11 @@
         <f>SimRecords!$B$5</f>
         <v>322.74</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" s="40" customFormat="1">
+      <c r="I56" s="40">
+        <v>318.13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:25" s="40" customFormat="1">
       <c r="A57" s="40" t="s">
         <v>109</v>
       </c>
@@ -5404,8 +5449,11 @@
         <f>SimRecords!$B$6</f>
         <v>296.47000000000003</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" s="40" customFormat="1">
+      <c r="I57" s="40">
+        <v>299.95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25" s="40" customFormat="1">
       <c r="A58" s="40" t="s">
         <v>117</v>
       </c>
@@ -5428,41 +5476,47 @@
         <f>SimRecords!$B$7</f>
         <v>7.6959</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" s="40" customFormat="1">
+      <c r="I58" s="40">
+        <v>5.0377000000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" s="40" customFormat="1">
       <c r="A59" s="40" t="s">
         <v>71</v>
       </c>
       <c r="B59" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="C59" s="40">
+      <c r="C59" s="24">
         <f>C58*0.0005</f>
         <v>1.0750550000000001E-3</v>
       </c>
-      <c r="D59" s="40">
+      <c r="D59" s="24">
         <f>D58*0.0005</f>
         <v>1.5754600000000001E-3</v>
       </c>
-      <c r="E59" s="40">
+      <c r="E59" s="24">
         <f>E58*0.0005</f>
         <v>1.937825E-3</v>
       </c>
-      <c r="F59" s="40">
+      <c r="F59" s="24">
         <f>F58*0.0005</f>
         <v>2.887485E-3</v>
       </c>
-      <c r="G59" s="40">
+      <c r="G59" s="24">
         <f>SimRecords!$B$8</f>
         <v>3.8479500000000002E-3</v>
       </c>
       <c r="H59" s="17"/>
-      <c r="I59" s="17"/>
+      <c r="I59" s="24">
+        <f>I58*0.0005</f>
+        <v>2.51885E-3</v>
+      </c>
       <c r="J59" s="17"/>
       <c r="K59" s="17"/>
       <c r="L59" s="17"/>
     </row>
-    <row r="60" spans="1:12">
+    <row r="60" spans="1:25">
       <c r="A60" s="40" t="s">
         <v>121</v>
       </c>
@@ -5475,19 +5529,23 @@
         <v>1.2004269863037987E-3</v>
       </c>
       <c r="E60" s="24">
-        <f t="shared" ref="E60:G60" si="10">(E43-E56)/E43</f>
+        <f t="shared" ref="E60:G60" si="17">(E43-E56)/E43</f>
         <v>9.4837740783661011E-4</v>
       </c>
       <c r="F60" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>1.5239093019371039E-3</v>
       </c>
       <c r="G60" s="24">
-        <f t="shared" si="10"/>
+        <f t="shared" si="17"/>
         <v>2.7766419425072604E-3</v>
       </c>
-    </row>
-    <row r="61" spans="1:12">
+      <c r="I60" s="24">
+        <f t="shared" ref="I60" si="18">(I43-I56)/I43</f>
+        <v>5.4257900331065141E-4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25">
       <c r="A61" s="40" t="s">
         <v>122</v>
       </c>
@@ -5500,19 +5558,23 @@
         <v>-7.9313634938556589E-4</v>
       </c>
       <c r="E61" s="24">
-        <f t="shared" ref="E61:G61" si="11">(E47-E57)/E47</f>
+        <f t="shared" ref="E61:G61" si="19">(E47-E57)/E47</f>
         <v>-1.3512555486357143E-3</v>
       </c>
       <c r="F61" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>-2.5838197938558632E-3</v>
       </c>
       <c r="G61" s="24">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>-4.4952745416857081E-3</v>
       </c>
-    </row>
-    <row r="62" spans="1:12">
+      <c r="I61" s="24">
+        <f t="shared" ref="I61" si="20">(I47-I57)/I47</f>
+        <v>-2.4340166047628E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25">
       <c r="A62" s="40" t="s">
         <v>123</v>
       </c>
@@ -5525,19 +5587,23 @@
         <v>-6.5537445671729399E-4</v>
       </c>
       <c r="E62" s="25">
-        <f t="shared" ref="E62:G62" si="12">(E48-E59)/E48</f>
+        <f t="shared" ref="E62:G62" si="21">(E48-E59)/E48</f>
         <v>4.4822209880538222E-3</v>
       </c>
       <c r="F62" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>3.1125204922697346E-2</v>
       </c>
       <c r="G62" s="25">
-        <f t="shared" si="12"/>
+        <f t="shared" si="21"/>
         <v>1.7975106958396075E-2</v>
       </c>
-    </row>
-    <row r="63" spans="1:12">
+      <c r="I62" s="25">
+        <f t="shared" ref="I62" si="22">(I48-I59)/I48</f>
+        <v>1.9926560748551023E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25">
       <c r="A63" s="40" t="s">
         <v>120</v>
       </c>
@@ -5550,22 +5616,26 @@
         <v>1.5810141987599514E-3</v>
       </c>
       <c r="E63" s="24">
-        <f t="shared" ref="E63:G63" si="13">SQRT(E60^2+E61^2+E62^2)</f>
+        <f t="shared" ref="E63:G63" si="23">SQRT(E60^2+E61^2+E62^2)</f>
         <v>4.7765695065772754E-3</v>
       </c>
       <c r="F63" s="24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="23"/>
         <v>3.1269422856323316E-2</v>
       </c>
       <c r="G63" s="24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="23"/>
         <v>1.8735573219087726E-2</v>
+      </c>
+      <c r="I63" s="24">
+        <f t="shared" ref="I63" si="24">SQRT(I60^2+I61^2+I62^2)</f>
+        <v>2.0081998209162077E-2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0.94488188976377963" bottom="0.94488188976377963" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0.23622047244094491" bottom="0.23622047244094491" header="0.11811023622047245" footer="0.11811023622047245"/>
+  <pageSetup paperSize="9" scale="55" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7584,75 +7654,75 @@
         <v>14.106180095999997</v>
       </c>
       <c r="S23">
-        <f>S10</f>
+        <f t="shared" ref="S23:AJ23" si="37">S10</f>
         <v>10.728884735999999</v>
       </c>
       <c r="T23">
-        <f>T10</f>
+        <f t="shared" si="37"/>
         <v>9.2522250239999995</v>
       </c>
       <c r="U23">
-        <f>U10</f>
+        <f t="shared" si="37"/>
         <v>7.6446888960000008</v>
       </c>
       <c r="V23">
-        <f>V10</f>
+        <f t="shared" si="37"/>
         <v>5.6193918719999987</v>
       </c>
       <c r="W23">
-        <f>W10</f>
+        <f t="shared" si="37"/>
         <v>3.5767384319999995</v>
       </c>
       <c r="X23">
-        <f>X10</f>
+        <f t="shared" si="37"/>
         <v>10.576399104</v>
       </c>
       <c r="Y23">
-        <f>Y10</f>
+        <f t="shared" si="37"/>
         <v>10.284390143999998</v>
       </c>
       <c r="Z23">
-        <f>Z10</f>
+        <f t="shared" si="37"/>
         <v>10.728884735999999</v>
       </c>
       <c r="AA23">
-        <f>AA10</f>
+        <f t="shared" si="37"/>
         <v>10.960891391999999</v>
       </c>
       <c r="AB23">
-        <f>AB10</f>
+        <f t="shared" si="37"/>
         <v>11.167119743999999</v>
       </c>
       <c r="AC23">
-        <f>AC10</f>
+        <f t="shared" si="37"/>
         <v>9.8861740800000018</v>
       </c>
       <c r="AD23">
-        <f>AD10</f>
+        <f t="shared" si="37"/>
         <v>10.167006336</v>
       </c>
       <c r="AE23">
-        <f>AE10</f>
+        <f t="shared" si="37"/>
         <v>10.728884735999999</v>
       </c>
       <c r="AF23">
-        <f>AF10</f>
+        <f t="shared" si="37"/>
         <v>11.559156864</v>
       </c>
       <c r="AG23">
-        <f>AG10</f>
+        <f t="shared" si="37"/>
         <v>11.892979584000001</v>
       </c>
       <c r="AH23">
-        <f>AH10</f>
+        <f t="shared" si="37"/>
         <v>10.728884735999999</v>
       </c>
       <c r="AI23">
-        <f>AI10</f>
+        <f t="shared" si="37"/>
         <v>3.5032684799999991</v>
       </c>
       <c r="AJ23">
-        <f>AJ10</f>
+        <f t="shared" si="37"/>
         <v>4.8133098240000001</v>
       </c>
     </row>
@@ -7701,91 +7771,91 @@
         <v/>
       </c>
       <c r="O24" s="44" t="str">
-        <f t="shared" ref="O24:AJ24" si="37">IF(O26=1, "duplicate","")</f>
+        <f t="shared" ref="O24:AJ24" si="38">IF(O26=1, "duplicate","")</f>
         <v/>
       </c>
       <c r="P24" s="44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="Q24" s="44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="R24" s="44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="S24" s="44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>duplicate</v>
       </c>
       <c r="T24" s="44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="U24" s="44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="V24" s="44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="W24" s="44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="X24" s="44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="Y24" s="44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="Z24" s="44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>duplicate</v>
       </c>
       <c r="AA24" s="44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="AB24" s="44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="AC24" s="44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="AD24" s="44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="AE24" s="44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>duplicate</v>
       </c>
       <c r="AF24" s="44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="AG24" s="44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="AH24" s="44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>duplicate</v>
       </c>
       <c r="AI24" s="44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="AJ24" s="44" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
     </row>
@@ -7941,91 +8011,91 @@
         <v>0</v>
       </c>
       <c r="O26" s="43">
-        <f t="shared" ref="O26:AJ26" si="38">HLOOKUP(O25,$N28:$AJ31,4,FALSE)</f>
+        <f t="shared" ref="O26:AJ26" si="39">HLOOKUP(O25,$N28:$AJ31,4,FALSE)</f>
         <v>0</v>
       </c>
       <c r="P26" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Q26" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="R26" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="S26" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>1</v>
       </c>
       <c r="T26" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="U26" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="V26" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="W26" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="X26" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y26" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Z26" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>1</v>
       </c>
       <c r="AA26" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AB26" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AC26" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AD26" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AE26" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>1</v>
       </c>
       <c r="AF26" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AG26" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AH26" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>1</v>
       </c>
       <c r="AI26" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AJ26" s="43">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
     </row>
@@ -8387,91 +8457,91 @@
         <v>0</v>
       </c>
       <c r="O31" s="43">
-        <f t="shared" ref="O31:AJ31" si="39">IF(MATCH(O29,$N29:$AN29,0)=O30, 0, 1)</f>
+        <f t="shared" ref="O31:AJ31" si="40">IF(MATCH(O29,$N29:$AN29,0)=O30, 0, 1)</f>
         <v>0</v>
       </c>
       <c r="P31" s="43">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="Q31" s="43">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="R31" s="43">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="S31" s="43">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="T31" s="43">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="U31" s="43">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="V31" s="43">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="W31" s="43">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="X31" s="43">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="Y31" s="43">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="Z31" s="43">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="AA31" s="43">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="AB31" s="43">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1</v>
       </c>
       <c r="AC31" s="43">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1</v>
       </c>
       <c r="AD31" s="43">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1</v>
       </c>
       <c r="AE31" s="43">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>1</v>
       </c>
       <c r="AF31" s="43">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="AG31" s="43">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="AH31" s="43">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="AI31" s="43">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="AJ31" s="43">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add the case and data files of 16GGQ-2-7
</commit_message>
<xml_diff>
--- a/bin/2d_s_cc/reorganized exp.data.xlsx
+++ b/bin/2d_s_cc/reorganized exp.data.xlsx
@@ -1299,23 +1299,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="154027136"/>
-        <c:axId val="154028672"/>
+        <c:axId val="184235136"/>
+        <c:axId val="184236672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="154027136"/>
+        <c:axId val="184235136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154028672"/>
+        <c:crossAx val="184236672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="154028672"/>
+        <c:axId val="184236672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1323,7 +1323,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154027136"/>
+        <c:crossAx val="184235136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1335,7 +1335,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2886,8 +2886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="K57" sqref="K57"/>
+    <sheetView tabSelected="1" topLeftCell="B52" workbookViewId="0">
+      <selection activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5425,6 +5425,9 @@
       <c r="I56" s="40">
         <v>318.13</v>
       </c>
+      <c r="J56" s="40">
+        <v>318.58</v>
+      </c>
     </row>
     <row r="57" spans="1:25" s="40" customFormat="1">
       <c r="A57" s="40" t="s">
@@ -5452,6 +5455,9 @@
       <c r="I57" s="40">
         <v>299.95</v>
       </c>
+      <c r="J57" s="40">
+        <v>304.49</v>
+      </c>
     </row>
     <row r="58" spans="1:25" s="40" customFormat="1">
       <c r="A58" s="40" t="s">
@@ -5478,6 +5484,9 @@
       </c>
       <c r="I58" s="40">
         <v>5.0377000000000001</v>
+      </c>
+      <c r="J58" s="40">
+        <v>4.1998899999999999</v>
       </c>
     </row>
     <row r="59" spans="1:25" s="40" customFormat="1">
@@ -5512,7 +5521,10 @@
         <f>I58*0.0005</f>
         <v>2.51885E-3</v>
       </c>
-      <c r="J59" s="17"/>
+      <c r="J59" s="24">
+        <f>J58*0.0005</f>
+        <v>2.0999450000000002E-3</v>
+      </c>
       <c r="K59" s="17"/>
       <c r="L59" s="17"/>
     </row>
@@ -5541,8 +5553,12 @@
         <v>2.7766419425072604E-3</v>
       </c>
       <c r="I60" s="24">
-        <f t="shared" ref="I60" si="18">(I43-I56)/I43</f>
+        <f t="shared" ref="I60:J60" si="18">(I43-I56)/I43</f>
         <v>5.4257900331065141E-4</v>
+      </c>
+      <c r="J60" s="24">
+        <f t="shared" si="18"/>
+        <v>-3.047658414628378E-4</v>
       </c>
     </row>
     <row r="61" spans="1:25">
@@ -5570,8 +5586,12 @@
         <v>-4.4952745416857081E-3</v>
       </c>
       <c r="I61" s="24">
-        <f t="shared" ref="I61" si="20">(I47-I57)/I47</f>
+        <f t="shared" ref="I61:J61" si="20">(I47-I57)/I47</f>
         <v>-2.4340166047628E-3</v>
+      </c>
+      <c r="J61" s="24">
+        <f t="shared" si="20"/>
+        <v>-1.9035563338051613E-3</v>
       </c>
     </row>
     <row r="62" spans="1:25">
@@ -5599,8 +5619,12 @@
         <v>1.7975106958396075E-2</v>
       </c>
       <c r="I62" s="25">
-        <f t="shared" ref="I62" si="22">(I48-I59)/I48</f>
+        <f t="shared" ref="I62:J62" si="22">(I48-I59)/I48</f>
         <v>1.9926560748551023E-2</v>
+      </c>
+      <c r="J62" s="25">
+        <f t="shared" si="22"/>
+        <v>1.1104035383887956E-2</v>
       </c>
     </row>
     <row r="63" spans="1:25">
@@ -5628,8 +5652,12 @@
         <v>1.8735573219087726E-2</v>
       </c>
       <c r="I63" s="24">
-        <f t="shared" ref="I63" si="24">SQRT(I60^2+I61^2+I62^2)</f>
+        <f t="shared" ref="I63:J63" si="24">SQRT(I60^2+I61^2+I62^2)</f>
         <v>2.0081998209162077E-2</v>
+      </c>
+      <c r="J63" s="24">
+        <f t="shared" si="24"/>
+        <v>1.1270138008947718E-2</v>
       </c>
     </row>
   </sheetData>
@@ -5643,7 +5671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AL33"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="N24" sqref="N24:AJ24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Correct the uncorrected specification of flowrates in "reorganized exp.data.xlsx"
</commit_message>
<xml_diff>
--- a/bin/2d_s_cc/reorganized exp.data.xlsx
+++ b/bin/2d_s_cc/reorganized exp.data.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OneDrive - mail.scut.edu.cn\git\bin\2d_s_cc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="2340" yWindow="75" windowWidth="17235" windowHeight="8955" activeTab="1"/>
   </bookViews>
@@ -25,7 +20,7 @@
     <definedName name="MOD1L">'Yao2016(preparing)'!$C$15</definedName>
     <definedName name="MOD1W">'Yao2016(preparing)'!$C$16</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -35,7 +30,7 @@
     <author>Guoqiang GUAN</author>
   </authors>
   <commentList>
-    <comment ref="C6" authorId="0" shapeId="0">
+    <comment ref="C6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -59,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C14" authorId="0" shapeId="0">
+    <comment ref="C14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -83,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C16" authorId="0" shapeId="0">
+    <comment ref="C16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C34" authorId="0" shapeId="0">
+    <comment ref="C34" authorId="0">
       <text>
         <r>
           <rPr>
@@ -131,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D34" authorId="0" shapeId="0">
+    <comment ref="D34" authorId="0">
       <text>
         <r>
           <rPr>
@@ -155,7 +150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E34" authorId="0" shapeId="0">
+    <comment ref="E34" authorId="0">
       <text>
         <r>
           <rPr>
@@ -179,7 +174,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F34" authorId="0" shapeId="0">
+    <comment ref="F34" authorId="0">
       <text>
         <r>
           <rPr>
@@ -203,7 +198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G34" authorId="0" shapeId="0">
+    <comment ref="G34" authorId="0">
       <text>
         <r>
           <rPr>
@@ -409,7 +404,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="宋体"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -729,22 +724,22 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -823,7 +818,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -831,7 +826,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -839,14 +834,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -854,7 +849,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -862,26 +857,26 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -926,12 +921,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1078,7 +1067,7 @@
     <xf numFmtId="0" fontId="17" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1154,9 +1143,6 @@
     <xf numFmtId="0" fontId="17" fillId="8" borderId="1" xfId="8" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="17" fillId="8" borderId="1" xfId="8" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
@@ -1193,7 +1179,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -1247,27 +1233,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="1" xfId="8" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="1" xfId="8" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="8" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="20% - 着色 1" xfId="2" builtinId="30"/>
-    <cellStyle name="20% - 着色 2" xfId="3" builtinId="34"/>
-    <cellStyle name="20% - 着色 3" xfId="4" builtinId="38"/>
-    <cellStyle name="20% - 着色 4" xfId="5" builtinId="42"/>
-    <cellStyle name="20% - 着色 6" xfId="6" builtinId="50"/>
-    <cellStyle name="常规" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="计算" xfId="8" builtinId="22"/>
-    <cellStyle name="解释性文本" xfId="1" builtinId="53"/>
-    <cellStyle name="链接单元格" xfId="9" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="输入" xfId="7" builtinId="20"/>
+    <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
+    <cellStyle name="20% - Accent2" xfId="3" builtinId="34"/>
+    <cellStyle name="20% - Accent3" xfId="4" builtinId="38"/>
+    <cellStyle name="20% - Accent4" xfId="5" builtinId="42"/>
+    <cellStyle name="20% - Accent6" xfId="6" builtinId="50"/>
+    <cellStyle name="Calculation" xfId="8" builtinId="22"/>
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
+    <cellStyle name="Input" xfId="7" builtinId="20"/>
+    <cellStyle name="Linked Cell" xfId="9" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1284,24 +1270,12 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
+  <c:lang val="en-SG"/>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1349,60 +1323,45 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="-211645888"/>
-        <c:axId val="-211651328"/>
+        <c:dLbls/>
+        <c:axId val="183732096"/>
+        <c:axId val="183733632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-211645888"/>
+        <c:axId val="183732096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-211651328"/>
+        <c:crossAx val="183733632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-211651328"/>
+        <c:axId val="183733632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-211645888"/>
+        <c:crossAx val="183732096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1444,7 +1403,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="汇总数据"/>
@@ -1461,9 +1420,9 @@
       <sheetName val="安托因方程"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
       <sheetData sheetId="3">
         <row r="12">
           <cell r="U12" t="str">
@@ -1823,7 +1782,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="5"/>
+      <sheetData sheetId="5" refreshError="1"/>
       <sheetData sheetId="6">
         <row r="13">
           <cell r="S13" t="str">
@@ -2207,16 +2166,16 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2258,7 +2217,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2290,10 +2249,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2325,7 +2283,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2501,30 +2458,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.25" customWidth="1"/>
-    <col min="2" max="2" width="11.375" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="16.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="16.5">
       <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" s="3" customFormat="1" ht="16.5">
       <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
@@ -2532,7 +2489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" s="3" customFormat="1" ht="16.5">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
@@ -2540,7 +2497,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" s="3" customFormat="1" ht="16.5">
       <c r="A6" s="8" t="s">
         <v>9</v>
       </c>
@@ -2548,7 +2505,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" s="3" customFormat="1" ht="16.5">
       <c r="A7" s="8" t="s">
         <v>6</v>
       </c>
@@ -2559,7 +2516,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" s="3" customFormat="1" ht="16.5">
       <c r="A8" s="8" t="s">
         <v>23</v>
       </c>
@@ -2570,12 +2527,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" s="3" customFormat="1" ht="16.5">
       <c r="A9" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" s="3" customFormat="1" ht="16.5">
       <c r="A10" s="8" t="s">
         <v>18</v>
       </c>
@@ -2586,7 +2543,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" s="3" customFormat="1" ht="16.5">
       <c r="A11" s="8" t="s">
         <v>19</v>
       </c>
@@ -2597,7 +2554,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" s="3" customFormat="1" ht="16.5">
       <c r="A12" s="8" t="s">
         <v>21</v>
       </c>
@@ -2608,12 +2565,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" s="3" customFormat="1" ht="16.5">
       <c r="A13" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" s="3" customFormat="1" ht="16.5">
       <c r="A14" s="8" t="s">
         <v>30</v>
       </c>
@@ -2624,7 +2581,7 @@
         <v>73.8</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" s="3" customFormat="1" ht="16.5">
       <c r="A15" s="8" t="s">
         <v>31</v>
       </c>
@@ -2635,7 +2592,7 @@
         <v>68.5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" s="3" customFormat="1" ht="16.5">
       <c r="A16" s="8" t="s">
         <v>32</v>
       </c>
@@ -2643,7 +2600,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="3" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" s="3" customFormat="1" ht="16.5">
       <c r="A17" s="8" t="s">
         <v>33</v>
       </c>
@@ -2654,12 +2611,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="16.5">
       <c r="A18" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="4" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" s="4" customFormat="1" ht="16.5">
       <c r="A19" s="7" t="s">
         <v>27</v>
       </c>
@@ -2671,7 +2628,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="4" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" s="4" customFormat="1" ht="16.5">
       <c r="A20" s="7" t="s">
         <v>8</v>
       </c>
@@ -2682,7 +2639,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="4" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" s="4" customFormat="1" ht="16.5">
       <c r="A21" s="7" t="s">
         <v>11</v>
       </c>
@@ -2690,7 +2647,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" s="4" customFormat="1" ht="16.5">
       <c r="A22" s="7" t="s">
         <v>13</v>
       </c>
@@ -2698,13 +2655,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="16.5">
       <c r="A23" s="10" t="s">
         <v>35</v>
       </c>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" s="6" customFormat="1" ht="16.5">
       <c r="A24" s="6" t="s">
         <v>15</v>
       </c>
@@ -2715,12 +2672,12 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" s="6" customFormat="1" ht="16.5">
       <c r="A25" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" s="6" customFormat="1" ht="16.5">
       <c r="A26" s="6" t="s">
         <v>36</v>
       </c>
@@ -2731,7 +2688,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" s="6" customFormat="1" ht="16.5">
       <c r="A27" s="6" t="s">
         <v>37</v>
       </c>
@@ -2754,7 +2711,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:7" s="6" customFormat="1" ht="16.5">
       <c r="B28" s="12" t="s">
         <v>90</v>
       </c>
@@ -2779,12 +2736,12 @@
         <v>313.14999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:7" s="6" customFormat="1" ht="16.5">
       <c r="A29" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:7" s="6" customFormat="1" ht="16.5">
       <c r="A30" s="6" t="s">
         <v>36</v>
       </c>
@@ -2795,7 +2752,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:7" s="6" customFormat="1" ht="16.5">
       <c r="A31" s="6" t="s">
         <v>37</v>
       </c>
@@ -2818,7 +2775,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="6" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:7" s="6" customFormat="1" ht="16.5">
       <c r="B32" s="12" t="s">
         <v>90</v>
       </c>
@@ -2843,12 +2800,12 @@
         <v>290.64999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:7" ht="16.5">
       <c r="A33" s="10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="13" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:7" s="13" customFormat="1" ht="16.5">
       <c r="A34" s="14" t="s">
         <v>44</v>
       </c>
@@ -2871,7 +2828,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="13" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:7" s="13" customFormat="1" ht="16.5">
       <c r="A35" s="14"/>
       <c r="B35" s="13" t="s">
         <v>89</v>
@@ -2897,7 +2854,7 @@
         <v>1.7222222222222222E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="13" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:7" s="13" customFormat="1" ht="16.5">
       <c r="A36" s="14" t="s">
         <v>46</v>
       </c>
@@ -2920,7 +2877,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="13" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:7" s="13" customFormat="1" ht="16.5">
       <c r="A37" s="14" t="s">
         <v>47</v>
       </c>
@@ -2952,253 +2909,257 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="S47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="O38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y63" sqref="Y63"/>
+      <selection pane="bottomRight" activeCell="AC39" sqref="AC39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.75" style="17" customWidth="1"/>
-    <col min="2" max="2" width="10.25" style="17" customWidth="1"/>
-    <col min="3" max="3" width="9.25" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" style="17" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="17" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.25" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="9.125" style="17"/>
-    <col min="12" max="12" width="11.25" style="17" customWidth="1"/>
-    <col min="13" max="13" width="9.125" style="17"/>
-    <col min="14" max="14" width="9.75" style="17" customWidth="1"/>
-    <col min="15" max="16384" width="9.125" style="17"/>
+    <col min="5" max="6" width="9.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="9.140625" style="17"/>
+    <col min="12" max="12" width="11.28515625" style="17" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="17"/>
+    <col min="14" max="14" width="9.7109375" style="17" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="17"/>
+    <col min="16" max="19" width="10" style="17" bestFit="1" customWidth="1"/>
+    <col min="20" max="23" width="9.140625" style="17"/>
+    <col min="24" max="25" width="10.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5">
       <c r="A1" s="16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5">
       <c r="A3" s="18" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="31" t="s">
+    <row r="4" spans="1:5" s="30" customFormat="1">
+      <c r="A4" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="30" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="31" t="s">
+    <row r="5" spans="1:5" s="30" customFormat="1">
+      <c r="A5" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="30" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="31" t="s">
+    <row r="6" spans="1:5" s="30" customFormat="1">
+      <c r="A6" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="30" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="31" t="s">
+    <row r="7" spans="1:5" s="30" customFormat="1">
+      <c r="A7" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="31">
         <f>C8*C9</f>
         <v>31.25</v>
       </c>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32">
+      <c r="D7" s="31"/>
+      <c r="E7" s="31">
         <f>E8*E9</f>
         <v>31.25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="31" t="s">
+    <row r="8" spans="1:5" s="30" customFormat="1">
+      <c r="A8" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="31">
         <v>12.5</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32">
+      <c r="D8" s="31"/>
+      <c r="E8" s="31">
         <v>12.5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="31" t="s">
+    <row r="9" spans="1:5" s="30" customFormat="1">
+      <c r="A9" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="31">
         <v>2.5</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32">
+      <c r="D9" s="31"/>
+      <c r="E9" s="31">
         <v>2.5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="31" t="s">
+    <row r="10" spans="1:5" s="30" customFormat="1">
+      <c r="A10" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="30">
         <v>18.7</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="30">
         <v>11</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E10" s="30">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="31" t="s">
+    <row r="11" spans="1:5" s="30" customFormat="1">
+      <c r="A11" s="30" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="31" t="s">
+    <row r="12" spans="1:5" s="30" customFormat="1">
+      <c r="A12" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="31">
+      <c r="C12" s="30">
         <v>132.25</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="30">
         <v>110.63</v>
       </c>
-      <c r="E12" s="31">
+      <c r="E12" s="30">
         <v>125.25</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="31" t="s">
+    <row r="13" spans="1:5" s="30" customFormat="1">
+      <c r="A13" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="30" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="33" t="s">
+    <row r="14" spans="1:5" s="27" customFormat="1">
+      <c r="A14" s="32" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="34" t="s">
+    <row r="15" spans="1:5" s="34" customFormat="1">
+      <c r="A15" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="34">
+      <c r="C15" s="33">
         <v>12.5</v>
       </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-    </row>
-    <row r="16" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="34" t="s">
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+    </row>
+    <row r="16" spans="1:5" s="34" customFormat="1">
+      <c r="A16" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="34">
+      <c r="C16" s="33">
         <v>2.5</v>
       </c>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-    </row>
-    <row r="17" spans="1:25" s="35" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="34" t="s">
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+    </row>
+    <row r="17" spans="1:25" s="34" customFormat="1">
+      <c r="A17" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="C17" s="34">
+      <c r="C17" s="33">
         <v>1.5</v>
       </c>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-    </row>
-    <row r="18" spans="1:25" s="35" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="34" t="s">
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+    </row>
+    <row r="18" spans="1:25" s="34" customFormat="1">
+      <c r="A18" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34" t="s">
+      <c r="B18" s="33"/>
+      <c r="C18" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-    </row>
-    <row r="19" spans="1:25" s="35" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="34" t="s">
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+    </row>
+    <row r="19" spans="1:25" s="34" customFormat="1">
+      <c r="A19" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34" t="s">
+      <c r="B19" s="33"/>
+      <c r="C19" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+    </row>
+    <row r="20" spans="1:25">
       <c r="A20" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C20" s="19"/>
     </row>
-    <row r="21" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="27" t="s">
+    <row r="21" spans="1:25" s="27" customFormat="1">
+      <c r="A21" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="26" t="s">
         <v>95</v>
       </c>
       <c r="C21" s="20">
@@ -3271,40 +3232,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="29" t="s">
+    <row r="22" spans="1:25" s="27" customFormat="1">
+      <c r="A22" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="27"/>
-      <c r="P22" s="27"/>
-      <c r="Q22" s="27"/>
-      <c r="R22" s="27"/>
-      <c r="S22" s="27"/>
-      <c r="T22" s="27"/>
-      <c r="U22" s="27"/>
-      <c r="V22" s="27"/>
-      <c r="W22" s="27"/>
-      <c r="X22" s="27"/>
-      <c r="Y22" s="27"/>
-    </row>
-    <row r="23" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="27" t="s">
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="26"/>
+      <c r="Q22" s="26"/>
+      <c r="R22" s="26"/>
+      <c r="S22" s="26"/>
+      <c r="T22" s="26"/>
+      <c r="U22" s="26"/>
+      <c r="V22" s="26"/>
+      <c r="W22" s="26"/>
+      <c r="X22" s="26"/>
+      <c r="Y22" s="26"/>
+    </row>
+    <row r="23" spans="1:25" s="27" customFormat="1">
+      <c r="A23" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="26" t="s">
         <v>61</v>
       </c>
       <c r="C23" s="20">
@@ -3338,19 +3299,19 @@
         <v>100</v>
       </c>
       <c r="M23" s="20">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="N23" s="20">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="O23" s="20">
         <v>100</v>
       </c>
       <c r="P23" s="20">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="Q23" s="20">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="R23" s="20">
         <v>100</v>
@@ -3377,11 +3338,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="30" t="s">
+    <row r="24" spans="1:25" s="27" customFormat="1">
+      <c r="A24" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="26" t="s">
         <v>61</v>
       </c>
       <c r="C24" s="20">
@@ -3430,19 +3391,19 @@
         <v>100</v>
       </c>
       <c r="R24" s="20">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="S24" s="20">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="T24" s="20">
         <v>100</v>
       </c>
       <c r="U24" s="20">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="V24" s="20">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="W24" s="20">
         <v>100</v>
@@ -3454,40 +3415,40 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="29" t="s">
+    <row r="25" spans="1:25" s="27" customFormat="1">
+      <c r="A25" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="30"/>
-      <c r="J25" s="30"/>
-      <c r="K25" s="30"/>
-      <c r="L25" s="30"/>
-      <c r="M25" s="27"/>
-      <c r="N25" s="30"/>
-      <c r="O25" s="30"/>
-      <c r="P25" s="30"/>
-      <c r="Q25" s="30"/>
-      <c r="R25" s="27"/>
-      <c r="S25" s="30"/>
-      <c r="T25" s="30"/>
-      <c r="U25" s="30"/>
-      <c r="V25" s="30"/>
-      <c r="W25" s="27"/>
-      <c r="X25" s="30"/>
-      <c r="Y25" s="30"/>
-    </row>
-    <row r="26" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="27" t="s">
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="29"/>
+      <c r="O25" s="29"/>
+      <c r="P25" s="29"/>
+      <c r="Q25" s="29"/>
+      <c r="R25" s="26"/>
+      <c r="S25" s="29"/>
+      <c r="T25" s="29"/>
+      <c r="U25" s="29"/>
+      <c r="V25" s="29"/>
+      <c r="W25" s="26"/>
+      <c r="X25" s="29"/>
+      <c r="Y25" s="29"/>
+    </row>
+    <row r="26" spans="1:25" s="27" customFormat="1">
+      <c r="A26" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="26" t="s">
         <v>62</v>
       </c>
       <c r="C26" s="24">
@@ -3532,11 +3493,11 @@
       </c>
       <c r="M26" s="24">
         <f>-22.11+2.12*M23</f>
-        <v>189.89</v>
+        <v>83.89</v>
       </c>
       <c r="N26" s="24">
         <f t="shared" ref="N26:Q26" si="2">-22.11+2.12*N23</f>
-        <v>189.89</v>
+        <v>136.88999999999999</v>
       </c>
       <c r="O26" s="24">
         <f t="shared" si="2"/>
@@ -3544,11 +3505,11 @@
       </c>
       <c r="P26" s="24">
         <f t="shared" si="2"/>
-        <v>189.89</v>
+        <v>242.89</v>
       </c>
       <c r="Q26" s="24">
         <f t="shared" si="2"/>
-        <v>189.89</v>
+        <v>295.89</v>
       </c>
       <c r="R26" s="24">
         <f>-22.11+2.12*R23</f>
@@ -3583,11 +3544,11 @@
         <v>189.89</v>
       </c>
     </row>
-    <row r="27" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="30" t="s">
+    <row r="27" spans="1:25" s="27" customFormat="1">
+      <c r="A27" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="26" t="s">
         <v>62</v>
       </c>
       <c r="C27" s="24">
@@ -3652,11 +3613,11 @@
       </c>
       <c r="R27" s="24">
         <f>-7.24+2.04*R24</f>
-        <v>196.76</v>
+        <v>94.76</v>
       </c>
       <c r="S27" s="24">
         <f t="shared" ref="S27:V27" si="8">-7.24+2.04*S24</f>
-        <v>196.76</v>
+        <v>145.76</v>
       </c>
       <c r="T27" s="24">
         <f t="shared" si="8"/>
@@ -3664,11 +3625,11 @@
       </c>
       <c r="U27" s="24">
         <f t="shared" si="8"/>
-        <v>196.76</v>
+        <v>247.76</v>
       </c>
       <c r="V27" s="24">
         <f t="shared" si="8"/>
-        <v>196.76</v>
+        <v>298.76</v>
       </c>
       <c r="W27" s="24">
         <f>-7.24+2.04*W24</f>
@@ -3683,459 +3644,459 @@
         <v>196.76</v>
       </c>
     </row>
-    <row r="28" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="29" t="s">
+    <row r="28" spans="1:25" s="27" customFormat="1">
+      <c r="A28" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="27"/>
-      <c r="M28" s="27"/>
-      <c r="N28" s="27"/>
-      <c r="O28" s="27"/>
-      <c r="R28" s="27"/>
-      <c r="S28" s="27"/>
-      <c r="T28" s="27"/>
-      <c r="W28" s="27"/>
-      <c r="X28" s="27"/>
-      <c r="Y28" s="27"/>
-    </row>
-    <row r="29" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="27" t="s">
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+      <c r="M28" s="26"/>
+      <c r="N28" s="26"/>
+      <c r="O28" s="26"/>
+      <c r="R28" s="26"/>
+      <c r="S28" s="26"/>
+      <c r="T28" s="26"/>
+      <c r="W28" s="26"/>
+      <c r="X28" s="26"/>
+      <c r="Y28" s="26"/>
+    </row>
+    <row r="29" spans="1:25" s="27" customFormat="1">
+      <c r="A29" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="41">
+      <c r="C29" s="40">
         <f>ExpData!N15</f>
         <v>1.0570055555555555E-2</v>
       </c>
-      <c r="D29" s="41">
+      <c r="D29" s="40">
         <f>ExpData!O15</f>
         <v>1.0570055555555555E-2</v>
       </c>
-      <c r="E29" s="41">
+      <c r="E29" s="40">
         <f>ExpData!P15</f>
         <v>1.0570055555555555E-2</v>
       </c>
-      <c r="F29" s="41">
+      <c r="F29" s="40">
         <f>ExpData!Q15</f>
         <v>1.0570055555555555E-2</v>
       </c>
-      <c r="G29" s="41">
+      <c r="G29" s="40">
         <f>ExpData!R15</f>
         <v>1.0570055555555555E-2</v>
       </c>
-      <c r="H29" s="41">
+      <c r="H29" s="40">
         <f>ExpData!S15</f>
         <v>1.0570055555555555E-2</v>
       </c>
-      <c r="I29" s="41">
+      <c r="I29" s="40">
         <f>ExpData!T15</f>
         <v>1.0570055555555555E-2</v>
       </c>
-      <c r="J29" s="41">
+      <c r="J29" s="40">
         <f>ExpData!U15</f>
         <v>1.0570055555555555E-2</v>
       </c>
-      <c r="K29" s="41">
+      <c r="K29" s="40">
         <f>ExpData!V15</f>
         <v>1.0570055555555555E-2</v>
       </c>
-      <c r="L29" s="41">
+      <c r="L29" s="40">
         <f>ExpData!W15</f>
         <v>1.0570055555555555E-2</v>
       </c>
-      <c r="M29" s="41">
+      <c r="M29" s="40">
         <f>ExpData!X15</f>
         <v>5.2783888888888889E-3</v>
       </c>
-      <c r="N29" s="41">
+      <c r="N29" s="40">
         <f>ExpData!Y15</f>
         <v>7.9242222222222214E-3</v>
       </c>
-      <c r="O29" s="41">
+      <c r="O29" s="40">
         <f>ExpData!Z15</f>
         <v>1.0570055555555555E-2</v>
       </c>
-      <c r="P29" s="41">
+      <c r="P29" s="40">
         <f>ExpData!AA15</f>
         <v>1.321588888888889E-2</v>
       </c>
-      <c r="Q29" s="41">
+      <c r="Q29" s="40">
         <f>ExpData!AB15</f>
         <v>1.5861722222222222E-2</v>
       </c>
-      <c r="R29" s="41">
+      <c r="R29" s="40">
         <f>ExpData!AC15</f>
         <v>1.0570055555555555E-2</v>
       </c>
-      <c r="S29" s="41">
+      <c r="S29" s="40">
         <f>ExpData!AD15</f>
         <v>1.0570055555555555E-2</v>
       </c>
-      <c r="T29" s="41">
+      <c r="T29" s="40">
         <f>ExpData!AE15</f>
         <v>1.0570055555555555E-2</v>
       </c>
-      <c r="U29" s="41">
+      <c r="U29" s="40">
         <f>ExpData!AF15</f>
         <v>1.0570055555555555E-2</v>
       </c>
-      <c r="V29" s="41">
+      <c r="V29" s="40">
         <f>ExpData!AG15</f>
         <v>1.0570055555555555E-2</v>
       </c>
-      <c r="W29" s="41">
+      <c r="W29" s="40">
         <f>ExpData!AH15</f>
         <v>1.0575562188444444E-2</v>
       </c>
-      <c r="X29" s="41">
+      <c r="X29" s="40">
         <f>ExpData!AI15</f>
         <v>1.0575562188444444E-2</v>
       </c>
-      <c r="Y29" s="41">
+      <c r="Y29" s="40">
         <f>ExpData!AJ15</f>
         <v>1.0575562188444444E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="27" t="s">
+    <row r="30" spans="1:25" s="27" customFormat="1">
+      <c r="A30" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="41">
+      <c r="C30" s="40">
         <f>ExpData!N16</f>
         <v>32.804908589380183</v>
       </c>
-      <c r="D30" s="41">
+      <c r="D30" s="40">
         <f>ExpData!O16</f>
         <v>37.545921167879214</v>
       </c>
-      <c r="E30" s="41">
+      <c r="E30" s="40">
         <f>ExpData!P16</f>
         <v>40.462794041113561</v>
       </c>
-      <c r="F30" s="41">
+      <c r="F30" s="40">
         <f>ExpData!Q16</f>
         <v>46.813272232415727</v>
       </c>
-      <c r="G30" s="41">
+      <c r="G30" s="40">
         <f>ExpData!R16</f>
         <v>52.28803056208195</v>
       </c>
-      <c r="H30" s="41">
+      <c r="H30" s="40">
         <f>ExpData!S16</f>
         <v>46.813272232415727</v>
       </c>
-      <c r="I30" s="41">
+      <c r="I30" s="40">
         <f>ExpData!T16</f>
         <v>46.735559551037205</v>
       </c>
-      <c r="J30" s="41">
+      <c r="J30" s="40">
         <f>ExpData!U16</f>
         <v>46.756376974131932</v>
       </c>
-      <c r="K30" s="41">
+      <c r="K30" s="40">
         <f>ExpData!V16</f>
         <v>46.759715513146396</v>
       </c>
-      <c r="L30" s="41">
+      <c r="L30" s="40">
         <f>ExpData!W16</f>
         <v>46.795754117384256</v>
       </c>
-      <c r="M30" s="41">
+      <c r="M30" s="40">
         <f>ExpData!X16</f>
         <v>46.765960784537164</v>
       </c>
-      <c r="N30" s="41">
+      <c r="N30" s="40">
         <f>ExpData!Y16</f>
         <v>46.747797849449768</v>
       </c>
-      <c r="O30" s="41">
+      <c r="O30" s="40">
         <f>ExpData!Z16</f>
         <v>46.813272232415727</v>
       </c>
-      <c r="P30" s="41">
+      <c r="P30" s="40">
         <f>ExpData!AA16</f>
         <v>46.780135265158755</v>
       </c>
-      <c r="Q30" s="41">
+      <c r="Q30" s="40">
         <f>ExpData!AB16</f>
         <v>46.785915070345858</v>
       </c>
-      <c r="R30" s="41">
+      <c r="R30" s="40">
         <f>ExpData!AC16</f>
         <v>46.831304444044484</v>
       </c>
-      <c r="S30" s="41">
+      <c r="S30" s="40">
         <f>ExpData!AD16</f>
         <v>46.835636390276221</v>
       </c>
-      <c r="T30" s="41">
+      <c r="T30" s="40">
         <f>ExpData!AE16</f>
         <v>46.813272232415727</v>
       </c>
-      <c r="U30" s="41">
+      <c r="U30" s="40">
         <f>ExpData!AF16</f>
         <v>46.773248419935193</v>
       </c>
-      <c r="V30" s="41">
+      <c r="V30" s="40">
         <f>ExpData!AG16</f>
         <v>46.772998389800364</v>
       </c>
-      <c r="W30" s="41">
+      <c r="W30" s="40">
         <f>ExpData!AH16</f>
         <v>46.813272232415727</v>
       </c>
-      <c r="X30" s="41">
+      <c r="X30" s="40">
         <f>ExpData!AI16</f>
         <v>46.83837113278085</v>
       </c>
-      <c r="Y30" s="41">
+      <c r="Y30" s="40">
         <f>ExpData!AJ16</f>
         <v>46.843521688179884</v>
       </c>
     </row>
-    <row r="31" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="29" t="s">
+    <row r="31" spans="1:25" s="27" customFormat="1">
+      <c r="A31" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="42"/>
-      <c r="K31" s="42"/>
-      <c r="L31" s="42"/>
-      <c r="M31" s="42"/>
-      <c r="N31" s="42"/>
-      <c r="O31" s="42"/>
-      <c r="P31" s="42"/>
-      <c r="Q31" s="42"/>
-      <c r="R31" s="42"/>
-      <c r="S31" s="42"/>
-      <c r="T31" s="42"/>
-      <c r="U31" s="42"/>
-      <c r="V31" s="42"/>
-      <c r="W31" s="42"/>
-      <c r="X31" s="42"/>
-      <c r="Y31" s="42"/>
-    </row>
-    <row r="32" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="27" t="s">
+      <c r="B31" s="26"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="41"/>
+      <c r="K31" s="41"/>
+      <c r="L31" s="41"/>
+      <c r="M31" s="41"/>
+      <c r="N31" s="41"/>
+      <c r="O31" s="41"/>
+      <c r="P31" s="41"/>
+      <c r="Q31" s="41"/>
+      <c r="R31" s="41"/>
+      <c r="S31" s="41"/>
+      <c r="T31" s="41"/>
+      <c r="U31" s="41"/>
+      <c r="V31" s="41"/>
+      <c r="W31" s="41"/>
+      <c r="X31" s="41"/>
+      <c r="Y31" s="41"/>
+    </row>
+    <row r="32" spans="1:25" s="27" customFormat="1">
+      <c r="A32" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="41">
+      <c r="C32" s="40">
         <f>ExpData!N18</f>
         <v>1.0024555555555557E-2</v>
       </c>
-      <c r="D32" s="41">
+      <c r="D32" s="40">
         <f>ExpData!O18</f>
         <v>1.0024555555555557E-2</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="40">
         <f>ExpData!P18</f>
         <v>1.0024555555555557E-2</v>
       </c>
-      <c r="F32" s="41">
+      <c r="F32" s="40">
         <f>ExpData!Q18</f>
         <v>1.0024555555555557E-2</v>
       </c>
-      <c r="G32" s="41">
+      <c r="G32" s="40">
         <f>ExpData!R18</f>
         <v>1.0024555555555557E-2</v>
       </c>
-      <c r="H32" s="41">
+      <c r="H32" s="40">
         <f>ExpData!S18</f>
         <v>1.0024555555555557E-2</v>
       </c>
-      <c r="I32" s="41">
+      <c r="I32" s="40">
         <f>ExpData!T18</f>
         <v>1.0024555555555557E-2</v>
       </c>
-      <c r="J32" s="41">
+      <c r="J32" s="40">
         <f>ExpData!U18</f>
         <v>1.0024555555555557E-2</v>
       </c>
-      <c r="K32" s="41">
+      <c r="K32" s="40">
         <f>ExpData!V18</f>
         <v>1.0024555555555557E-2</v>
       </c>
-      <c r="L32" s="41">
+      <c r="L32" s="40">
         <f>ExpData!W18</f>
         <v>1.0024555555555557E-2</v>
       </c>
-      <c r="M32" s="41">
+      <c r="M32" s="40">
         <f>ExpData!X18</f>
         <v>1.0024555555555557E-2</v>
       </c>
-      <c r="N32" s="41">
+      <c r="N32" s="40">
         <f>ExpData!Y18</f>
         <v>1.0024555555555557E-2</v>
       </c>
-      <c r="O32" s="41">
+      <c r="O32" s="40">
         <f>ExpData!Z18</f>
         <v>1.0024555555555557E-2</v>
       </c>
-      <c r="P32" s="41">
+      <c r="P32" s="40">
         <f>ExpData!AA18</f>
         <v>1.0024555555555557E-2</v>
       </c>
-      <c r="Q32" s="41">
+      <c r="Q32" s="40">
         <f>ExpData!AB18</f>
         <v>1.0024555555555571E-2</v>
       </c>
-      <c r="R32" s="41">
+      <c r="R32" s="40">
         <f>ExpData!AC18</f>
         <v>4.9995555555555557E-3</v>
       </c>
-      <c r="S32" s="41">
+      <c r="S32" s="40">
         <f>ExpData!AD18</f>
         <v>7.5120555555555539E-3</v>
       </c>
-      <c r="T32" s="41">
+      <c r="T32" s="40">
         <f>ExpData!AE18</f>
         <v>1.0024555555555557E-2</v>
       </c>
-      <c r="U32" s="41">
+      <c r="U32" s="40">
         <f>ExpData!AF18</f>
         <v>1.2537055555555556E-2</v>
       </c>
-      <c r="V32" s="41">
+      <c r="V32" s="40">
         <f>ExpData!AG18</f>
         <v>1.5049555555555552E-2</v>
       </c>
-      <c r="W32" s="41">
+      <c r="W32" s="40">
         <f>ExpData!AH18</f>
         <v>1.0878928809055555E-2</v>
       </c>
-      <c r="X32" s="41">
+      <c r="X32" s="40">
         <f>ExpData!AI18</f>
         <v>1.0878928809055555E-2</v>
       </c>
-      <c r="Y32" s="41">
+      <c r="Y32" s="40">
         <f>ExpData!AJ18</f>
         <v>1.0878928809055555E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="27" t="s">
+    <row r="33" spans="1:25" s="27" customFormat="1">
+      <c r="A33" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B33" s="27" t="s">
+      <c r="B33" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="C33" s="41">
+      <c r="C33" s="40">
         <f>ExpData!N19</f>
         <v>20.020584823493895</v>
       </c>
-      <c r="D33" s="41">
+      <c r="D33" s="40">
         <f>ExpData!O19</f>
         <v>20.013996907080195</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="40">
         <f>ExpData!P19</f>
         <v>20.040555205268429</v>
       </c>
-      <c r="F33" s="41">
+      <c r="F33" s="40">
         <f>ExpData!Q19</f>
         <v>19.965192717598594</v>
       </c>
-      <c r="G33" s="41">
+      <c r="G33" s="40">
         <f>ExpData!R19</f>
         <v>20.531591054442632</v>
       </c>
-      <c r="H33" s="41">
+      <c r="H33" s="40">
         <f>ExpData!S19</f>
         <v>19.965192717598594</v>
       </c>
-      <c r="I33" s="41">
+      <c r="I33" s="40">
         <f>ExpData!T19</f>
         <v>25.020477816258023</v>
       </c>
-      <c r="J33" s="41">
+      <c r="J33" s="40">
         <f>ExpData!U19</f>
         <v>29.996660937349375</v>
       </c>
-      <c r="K33" s="41">
+      <c r="K33" s="40">
         <f>ExpData!V19</f>
         <v>34.981044802983121</v>
       </c>
-      <c r="L33" s="41">
+      <c r="L33" s="40">
         <f>ExpData!W19</f>
         <v>39.995611966534248</v>
       </c>
-      <c r="M33" s="41">
+      <c r="M33" s="40">
         <f>ExpData!X19</f>
         <v>19.95147626262694</v>
       </c>
-      <c r="N33" s="41">
+      <c r="N33" s="40">
         <f>ExpData!Y19</f>
         <v>19.98472615642196</v>
       </c>
-      <c r="O33" s="41">
+      <c r="O33" s="40">
         <f>ExpData!Z19</f>
         <v>19.965192717598594</v>
       </c>
-      <c r="P33" s="41">
+      <c r="P33" s="40">
         <f>ExpData!AA19</f>
         <v>19.98426554012838</v>
       </c>
-      <c r="Q33" s="41">
+      <c r="Q33" s="40">
         <f>ExpData!AB19</f>
         <v>20.033552339221512</v>
       </c>
-      <c r="R33" s="41">
+      <c r="R33" s="40">
         <f>ExpData!AC19</f>
         <v>19.99611427063822</v>
       </c>
-      <c r="S33" s="41">
+      <c r="S33" s="40">
         <f>ExpData!AD19</f>
         <v>19.985256383306695</v>
       </c>
-      <c r="T33" s="41">
+      <c r="T33" s="40">
         <f>ExpData!AE19</f>
         <v>19.965192717598594</v>
       </c>
-      <c r="U33" s="41">
+      <c r="U33" s="40">
         <f>ExpData!AF19</f>
         <v>19.978884732789933</v>
       </c>
-      <c r="V33" s="41">
+      <c r="V33" s="40">
         <f>ExpData!AG19</f>
         <v>19.940144584158414</v>
       </c>
-      <c r="W33" s="41">
+      <c r="W33" s="40">
         <f>ExpData!AH19</f>
         <v>19.965192717598594</v>
       </c>
-      <c r="X33" s="41">
+      <c r="X33" s="40">
         <f>ExpData!AI19</f>
         <v>19.962840387781814</v>
       </c>
-      <c r="Y33" s="41">
+      <c r="Y33" s="40">
         <f>ExpData!AJ19</f>
         <v>19.94308391529044</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:25">
       <c r="A34" s="18" t="s">
         <v>70</v>
       </c>
@@ -4163,409 +4124,409 @@
       <c r="X34" s="19"/>
       <c r="Y34" s="19"/>
     </row>
-    <row r="35" spans="1:25" s="26" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="26" t="s">
+    <row r="35" spans="1:25" s="25" customFormat="1">
+      <c r="A35" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="41">
+      <c r="C35" s="40">
         <f>ExpData!N21</f>
         <v>32.209159619805561</v>
       </c>
-      <c r="D35" s="41">
+      <c r="D35" s="40">
         <f>ExpData!O21</f>
         <v>36.641882535934052</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="40">
         <f>ExpData!P21</f>
         <v>39.206231593240013</v>
       </c>
-      <c r="F35" s="41">
+      <c r="F35" s="40">
         <f>ExpData!Q21</f>
         <v>45.115007004655496</v>
       </c>
-      <c r="G35" s="41">
+      <c r="G35" s="40">
         <f>ExpData!R21</f>
         <v>50.488628590359532</v>
       </c>
-      <c r="H35" s="41">
+      <c r="H35" s="40">
         <f>ExpData!S21</f>
         <v>45.115007004655496</v>
       </c>
-      <c r="I35" s="41">
+      <c r="I35" s="40">
         <f>ExpData!T21</f>
         <v>45.152704364084947</v>
       </c>
-      <c r="J35" s="41">
+      <c r="J35" s="40">
         <f>ExpData!U21</f>
         <v>45.332937279628425</v>
       </c>
-      <c r="K35" s="41">
+      <c r="K35" s="40">
         <f>ExpData!V21</f>
         <v>45.65301197436299</v>
       </c>
-      <c r="L35" s="41">
+      <c r="L35" s="40">
         <f>ExpData!W21</f>
         <v>45.862899949634645</v>
       </c>
-      <c r="M35" s="41">
+      <c r="M35" s="40">
         <f>ExpData!X21</f>
         <v>46.414726050719302</v>
       </c>
-      <c r="N35" s="41">
+      <c r="N35" s="40">
         <f>ExpData!Y21</f>
         <v>45.253056164715588</v>
       </c>
-      <c r="O35" s="41">
+      <c r="O35" s="40">
         <f>ExpData!Z21</f>
         <v>45.115007004655496</v>
       </c>
-      <c r="P35" s="41">
+      <c r="P35" s="40">
         <f>ExpData!AA21</f>
         <v>45.554121695468943</v>
       </c>
-      <c r="Q35" s="41">
+      <c r="Q35" s="40">
         <f>ExpData!AB21</f>
         <v>45.667769594471679</v>
       </c>
-      <c r="R35" s="41">
+      <c r="R35" s="40">
         <f>ExpData!AC21</f>
         <v>45.410532556242877</v>
       </c>
-      <c r="S35" s="41">
+      <c r="S35" s="40">
         <f>ExpData!AD21</f>
         <v>45.366644909743457</v>
       </c>
-      <c r="T35" s="41">
+      <c r="T35" s="40">
         <f>ExpData!AE21</f>
         <v>45.115007004655496</v>
       </c>
-      <c r="U35" s="41">
+      <c r="U35" s="40">
         <f>ExpData!AF21</f>
         <v>45.184878246406505</v>
       </c>
-      <c r="V35" s="41">
+      <c r="V35" s="40">
         <f>ExpData!AG21</f>
         <v>45.148270505308638</v>
       </c>
-      <c r="W35" s="41">
+      <c r="W35" s="40">
         <f>ExpData!AH21</f>
         <v>45.115007004655496</v>
       </c>
-      <c r="X35" s="41">
+      <c r="X35" s="40">
         <f>ExpData!AI21</f>
         <v>45.243818979301523</v>
       </c>
-      <c r="Y35" s="41">
+      <c r="Y35" s="40">
         <f>ExpData!AJ21</f>
         <v>44.928683240302114</v>
       </c>
     </row>
-    <row r="36" spans="1:25" s="26" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="26" t="s">
+    <row r="36" spans="1:25" s="25" customFormat="1">
+      <c r="A36" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="41">
+      <c r="C36" s="40">
         <f>ExpData!N22</f>
         <v>21.1468268936618</v>
       </c>
-      <c r="D36" s="41">
+      <c r="D36" s="40">
         <f>ExpData!O22</f>
         <v>21.066646083396979</v>
       </c>
-      <c r="E36" s="41">
+      <c r="E36" s="40">
         <f>ExpData!P22</f>
         <v>21.202254882336835</v>
       </c>
-      <c r="F36" s="41">
+      <c r="F36" s="40">
         <f>ExpData!Q22</f>
         <v>21.428861307302665</v>
       </c>
-      <c r="G36" s="41">
+      <c r="G36" s="40">
         <f>ExpData!R22</f>
         <v>21.993250061846652</v>
       </c>
-      <c r="H36" s="41">
+      <c r="H36" s="40">
         <f>ExpData!S22</f>
         <v>21.428861307302665</v>
       </c>
-      <c r="I36" s="41">
+      <c r="I36" s="40">
         <f>ExpData!T22</f>
         <v>26.071689439399325</v>
       </c>
-      <c r="J36" s="41">
+      <c r="J36" s="40">
         <f>ExpData!U22</f>
         <v>30.76148736331346</v>
       </c>
-      <c r="K36" s="41">
+      <c r="K36" s="40">
         <f>ExpData!V22</f>
         <v>35.502290509265826</v>
       </c>
-      <c r="L36" s="41">
+      <c r="L36" s="40">
         <f>ExpData!W22</f>
         <v>40.423454833974333</v>
       </c>
-      <c r="M36" s="41">
+      <c r="M36" s="40">
         <f>ExpData!X22</f>
         <v>21.494944118539394</v>
       </c>
-      <c r="N36" s="41">
+      <c r="N36" s="40">
         <f>ExpData!Y22</f>
         <v>21.517883020301912</v>
       </c>
-      <c r="O36" s="41">
+      <c r="O36" s="40">
         <f>ExpData!Z22</f>
         <v>21.428861307302665</v>
       </c>
-      <c r="P36" s="41">
+      <c r="P36" s="40">
         <f>ExpData!AA22</f>
         <v>21.595394953178555</v>
       </c>
-      <c r="Q36" s="41">
+      <c r="Q36" s="40">
         <f>ExpData!AB22</f>
         <v>21.805176462942171</v>
       </c>
-      <c r="R36" s="41">
+      <c r="R36" s="40">
         <f>ExpData!AC22</f>
         <v>21.733402276973759</v>
       </c>
-      <c r="S36" s="41">
+      <c r="S36" s="40">
         <f>ExpData!AD22</f>
         <v>21.854517375313929</v>
       </c>
-      <c r="T36" s="41">
+      <c r="T36" s="40">
         <f>ExpData!AE22</f>
         <v>21.428861307302665</v>
       </c>
-      <c r="U36" s="41">
+      <c r="U36" s="40">
         <f>ExpData!AF22</f>
         <v>21.479081058045157</v>
       </c>
-      <c r="V36" s="41">
+      <c r="V36" s="40">
         <f>ExpData!AG22</f>
         <v>21.310467600503262</v>
       </c>
-      <c r="W36" s="41">
+      <c r="W36" s="40">
         <f>ExpData!AH22</f>
         <v>21.428861307302665</v>
       </c>
-      <c r="X36" s="41">
+      <c r="X36" s="40">
         <f>ExpData!AI22</f>
         <v>21.478318390552261</v>
       </c>
-      <c r="Y36" s="41">
+      <c r="Y36" s="40">
         <f>ExpData!AJ22</f>
         <v>21.306892948428231</v>
       </c>
     </row>
-    <row r="37" spans="1:25" s="26" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="26" t="s">
+    <row r="37" spans="1:25" s="25" customFormat="1">
+      <c r="A37" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="41">
+      <c r="C37" s="40">
         <f>ExpData!N23</f>
         <v>3.8848588799999995</v>
       </c>
-      <c r="D37" s="41">
+      <c r="D37" s="40">
         <f>ExpData!O23</f>
         <v>5.667941375999999</v>
       </c>
-      <c r="E37" s="41">
+      <c r="E37" s="40">
         <f>ExpData!P23</f>
         <v>7.0075795200000002</v>
       </c>
-      <c r="F37" s="41">
+      <c r="F37" s="40">
         <f>ExpData!Q23</f>
         <v>10.728884735999999</v>
       </c>
-      <c r="G37" s="41">
+      <c r="G37" s="40">
         <f>ExpData!R23</f>
         <v>14.106180095999997</v>
       </c>
-      <c r="H37" s="41">
+      <c r="H37" s="40">
         <f>ExpData!S23</f>
         <v>10.728884735999999</v>
       </c>
-      <c r="I37" s="41">
+      <c r="I37" s="40">
         <f>ExpData!T23</f>
         <v>9.2522250239999995</v>
       </c>
-      <c r="J37" s="41">
+      <c r="J37" s="40">
         <f>ExpData!U23</f>
         <v>7.6446888960000008</v>
       </c>
-      <c r="K37" s="41">
+      <c r="K37" s="40">
         <f>ExpData!V23</f>
         <v>5.6193918719999987</v>
       </c>
-      <c r="L37" s="41">
+      <c r="L37" s="40">
         <f>ExpData!W23</f>
         <v>3.5767384319999995</v>
       </c>
-      <c r="M37" s="41">
+      <c r="M37" s="40">
         <f>ExpData!X23</f>
         <v>10.576399104</v>
       </c>
-      <c r="N37" s="41">
+      <c r="N37" s="40">
         <f>ExpData!Y23</f>
         <v>10.284390143999998</v>
       </c>
-      <c r="O37" s="41">
+      <c r="O37" s="40">
         <f>ExpData!Z23</f>
         <v>10.728884735999999</v>
       </c>
-      <c r="P37" s="41">
+      <c r="P37" s="40">
         <f>ExpData!AA23</f>
         <v>10.960891391999999</v>
       </c>
-      <c r="Q37" s="41">
+      <c r="Q37" s="40">
         <f>ExpData!AB23</f>
         <v>11.167119743999999</v>
       </c>
-      <c r="R37" s="41">
+      <c r="R37" s="40">
         <f>ExpData!AC23</f>
         <v>9.8861740800000018</v>
       </c>
-      <c r="S37" s="41">
+      <c r="S37" s="40">
         <f>ExpData!AD23</f>
         <v>10.167006336</v>
       </c>
-      <c r="T37" s="41">
+      <c r="T37" s="40">
         <f>ExpData!AE23</f>
         <v>10.728884735999999</v>
       </c>
-      <c r="U37" s="41">
+      <c r="U37" s="40">
         <f>ExpData!AF23</f>
         <v>11.559156864</v>
       </c>
-      <c r="V37" s="41">
+      <c r="V37" s="40">
         <f>ExpData!AG23</f>
         <v>11.892979584000001</v>
       </c>
-      <c r="W37" s="41">
+      <c r="W37" s="40">
         <f>ExpData!AH23</f>
         <v>10.728884735999999</v>
       </c>
-      <c r="X37" s="41">
+      <c r="X37" s="40">
         <f>ExpData!AI23</f>
         <v>3.5032684799999991</v>
       </c>
-      <c r="Y37" s="41">
+      <c r="Y37" s="40">
         <f>ExpData!AJ23</f>
         <v>4.8133098240000001</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:25">
       <c r="A38" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C38" s="54" t="str">
+      <c r="C38" s="53" t="str">
         <f>ExpData!N24</f>
         <v/>
       </c>
-      <c r="D38" s="54" t="str">
+      <c r="D38" s="53" t="str">
         <f>ExpData!O24</f>
         <v/>
       </c>
-      <c r="E38" s="54" t="str">
+      <c r="E38" s="53" t="str">
         <f>ExpData!P24</f>
         <v/>
       </c>
-      <c r="F38" s="54" t="str">
+      <c r="F38" s="53" t="str">
         <f>ExpData!Q24</f>
         <v/>
       </c>
-      <c r="G38" s="54" t="str">
+      <c r="G38" s="53" t="str">
         <f>ExpData!R24</f>
         <v/>
       </c>
-      <c r="H38" s="54" t="str">
+      <c r="H38" s="53" t="str">
         <f>ExpData!S24</f>
         <v>duplicate</v>
       </c>
-      <c r="I38" s="54" t="str">
+      <c r="I38" s="53" t="str">
         <f>ExpData!T24</f>
         <v/>
       </c>
-      <c r="J38" s="54" t="str">
+      <c r="J38" s="53" t="str">
         <f>ExpData!U24</f>
         <v/>
       </c>
-      <c r="K38" s="54" t="str">
+      <c r="K38" s="53" t="str">
         <f>ExpData!V24</f>
         <v/>
       </c>
-      <c r="L38" s="54" t="str">
+      <c r="L38" s="53" t="str">
         <f>ExpData!W24</f>
         <v/>
       </c>
-      <c r="M38" s="54" t="str">
+      <c r="M38" s="53" t="str">
         <f>ExpData!X24</f>
         <v/>
       </c>
-      <c r="N38" s="54" t="str">
+      <c r="N38" s="53" t="str">
         <f>ExpData!Y24</f>
         <v/>
       </c>
-      <c r="O38" s="54" t="str">
+      <c r="O38" s="53" t="str">
         <f>ExpData!Z24</f>
         <v>duplicate</v>
       </c>
-      <c r="P38" s="54" t="str">
+      <c r="P38" s="53" t="str">
         <f>ExpData!AA24</f>
         <v/>
       </c>
-      <c r="Q38" s="54" t="str">
+      <c r="Q38" s="53" t="str">
         <f>ExpData!AB24</f>
         <v/>
       </c>
-      <c r="R38" s="54" t="str">
+      <c r="R38" s="53" t="str">
         <f>ExpData!AC24</f>
         <v/>
       </c>
-      <c r="S38" s="54" t="str">
+      <c r="S38" s="53" t="str">
         <f>ExpData!AD24</f>
         <v/>
       </c>
-      <c r="T38" s="54" t="str">
+      <c r="T38" s="53" t="str">
         <f>ExpData!AE24</f>
         <v>duplicate</v>
       </c>
-      <c r="U38" s="54" t="str">
+      <c r="U38" s="53" t="str">
         <f>ExpData!AF24</f>
         <v/>
       </c>
-      <c r="V38" s="54" t="str">
+      <c r="V38" s="53" t="str">
         <f>ExpData!AG24</f>
         <v/>
       </c>
-      <c r="W38" s="54" t="str">
+      <c r="W38" s="53" t="str">
         <f>ExpData!AH24</f>
         <v>duplicate</v>
       </c>
-      <c r="X38" s="54" t="str">
+      <c r="X38" s="53" t="str">
         <f>ExpData!AI24</f>
         <v/>
       </c>
-      <c r="Y38" s="54" t="str">
+      <c r="Y38" s="53" t="str">
         <f>ExpData!AJ24</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:25">
       <c r="A39" s="18" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:25">
       <c r="A40" s="18" t="s">
         <v>100</v>
       </c>
@@ -4574,21 +4535,21 @@
       <c r="J40"/>
       <c r="K40"/>
       <c r="L40"/>
-      <c r="M40" s="43"/>
-      <c r="N40" s="43"/>
-      <c r="O40" s="43"/>
-      <c r="P40" s="43"/>
-      <c r="Q40" s="43"/>
-      <c r="R40" s="43"/>
-      <c r="S40" s="43"/>
-      <c r="T40" s="43"/>
-      <c r="U40" s="43"/>
-      <c r="V40" s="43"/>
-      <c r="W40" s="43"/>
-      <c r="X40" s="43"/>
-      <c r="Y40" s="43"/>
-    </row>
-    <row r="41" spans="1:25" s="56" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M40" s="42"/>
+      <c r="N40" s="42"/>
+      <c r="O40" s="42"/>
+      <c r="P40" s="42"/>
+      <c r="Q40" s="42"/>
+      <c r="R40" s="42"/>
+      <c r="S40" s="42"/>
+      <c r="T40" s="42"/>
+      <c r="U40" s="42"/>
+      <c r="V40" s="42"/>
+      <c r="W40" s="42"/>
+      <c r="X40" s="42"/>
+      <c r="Y40" s="42"/>
+    </row>
+    <row r="41" spans="1:25" s="56" customFormat="1">
       <c r="A41" s="56" t="s">
         <v>87</v>
       </c>
@@ -4637,11 +4598,11 @@
       </c>
       <c r="M41" s="57">
         <f t="shared" si="10"/>
-        <v>8.4395555555555543E-3</v>
+        <v>3.7284444444444444E-3</v>
       </c>
       <c r="N41" s="57">
         <f t="shared" si="10"/>
-        <v>8.4395555555555543E-3</v>
+        <v>6.084E-3</v>
       </c>
       <c r="O41" s="57">
         <f t="shared" si="10"/>
@@ -4688,7 +4649,7 @@
         <v>1.0575562188444444E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:25" s="56" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:25" s="56" customFormat="1">
       <c r="A42" s="56" t="s">
         <v>102</v>
       </c>
@@ -4788,7 +4749,7 @@
         <v>319.99352168817984</v>
       </c>
     </row>
-    <row r="43" spans="1:25" s="56" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:25" s="56" customFormat="1">
       <c r="A43" s="56" t="s">
         <v>101</v>
       </c>
@@ -4888,12 +4849,12 @@
         <v>318.0786832403021</v>
       </c>
     </row>
-    <row r="44" spans="1:25" s="56" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="58" t="s">
+    <row r="44" spans="1:25" s="56" customFormat="1">
+      <c r="A44" s="32" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="45" spans="1:25" s="56" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:25" s="56" customFormat="1">
       <c r="A45" s="56" t="s">
         <v>87</v>
       </c>
@@ -4993,7 +4954,7 @@
         <v>1.0878928809055555E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:25" s="56" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:25" s="56" customFormat="1">
       <c r="A46" s="56" t="s">
         <v>102</v>
       </c>
@@ -5093,7 +5054,7 @@
         <v>293.09308391529044</v>
       </c>
     </row>
-    <row r="47" spans="1:25" s="56" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:25" s="56" customFormat="1">
       <c r="A47" s="56" t="s">
         <v>101</v>
       </c>
@@ -5193,8 +5154,8 @@
         <v>294.45689294842822</v>
       </c>
     </row>
-    <row r="48" spans="1:25" s="56" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="58" t="s">
+    <row r="48" spans="1:25" s="56" customFormat="1">
+      <c r="A48" s="32" t="s">
         <v>71</v>
       </c>
       <c r="B48" s="56" t="s">
@@ -5293,378 +5254,378 @@
         <v>1.3370305066666666E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:25" customFormat="1">
       <c r="A49" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="H49" s="36"/>
-      <c r="I49" s="36"/>
-      <c r="J49" s="36"/>
-      <c r="K49" s="36"/>
-      <c r="L49" s="36"/>
-    </row>
-    <row r="50" spans="1:25" s="36" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="37" t="s">
+      <c r="H49" s="35"/>
+      <c r="I49" s="35"/>
+      <c r="J49" s="35"/>
+      <c r="K49" s="35"/>
+      <c r="L49" s="35"/>
+    </row>
+    <row r="50" spans="1:25" s="35" customFormat="1">
+      <c r="A50" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="B50" s="36" t="s">
+      <c r="B50" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="C50" s="36">
+      <c r="C50" s="35">
         <v>1</v>
       </c>
-      <c r="D50" s="36">
+      <c r="D50" s="35">
         <v>2</v>
       </c>
-      <c r="E50" s="36">
+      <c r="E50" s="35">
         <v>3</v>
       </c>
-      <c r="F50" s="36">
+      <c r="F50" s="35">
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:25" s="36" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="37" t="s">
+    <row r="51" spans="1:25" s="35" customFormat="1">
+      <c r="A51" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="B51" s="36" t="s">
+      <c r="B51" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="C51" s="36">
+      <c r="C51" s="35">
         <v>304.49</v>
       </c>
-      <c r="D51" s="36">
+      <c r="D51" s="35">
         <v>308.7</v>
       </c>
-      <c r="E51" s="36">
+      <c r="E51" s="35">
         <v>311.29000000000002</v>
       </c>
-      <c r="F51" s="36">
+      <c r="F51" s="35">
         <v>317.02</v>
       </c>
     </row>
-    <row r="52" spans="1:25" s="36" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="37" t="s">
+    <row r="52" spans="1:25" s="35" customFormat="1">
+      <c r="A52" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="B52" s="36" t="s">
+      <c r="B52" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="C52" s="36">
+      <c r="C52" s="35">
         <v>294.58999999999997</v>
       </c>
-      <c r="D52" s="36">
+      <c r="D52" s="35">
         <v>295.12</v>
       </c>
-      <c r="E52" s="36">
+      <c r="E52" s="35">
         <v>295.47000000000003</v>
       </c>
-      <c r="F52" s="36">
+      <c r="F52" s="35">
         <v>296.02</v>
       </c>
     </row>
-    <row r="53" spans="1:25" s="36" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="36" t="s">
+    <row r="53" spans="1:25" s="35" customFormat="1">
+      <c r="A53" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B53" s="36" t="s">
+      <c r="B53" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="C53" s="38">
+      <c r="C53" s="37">
         <v>9.6889999999999997E-4</v>
       </c>
-      <c r="D53" s="38">
+      <c r="D53" s="37">
         <v>1.387E-3</v>
       </c>
-      <c r="E53" s="38">
+      <c r="E53" s="37">
         <v>1.7049999999999999E-3</v>
       </c>
-      <c r="F53" s="38">
+      <c r="F53" s="37">
         <v>2.3249999999999998E-3</v>
       </c>
-      <c r="G53" s="38"/>
-      <c r="H53" s="28"/>
-      <c r="I53" s="28"/>
-      <c r="J53" s="28"/>
-      <c r="K53" s="28"/>
-      <c r="L53" s="28"/>
-    </row>
-    <row r="54" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="E54" s="39"/>
-      <c r="H54" s="40"/>
-      <c r="I54" s="40"/>
-      <c r="J54" s="40"/>
-      <c r="K54" s="40"/>
-      <c r="L54" s="40"/>
-    </row>
-    <row r="55" spans="1:25" s="40" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="40" t="s">
+      <c r="G53" s="37"/>
+      <c r="H53" s="27"/>
+      <c r="I53" s="27"/>
+      <c r="J53" s="27"/>
+      <c r="K53" s="27"/>
+      <c r="L53" s="27"/>
+    </row>
+    <row r="54" spans="1:25" s="27" customFormat="1">
+      <c r="E54" s="38"/>
+      <c r="H54" s="39"/>
+      <c r="I54" s="39"/>
+      <c r="J54" s="39"/>
+      <c r="K54" s="39"/>
+      <c r="L54" s="39"/>
+    </row>
+    <row r="55" spans="1:25" s="39" customFormat="1">
+      <c r="A55" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="B55" s="40" t="s">
+      <c r="B55" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="C55" s="40">
+      <c r="C55" s="39">
         <v>1</v>
       </c>
-      <c r="D55" s="40">
+      <c r="D55" s="39">
         <v>2</v>
       </c>
-      <c r="E55" s="40">
+      <c r="E55" s="39">
         <v>3</v>
       </c>
-      <c r="F55" s="40">
+      <c r="F55" s="39">
         <v>4</v>
       </c>
-      <c r="G55" s="40">
+      <c r="G55" s="39">
         <v>5</v>
       </c>
-      <c r="I55" s="40">
+      <c r="I55" s="39">
         <v>6</v>
       </c>
-      <c r="J55" s="40">
+      <c r="J55" s="39">
         <v>7</v>
       </c>
-      <c r="K55" s="40">
+      <c r="K55" s="39">
         <v>8</v>
       </c>
-      <c r="L55" s="40">
+      <c r="L55" s="39">
         <v>9</v>
       </c>
-      <c r="M55" s="40">
+      <c r="M55" s="39">
         <v>10</v>
       </c>
-      <c r="N55" s="40">
+      <c r="N55" s="39">
         <v>11</v>
       </c>
-      <c r="P55" s="40">
+      <c r="P55" s="39">
         <v>12</v>
       </c>
-      <c r="Q55" s="40">
+      <c r="Q55" s="39">
         <v>13</v>
       </c>
-      <c r="R55" s="40">
+      <c r="R55" s="39">
         <v>14</v>
       </c>
-      <c r="S55" s="40">
+      <c r="S55" s="39">
         <v>15</v>
       </c>
-      <c r="U55" s="40">
+      <c r="U55" s="39">
         <v>16</v>
       </c>
-      <c r="V55" s="40">
+      <c r="V55" s="39">
         <v>17</v>
       </c>
-      <c r="X55" s="40">
+      <c r="X55" s="39">
         <v>18</v>
       </c>
-      <c r="Y55" s="40">
+      <c r="Y55" s="39">
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:25" s="40" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="40" t="s">
+    <row r="56" spans="1:25" s="39" customFormat="1">
+      <c r="A56" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="B56" s="40" t="s">
+      <c r="B56" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="C56" s="40">
+      <c r="C56" s="39">
         <v>305.07</v>
       </c>
-      <c r="D56" s="40">
+      <c r="D56" s="39">
         <v>309.42</v>
       </c>
-      <c r="E56" s="40">
+      <c r="E56" s="39">
         <v>312.06</v>
       </c>
-      <c r="F56" s="40">
+      <c r="F56" s="39">
         <v>317.77999999999997</v>
       </c>
-      <c r="G56" s="40">
+      <c r="G56" s="39">
         <f>SimRecords!$B$5</f>
         <v>322.74</v>
       </c>
-      <c r="I56" s="40">
+      <c r="I56" s="39">
         <v>318.13</v>
       </c>
-      <c r="J56" s="40">
+      <c r="J56" s="39">
         <v>318.58</v>
       </c>
-      <c r="K56" s="40">
+      <c r="K56" s="39">
         <v>319.00351000000001</v>
       </c>
-      <c r="L56" s="40">
+      <c r="L56" s="39">
         <v>319.28005999999999</v>
       </c>
-      <c r="M56" s="40">
+      <c r="M56" s="39">
         <v>317.73446999999999</v>
       </c>
-      <c r="N56" s="40">
+      <c r="N56" s="39">
         <v>317.72046</v>
       </c>
-      <c r="P56" s="40">
+      <c r="P56" s="39">
         <v>318.26294000000001</v>
       </c>
-      <c r="Q56" s="40">
+      <c r="Q56" s="39">
         <v>318.48025999999999</v>
       </c>
-      <c r="R56" s="40">
+      <c r="R56" s="39">
         <v>318.41379000000001</v>
       </c>
-      <c r="S56" s="40">
+      <c r="S56" s="39">
         <v>318.17993000000001</v>
       </c>
-      <c r="U56" s="40">
+      <c r="U56" s="39">
         <v>317.89227</v>
       </c>
-      <c r="V56" s="40">
+      <c r="V56" s="39">
         <v>317.83413999999999</v>
       </c>
-      <c r="X56" s="40">
+      <c r="X56" s="39">
         <v>318.00452000000001</v>
       </c>
-      <c r="Y56" s="40">
+      <c r="Y56" s="39">
         <v>318.00878999999998</v>
       </c>
     </row>
-    <row r="57" spans="1:25" s="40" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="40" t="s">
+    <row r="57" spans="1:25" s="39" customFormat="1">
+      <c r="A57" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="B57" s="40" t="s">
+      <c r="B57" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="C57" s="40">
+      <c r="C57" s="39">
         <v>294.04000000000002</v>
       </c>
-      <c r="D57" s="40">
+      <c r="D57" s="39">
         <v>294.45</v>
       </c>
-      <c r="E57" s="40">
+      <c r="E57" s="39">
         <v>294.75</v>
       </c>
-      <c r="F57" s="40">
+      <c r="F57" s="39">
         <v>295.33999999999997</v>
       </c>
-      <c r="G57" s="40">
+      <c r="G57" s="39">
         <f>SimRecords!$B$6</f>
         <v>296.47000000000003</v>
       </c>
-      <c r="I57" s="40">
+      <c r="I57" s="39">
         <v>299.95</v>
       </c>
-      <c r="J57" s="40">
+      <c r="J57" s="39">
         <v>304.49</v>
       </c>
-      <c r="K57" s="40">
+      <c r="K57" s="39">
         <v>309.03847999999999</v>
       </c>
-      <c r="L57" s="40">
+      <c r="L57" s="39">
         <v>313.75484999999998</v>
       </c>
-      <c r="M57" s="40">
+      <c r="M57" s="39">
         <v>295.32715000000002</v>
       </c>
-      <c r="N57" s="40">
+      <c r="N57" s="39">
         <v>295.35687000000001</v>
       </c>
-      <c r="P57" s="40">
+      <c r="P57" s="39">
         <v>295.41543999999999</v>
       </c>
-      <c r="Q57" s="40">
+      <c r="Q57" s="39">
         <v>295.55029000000002</v>
       </c>
-      <c r="R57" s="40">
+      <c r="R57" s="39">
         <v>296.52123999999998</v>
       </c>
-      <c r="S57" s="40">
+      <c r="S57" s="39">
         <v>295.77208999999999</v>
       </c>
-      <c r="U57" s="40">
+      <c r="U57" s="39">
         <v>294.94614000000001</v>
       </c>
-      <c r="V57" s="40">
+      <c r="V57" s="39">
         <v>294.66298999999998</v>
       </c>
-      <c r="X57" s="40">
+      <c r="X57" s="39">
         <v>295.14654999999999</v>
       </c>
-      <c r="Y57" s="40">
+      <c r="Y57" s="39">
         <v>295.12842000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:25" s="40" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="40" t="s">
+    <row r="58" spans="1:25" s="39" customFormat="1">
+      <c r="A58" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="B58" s="40" t="s">
+      <c r="B58" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="C58" s="40">
+      <c r="C58" s="39">
         <v>2.1501100000000002</v>
       </c>
-      <c r="D58" s="40">
+      <c r="D58" s="39">
         <v>3.1509200000000002</v>
       </c>
-      <c r="E58" s="40">
+      <c r="E58" s="39">
         <v>3.8756499999999998</v>
       </c>
-      <c r="F58" s="40">
+      <c r="F58" s="39">
         <v>5.7749699999999997</v>
       </c>
-      <c r="G58" s="40">
+      <c r="G58" s="39">
         <f>SimRecords!$B$7</f>
         <v>7.6959</v>
       </c>
-      <c r="I58" s="40">
+      <c r="I58" s="39">
         <v>5.0377000000000001</v>
       </c>
-      <c r="J58" s="40">
+      <c r="J58" s="39">
         <v>4.1998899999999999</v>
       </c>
-      <c r="K58" s="40">
+      <c r="K58" s="39">
         <v>2.9781647000000002</v>
       </c>
-      <c r="L58" s="40">
+      <c r="L58" s="39">
         <v>2.1364105000000002</v>
       </c>
-      <c r="M58" s="40">
+      <c r="M58" s="39">
         <v>5.7612939000000001</v>
       </c>
-      <c r="N58" s="40">
+      <c r="N58" s="39">
         <v>5.7513417999999996</v>
       </c>
-      <c r="P58" s="40">
+      <c r="P58" s="39">
         <v>6.4879875</v>
       </c>
-      <c r="Q58" s="40">
+      <c r="Q58" s="39">
         <v>6.7495941999999998</v>
       </c>
-      <c r="R58" s="40">
+      <c r="R58" s="39">
         <v>5.7365398000000001</v>
       </c>
-      <c r="S58" s="40">
+      <c r="S58" s="39">
         <v>6.0016074000000001</v>
       </c>
-      <c r="U58" s="40">
+      <c r="U58" s="39">
         <v>6.2727956999999996</v>
       </c>
-      <c r="V58" s="40">
+      <c r="V58" s="39">
         <v>6.3664417000000002</v>
       </c>
-      <c r="X58" s="40">
+      <c r="X58" s="39">
         <v>6.2245407000000004</v>
       </c>
-      <c r="Y58" s="40">
+      <c r="Y58" s="39">
         <v>6.2292604000000003</v>
       </c>
     </row>
-    <row r="59" spans="1:25" s="40" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="40" t="s">
+    <row r="59" spans="1:25" s="39" customFormat="1">
+      <c r="A59" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="B59" s="40" t="s">
+      <c r="B59" s="39" t="s">
         <v>89</v>
       </c>
       <c r="C59" s="24">
@@ -5731,7 +5692,7 @@
       </c>
       <c r="T59" s="24"/>
       <c r="U59" s="24">
-        <f t="shared" ref="T59:U59" si="22">U58*0.0005</f>
+        <f t="shared" ref="U59" si="22">U58*0.0005</f>
         <v>3.13639785E-3</v>
       </c>
       <c r="V59" s="24">
@@ -5748,8 +5709,8 @@
         <v>3.1146302000000002E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A60" s="40" t="s">
+    <row r="60" spans="1:25">
+      <c r="A60" s="39" t="s">
         <v>121</v>
       </c>
       <c r="C60" s="24">
@@ -5832,8 +5793,8 @@
         <v>2.1973569429460568E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A61" s="40" t="s">
+    <row r="61" spans="1:25">
+      <c r="A61" s="39" t="s">
         <v>122</v>
       </c>
       <c r="C61" s="24">
@@ -5916,92 +5877,93 @@
         <v>-2.2805614935609564E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A62" s="40" t="s">
+    <row r="62" spans="1:25">
+      <c r="A62" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="C62" s="25">
+      <c r="C62" s="55">
         <f>(C48-C59)/C48</f>
         <v>3.7738513683150884E-3</v>
       </c>
-      <c r="D62" s="25">
+      <c r="D62" s="55">
         <f>(D48-D59)/D48</f>
         <v>-6.5537445671729399E-4</v>
       </c>
-      <c r="E62" s="25">
+      <c r="E62" s="55">
         <f t="shared" ref="E62:G62" si="43">(E48-E59)/E48</f>
         <v>4.4822209880538222E-3</v>
       </c>
-      <c r="F62" s="25">
+      <c r="F62" s="55">
         <f t="shared" si="43"/>
         <v>3.1125204922697346E-2</v>
       </c>
-      <c r="G62" s="25">
+      <c r="G62" s="55">
         <f t="shared" si="43"/>
         <v>1.7975106958396075E-2</v>
       </c>
-      <c r="I62" s="25">
+      <c r="H62" s="19"/>
+      <c r="I62" s="55">
         <f t="shared" ref="I62:J62" si="44">(I48-I59)/I48</f>
         <v>1.9926560748551023E-2</v>
       </c>
-      <c r="J62" s="25">
+      <c r="J62" s="55">
         <f t="shared" si="44"/>
         <v>1.1104035383887956E-2</v>
       </c>
-      <c r="K62" s="25">
+      <c r="K62" s="55">
         <f t="shared" ref="K62" si="45">(K48-K59)/K48</f>
         <v>4.6036193576214461E-2</v>
       </c>
-      <c r="L62" s="25">
+      <c r="L62" s="55">
         <f>(L48-L59)/L48</f>
         <v>-7.5152397389511016E-2</v>
       </c>
-      <c r="M62" s="25">
+      <c r="M62" s="55">
         <f>(M48-M59)/M48</f>
         <v>1.9483954980676128E-2</v>
       </c>
-      <c r="N62" s="25">
+      <c r="N62" s="55">
         <f>(N48-N59)/N48</f>
         <v>-6.6144025117217996E-3</v>
       </c>
-      <c r="O62" s="25"/>
-      <c r="P62" s="25">
+      <c r="O62" s="55"/>
+      <c r="P62" s="55">
         <f t="shared" ref="P62" si="46">(P48-P59)/P48</f>
         <v>-6.545873709903488E-2</v>
       </c>
-      <c r="Q62" s="25">
+      <c r="Q62" s="55">
         <f t="shared" ref="Q62:R62" si="47">(Q48-Q59)/Q48</f>
         <v>-8.7950146368556942E-2</v>
       </c>
-      <c r="R62" s="25">
+      <c r="R62" s="55">
         <f t="shared" si="47"/>
         <v>-4.446589311929227E-2</v>
       </c>
-      <c r="S62" s="25">
+      <c r="S62" s="55">
         <f t="shared" ref="S62:U62" si="48">(S48-S59)/S48</f>
         <v>-6.2544171114402705E-2</v>
       </c>
-      <c r="T62" s="25"/>
-      <c r="U62" s="25">
+      <c r="T62" s="55"/>
+      <c r="U62" s="55">
         <f t="shared" si="48"/>
         <v>2.3195861701215525E-2</v>
       </c>
-      <c r="V62" s="25">
+      <c r="V62" s="55">
         <f t="shared" ref="V62:X62" si="49">(V48-V59)/V48</f>
         <v>3.6440365590389663E-2</v>
       </c>
-      <c r="W62" s="25"/>
-      <c r="X62" s="25">
+      <c r="W62" s="55"/>
+      <c r="X62" s="55">
         <f t="shared" si="49"/>
         <v>-2.1982057110278923</v>
       </c>
-      <c r="Y62" s="25">
+      <c r="Y62" s="55">
         <f t="shared" ref="Y62" si="50">(Y48-Y59)/Y48</f>
         <v>-1.3295131894671905</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A63" s="40" t="s">
+    <row r="63" spans="1:25">
+      <c r="A63" s="39" t="s">
         <v>120</v>
       </c>
       <c r="C63" s="24">
@@ -6084,8 +6046,8 @@
         <v>1.3295151635884876</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="L64" s="55"/>
+    <row r="64" spans="1:25">
+      <c r="L64" s="54"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -6095,19 +6057,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AL33"/>
   <sheetViews>
     <sheetView topLeftCell="O1" workbookViewId="0">
       <selection activeCell="AA8" sqref="AA8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="13" max="13" width="29.875" customWidth="1"/>
+    <col min="13" max="13" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:36" ht="16.5">
       <c r="A1" s="1" t="s">
         <v>129</v>
       </c>
@@ -6115,7 +6077,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:36">
       <c r="A2" t="str">
         <f>[1]热侧实验!U12</f>
         <v>膜类型</v>
@@ -6238,7 +6200,7 @@
         <v>PVDF</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:36">
       <c r="A3" t="str">
         <f>[1]热侧实验!U13</f>
         <v>ePTFE</v>
@@ -6356,7 +6318,7 @@
         <v>46.843521688179884</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:36">
       <c r="A4" t="str">
         <f>[1]热侧实验!U14</f>
         <v>ePTFE</v>
@@ -6474,7 +6436,7 @@
         <v>44.928683240302114</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:36">
       <c r="A5" t="str">
         <f>[1]热侧实验!U15</f>
         <v>ePTFE</v>
@@ -6592,7 +6554,7 @@
         <v>19.94308391529044</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:36">
       <c r="A6" t="str">
         <f>[1]热侧实验!U16</f>
         <v>ePTFE</v>
@@ -6710,7 +6672,7 @@
         <v>21.306892948428231</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:36">
       <c r="A7" t="str">
         <f>[1]热侧实验!U17</f>
         <v>ePTFE</v>
@@ -6828,7 +6790,7 @@
         <v>25.225507365699077</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:36">
       <c r="M8" t="str">
         <v>料液侧流速（m/s)</v>
       </c>
@@ -6902,7 +6864,7 @@
         <v>1.0575562188444444E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:36" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:36" ht="16.5">
       <c r="A9" s="1" t="s">
         <v>128</v>
       </c>
@@ -6979,7 +6941,7 @@
         <v>1.0878928809055555E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:36">
       <c r="A10" t="str">
         <f>[1]冷侧实验!U13</f>
         <v>ePTFE</v>
@@ -7089,7 +7051,7 @@
         <v>4.8133098240000001</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:36">
       <c r="A11" t="str">
         <f>[1]冷侧实验!U14</f>
         <v>ePTFE</v>
@@ -7145,7 +7107,7 @@
         <v>6.5176549910266864E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:36">
       <c r="A12" t="str">
         <f>[1]冷侧实验!U15</f>
         <v>ePTFE</v>
@@ -7201,7 +7163,7 @@
         <v>0.34642769182840333</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:36">
       <c r="A13" t="str">
         <f>[1]冷侧实验!U16</f>
         <v>ePTFE</v>
@@ -7239,7 +7201,7 @@
         <v>5.6193918719999987</v>
       </c>
     </row>
-    <row r="14" spans="1:36" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:36" ht="16.5">
       <c r="A14" t="str">
         <f>[1]冷侧实验!U17</f>
         <v>ePTFE</v>
@@ -7295,28 +7257,28 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:36">
       <c r="M15" t="str">
         <f t="shared" ref="M15" si="0">M8</f>
         <v>料液侧流速（m/s)</v>
       </c>
-      <c r="N15" s="46">
+      <c r="N15" s="45">
         <f t="shared" ref="N15:R15" si="1">N8</f>
         <v>1.0570055555555555E-2</v>
       </c>
-      <c r="O15" s="47">
+      <c r="O15" s="46">
         <f t="shared" si="1"/>
         <v>1.0570055555555555E-2</v>
       </c>
-      <c r="P15" s="47">
+      <c r="P15" s="46">
         <f t="shared" si="1"/>
         <v>1.0570055555555555E-2</v>
       </c>
-      <c r="Q15" s="47">
+      <c r="Q15" s="46">
         <f t="shared" si="1"/>
         <v>1.0570055555555555E-2</v>
       </c>
-      <c r="R15" s="48">
+      <c r="R15" s="47">
         <f t="shared" si="1"/>
         <v>1.0570055555555555E-2</v>
       </c>
@@ -7393,7 +7355,7 @@
         <v>1.0575562188444444E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:36" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:36" ht="16.5">
       <c r="A16" s="1" t="s">
         <v>130</v>
       </c>
@@ -7401,23 +7363,23 @@
         <f t="shared" ref="M16" si="6">M3</f>
         <v>料液侧入口温度（℃）</v>
       </c>
-      <c r="N16" s="49">
+      <c r="N16" s="48">
         <f t="shared" ref="N16:R16" si="7">N3</f>
         <v>32.804908589380183</v>
       </c>
-      <c r="O16" s="44">
+      <c r="O16" s="43">
         <f t="shared" si="7"/>
         <v>37.545921167879214</v>
       </c>
-      <c r="P16" s="44">
+      <c r="P16" s="43">
         <f t="shared" si="7"/>
         <v>40.462794041113561</v>
       </c>
-      <c r="Q16" s="44">
+      <c r="Q16" s="43">
         <f t="shared" si="7"/>
         <v>46.813272232415727</v>
       </c>
-      <c r="R16" s="50">
+      <c r="R16" s="49">
         <f t="shared" si="7"/>
         <v>52.28803056208195</v>
       </c>
@@ -7494,7 +7456,7 @@
         <v>46.843521688179884</v>
       </c>
     </row>
-    <row r="17" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:38">
       <c r="A17" t="str">
         <f>[1]热转速实验!S13</f>
         <v>ePTFE</v>
@@ -7531,13 +7493,13 @@
         <f>[1]热转速实验!AA13</f>
         <v>10.576399104</v>
       </c>
-      <c r="N17" s="49"/>
-      <c r="O17" s="44"/>
-      <c r="P17" s="44"/>
-      <c r="Q17" s="44"/>
-      <c r="R17" s="50"/>
-    </row>
-    <row r="18" spans="1:38" x14ac:dyDescent="0.15">
+      <c r="N17" s="48"/>
+      <c r="O17" s="43"/>
+      <c r="P17" s="43"/>
+      <c r="Q17" s="43"/>
+      <c r="R17" s="49"/>
+    </row>
+    <row r="18" spans="1:38">
       <c r="A18" t="str">
         <f>[1]热转速实验!S14</f>
         <v>ePTFE</v>
@@ -7578,23 +7540,23 @@
         <f t="shared" ref="M18" si="12">M9</f>
         <v>渗透侧流速（m/s)</v>
       </c>
-      <c r="N18" s="49">
+      <c r="N18" s="48">
         <f t="shared" ref="N18:R18" si="13">N9</f>
         <v>1.0024555555555557E-2</v>
       </c>
-      <c r="O18" s="44">
+      <c r="O18" s="43">
         <f t="shared" si="13"/>
         <v>1.0024555555555557E-2</v>
       </c>
-      <c r="P18" s="44">
+      <c r="P18" s="43">
         <f t="shared" si="13"/>
         <v>1.0024555555555557E-2</v>
       </c>
-      <c r="Q18" s="44">
+      <c r="Q18" s="43">
         <f t="shared" si="13"/>
         <v>1.0024555555555557E-2</v>
       </c>
-      <c r="R18" s="50">
+      <c r="R18" s="49">
         <f t="shared" si="13"/>
         <v>1.0024555555555557E-2</v>
       </c>
@@ -7671,7 +7633,7 @@
         <v>1.0878928809055555E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:38">
       <c r="A19" t="str">
         <f>[1]热转速实验!S15</f>
         <v>ePTFE</v>
@@ -7712,23 +7674,23 @@
         <f t="shared" ref="M19" si="18">M5</f>
         <v>渗透侧入口温度（℃）</v>
       </c>
-      <c r="N19" s="49">
+      <c r="N19" s="48">
         <f t="shared" ref="N19:R19" si="19">N5</f>
         <v>20.020584823493895</v>
       </c>
-      <c r="O19" s="44">
+      <c r="O19" s="43">
         <f t="shared" si="19"/>
         <v>20.013996907080195</v>
       </c>
-      <c r="P19" s="44">
+      <c r="P19" s="43">
         <f t="shared" si="19"/>
         <v>20.040555205268429</v>
       </c>
-      <c r="Q19" s="44">
+      <c r="Q19" s="43">
         <f t="shared" si="19"/>
         <v>19.965192717598594</v>
       </c>
-      <c r="R19" s="50">
+      <c r="R19" s="49">
         <f t="shared" si="19"/>
         <v>20.531591054442632</v>
       </c>
@@ -7805,7 +7767,7 @@
         <v>19.94308391529044</v>
       </c>
     </row>
-    <row r="20" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:38">
       <c r="A20" t="str">
         <f>[1]热转速实验!S16</f>
         <v>ePTFE</v>
@@ -7842,13 +7804,13 @@
         <f>[1]热转速实验!AA16</f>
         <v>10.960891391999999</v>
       </c>
-      <c r="N20" s="49"/>
-      <c r="O20" s="44"/>
-      <c r="P20" s="44"/>
-      <c r="Q20" s="44"/>
-      <c r="R20" s="50"/>
-    </row>
-    <row r="21" spans="1:38" x14ac:dyDescent="0.15">
+      <c r="N20" s="48"/>
+      <c r="O20" s="43"/>
+      <c r="P20" s="43"/>
+      <c r="Q20" s="43"/>
+      <c r="R20" s="49"/>
+    </row>
+    <row r="21" spans="1:38">
       <c r="A21" t="str">
         <f>[1]热转速实验!S17</f>
         <v>ePTFE</v>
@@ -7889,23 +7851,23 @@
         <f t="shared" ref="M21" si="24">M4</f>
         <v>料液侧出口温度（℃）</v>
       </c>
-      <c r="N21" s="49">
+      <c r="N21" s="48">
         <f t="shared" ref="N21:R21" si="25">N4</f>
         <v>32.209159619805561</v>
       </c>
-      <c r="O21" s="44">
+      <c r="O21" s="43">
         <f t="shared" si="25"/>
         <v>36.641882535934052</v>
       </c>
-      <c r="P21" s="44">
+      <c r="P21" s="43">
         <f t="shared" si="25"/>
         <v>39.206231593240013</v>
       </c>
-      <c r="Q21" s="44">
+      <c r="Q21" s="43">
         <f t="shared" si="25"/>
         <v>45.115007004655496</v>
       </c>
-      <c r="R21" s="50">
+      <c r="R21" s="49">
         <f t="shared" si="25"/>
         <v>50.488628590359532</v>
       </c>
@@ -7982,28 +7944,28 @@
         <v>44.928683240302114</v>
       </c>
     </row>
-    <row r="22" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:38">
       <c r="M22" t="str">
         <f t="shared" ref="M22" si="30">M6</f>
         <v>渗透侧出口温度（℃）</v>
       </c>
-      <c r="N22" s="49">
+      <c r="N22" s="48">
         <f t="shared" ref="N22:R22" si="31">N6</f>
         <v>21.1468268936618</v>
       </c>
-      <c r="O22" s="44">
+      <c r="O22" s="43">
         <f t="shared" si="31"/>
         <v>21.066646083396979</v>
       </c>
-      <c r="P22" s="44">
+      <c r="P22" s="43">
         <f t="shared" si="31"/>
         <v>21.202254882336835</v>
       </c>
-      <c r="Q22" s="44">
+      <c r="Q22" s="43">
         <f t="shared" si="31"/>
         <v>21.428861307302665</v>
       </c>
-      <c r="R22" s="50">
+      <c r="R22" s="49">
         <f t="shared" si="31"/>
         <v>21.993250061846652</v>
       </c>
@@ -8080,7 +8042,7 @@
         <v>21.306892948428231</v>
       </c>
     </row>
-    <row r="23" spans="1:38" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:38" ht="16.5">
       <c r="A23" s="1" t="s">
         <v>127</v>
       </c>
@@ -8088,23 +8050,23 @@
         <f t="shared" ref="M23:R23" si="36">M10</f>
         <v>平均膜渗透通量（kg·m-2·h-1）</v>
       </c>
-      <c r="N23" s="51">
+      <c r="N23" s="50">
         <f t="shared" si="36"/>
         <v>3.8848588799999995</v>
       </c>
-      <c r="O23" s="45">
+      <c r="O23" s="44">
         <f t="shared" si="36"/>
         <v>5.667941375999999</v>
       </c>
-      <c r="P23" s="45">
+      <c r="P23" s="44">
         <f t="shared" si="36"/>
         <v>7.0075795200000002</v>
       </c>
-      <c r="Q23" s="45">
+      <c r="Q23" s="44">
         <f t="shared" si="36"/>
         <v>10.728884735999999</v>
       </c>
-      <c r="R23" s="52">
+      <c r="R23" s="51">
         <f t="shared" si="36"/>
         <v>14.106180095999997</v>
       </c>
@@ -8181,7 +8143,7 @@
         <v>4.8133098240000001</v>
       </c>
     </row>
-    <row r="24" spans="1:38" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:38" s="42" customFormat="1">
       <c r="A24" t="str">
         <f>[1]冷转速实验!T13</f>
         <v>ePTFE</v>
@@ -8218,103 +8180,103 @@
         <f>[1]冷转速实验!AB13</f>
         <v>9.8861740800000018</v>
       </c>
-      <c r="M24" s="43" t="s">
+      <c r="M24" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="N24" s="44" t="str">
+      <c r="N24" s="43" t="str">
         <f>IF(N26=1, "duplicate","")</f>
         <v/>
       </c>
-      <c r="O24" s="44" t="str">
+      <c r="O24" s="43" t="str">
         <f t="shared" ref="O24:AJ24" si="38">IF(O26=1, "duplicate","")</f>
         <v/>
       </c>
-      <c r="P24" s="44" t="str">
+      <c r="P24" s="43" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="Q24" s="44" t="str">
+      <c r="Q24" s="43" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="R24" s="44" t="str">
+      <c r="R24" s="43" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="S24" s="44" t="str">
+      <c r="S24" s="43" t="str">
         <f t="shared" si="38"/>
         <v>duplicate</v>
       </c>
-      <c r="T24" s="44" t="str">
+      <c r="T24" s="43" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="U24" s="44" t="str">
+      <c r="U24" s="43" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="V24" s="44" t="str">
+      <c r="V24" s="43" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="W24" s="44" t="str">
+      <c r="W24" s="43" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="X24" s="44" t="str">
+      <c r="X24" s="43" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="Y24" s="44" t="str">
+      <c r="Y24" s="43" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="Z24" s="44" t="str">
+      <c r="Z24" s="43" t="str">
         <f t="shared" si="38"/>
         <v>duplicate</v>
       </c>
-      <c r="AA24" s="44" t="str">
+      <c r="AA24" s="43" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="AB24" s="44" t="str">
+      <c r="AB24" s="43" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="AC24" s="44" t="str">
+      <c r="AC24" s="43" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="AD24" s="44" t="str">
+      <c r="AD24" s="43" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="AE24" s="44" t="str">
+      <c r="AE24" s="43" t="str">
         <f t="shared" si="38"/>
         <v>duplicate</v>
       </c>
-      <c r="AF24" s="44" t="str">
+      <c r="AF24" s="43" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="AG24" s="44" t="str">
+      <c r="AG24" s="43" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="AH24" s="44" t="str">
+      <c r="AH24" s="43" t="str">
         <f t="shared" si="38"/>
         <v>duplicate</v>
       </c>
-      <c r="AI24" s="44" t="str">
+      <c r="AI24" s="43" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="AJ24" s="44" t="str">
+      <c r="AJ24" s="43" t="str">
         <f t="shared" si="38"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:38">
       <c r="A25" t="str">
         <f>[1]冷转速实验!T14</f>
         <v>ePTFE</v>
@@ -8351,80 +8313,80 @@
         <f>[1]冷转速实验!AB14</f>
         <v>10.167006336</v>
       </c>
-      <c r="M25" s="43" t="s">
+      <c r="M25" s="42" t="s">
         <v>141</v>
       </c>
-      <c r="N25" s="43">
+      <c r="N25" s="42">
         <v>1</v>
       </c>
-      <c r="O25" s="43">
+      <c r="O25" s="42">
         <v>2</v>
       </c>
-      <c r="P25" s="43">
+      <c r="P25" s="42">
         <v>3</v>
       </c>
-      <c r="Q25" s="43">
+      <c r="Q25" s="42">
         <v>4</v>
       </c>
-      <c r="R25" s="43">
+      <c r="R25" s="42">
         <v>5</v>
       </c>
-      <c r="S25" s="43">
+      <c r="S25" s="42">
         <v>6</v>
       </c>
-      <c r="T25" s="43">
+      <c r="T25" s="42">
         <v>7</v>
       </c>
-      <c r="U25" s="43">
+      <c r="U25" s="42">
         <v>8</v>
       </c>
-      <c r="V25" s="43">
+      <c r="V25" s="42">
         <v>9</v>
       </c>
-      <c r="W25" s="43">
+      <c r="W25" s="42">
         <v>10</v>
       </c>
-      <c r="X25" s="43">
+      <c r="X25" s="42">
         <v>11</v>
       </c>
-      <c r="Y25" s="43">
+      <c r="Y25" s="42">
         <v>12</v>
       </c>
-      <c r="Z25" s="43">
+      <c r="Z25" s="42">
         <v>13</v>
       </c>
-      <c r="AA25" s="43">
+      <c r="AA25" s="42">
         <v>14</v>
       </c>
-      <c r="AB25" s="43">
+      <c r="AB25" s="42">
         <v>15</v>
       </c>
-      <c r="AC25" s="43">
+      <c r="AC25" s="42">
         <v>16</v>
       </c>
-      <c r="AD25" s="43">
+      <c r="AD25" s="42">
         <v>17</v>
       </c>
-      <c r="AE25" s="43">
+      <c r="AE25" s="42">
         <v>18</v>
       </c>
-      <c r="AF25" s="43">
+      <c r="AF25" s="42">
         <v>19</v>
       </c>
-      <c r="AG25" s="43">
+      <c r="AG25" s="42">
         <v>20</v>
       </c>
-      <c r="AH25" s="43">
+      <c r="AH25" s="42">
         <v>21</v>
       </c>
-      <c r="AI25" s="43">
+      <c r="AI25" s="42">
         <v>22</v>
       </c>
-      <c r="AJ25" s="43">
+      <c r="AJ25" s="42">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:38" s="43" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:38" s="42" customFormat="1">
       <c r="A26" t="str">
         <f>[1]冷转速实验!T15</f>
         <v>ePTFE</v>
@@ -8461,100 +8423,100 @@
         <f>[1]冷转速实验!AB15</f>
         <v>10.728884735999999</v>
       </c>
-      <c r="N26" s="43">
+      <c r="N26" s="42">
         <f>HLOOKUP(N25,$N28:$AJ31,4,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="O26" s="43">
+      <c r="O26" s="42">
         <f t="shared" ref="O26:AJ26" si="39">HLOOKUP(O25,$N28:$AJ31,4,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="P26" s="43">
+      <c r="P26" s="42">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="Q26" s="43">
+      <c r="Q26" s="42">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="R26" s="43">
+      <c r="R26" s="42">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="S26" s="43">
+      <c r="S26" s="42">
         <f t="shared" si="39"/>
         <v>1</v>
       </c>
-      <c r="T26" s="43">
+      <c r="T26" s="42">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="U26" s="43">
+      <c r="U26" s="42">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="V26" s="43">
+      <c r="V26" s="42">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="W26" s="43">
+      <c r="W26" s="42">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="X26" s="43">
+      <c r="X26" s="42">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="Y26" s="43">
+      <c r="Y26" s="42">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="Z26" s="43">
+      <c r="Z26" s="42">
         <f t="shared" si="39"/>
         <v>1</v>
       </c>
-      <c r="AA26" s="43">
+      <c r="AA26" s="42">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="AB26" s="43">
+      <c r="AB26" s="42">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="AC26" s="43">
+      <c r="AC26" s="42">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="AD26" s="43">
+      <c r="AD26" s="42">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="AE26" s="43">
+      <c r="AE26" s="42">
         <f t="shared" si="39"/>
         <v>1</v>
       </c>
-      <c r="AF26" s="43">
+      <c r="AF26" s="42">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="AG26" s="43">
+      <c r="AG26" s="42">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="AH26" s="43">
+      <c r="AH26" s="42">
         <f t="shared" si="39"/>
         <v>1</v>
       </c>
-      <c r="AI26" s="43">
+      <c r="AI26" s="42">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
-      <c r="AJ26" s="43">
+      <c r="AJ26" s="42">
         <f t="shared" si="39"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:38" ht="16.5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:38" ht="16.5">
       <c r="A27" t="str">
         <f>[1]冷转速实验!T16</f>
         <v>ePTFE</v>
@@ -8594,17 +8556,17 @@
       <c r="M27" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="O27" s="43"/>
-      <c r="P27" s="43"/>
-      <c r="Q27" s="43"/>
-      <c r="R27" s="43"/>
-      <c r="S27" s="43"/>
-      <c r="T27" s="43"/>
-      <c r="U27" s="43"/>
-      <c r="V27" s="43"/>
-      <c r="W27" s="43"/>
-    </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.15">
+      <c r="O27" s="42"/>
+      <c r="P27" s="42"/>
+      <c r="Q27" s="42"/>
+      <c r="R27" s="42"/>
+      <c r="S27" s="42"/>
+      <c r="T27" s="42"/>
+      <c r="U27" s="42"/>
+      <c r="V27" s="42"/>
+      <c r="W27" s="42"/>
+    </row>
+    <row r="28" spans="1:38">
       <c r="A28" t="str">
         <f>[1]冷转速实验!T17</f>
         <v>ePTFE</v>
@@ -8641,7 +8603,7 @@
         <f>[1]冷转速实验!AB17</f>
         <v>11.892979584000001</v>
       </c>
-      <c r="M28" s="43" t="s">
+      <c r="M28" s="42" t="s">
         <v>138</v>
       </c>
       <c r="N28">
@@ -8653,69 +8615,69 @@
       <c r="P28">
         <v>1</v>
       </c>
-      <c r="Q28" s="43">
+      <c r="Q28" s="42">
         <v>23</v>
       </c>
-      <c r="R28" s="43">
+      <c r="R28" s="42">
         <v>9</v>
       </c>
-      <c r="S28" s="43">
+      <c r="S28" s="42">
         <v>2</v>
       </c>
-      <c r="T28" s="43">
+      <c r="T28" s="42">
         <v>3</v>
       </c>
-      <c r="U28" s="43">
+      <c r="U28" s="42">
         <v>8</v>
       </c>
-      <c r="V28" s="43">
+      <c r="V28" s="42">
         <v>7</v>
       </c>
-      <c r="W28" s="43">
+      <c r="W28" s="42">
         <v>16</v>
       </c>
-      <c r="X28" s="43">
+      <c r="X28" s="42">
         <v>17</v>
       </c>
-      <c r="Y28" s="43">
+      <c r="Y28" s="42">
         <v>12</v>
       </c>
-      <c r="Z28" s="43">
+      <c r="Z28" s="42">
         <v>11</v>
       </c>
-      <c r="AA28" s="43">
+      <c r="AA28" s="42">
         <v>4</v>
       </c>
-      <c r="AB28" s="43">
+      <c r="AB28" s="42">
         <v>6</v>
       </c>
-      <c r="AC28" s="43">
+      <c r="AC28" s="42">
         <v>13</v>
       </c>
-      <c r="AD28" s="43">
+      <c r="AD28" s="42">
         <v>18</v>
       </c>
-      <c r="AE28" s="43">
+      <c r="AE28" s="42">
         <v>21</v>
       </c>
-      <c r="AF28" s="43">
+      <c r="AF28" s="42">
         <v>14</v>
       </c>
-      <c r="AG28" s="43">
+      <c r="AG28" s="42">
         <v>15</v>
       </c>
-      <c r="AH28" s="43">
+      <c r="AH28" s="42">
         <v>19</v>
       </c>
-      <c r="AI28" s="43">
+      <c r="AI28" s="42">
         <v>20</v>
       </c>
-      <c r="AJ28" s="43">
+      <c r="AJ28" s="42">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.15">
-      <c r="M29" s="43" t="s">
+    <row r="29" spans="1:38">
+      <c r="M29" s="42" t="s">
         <v>139</v>
       </c>
       <c r="N29">
@@ -8733,141 +8695,141 @@
       <c r="R29">
         <v>5.6193918719999987</v>
       </c>
-      <c r="S29" s="43">
+      <c r="S29" s="42">
         <v>5.667941375999999</v>
       </c>
-      <c r="T29" s="43">
+      <c r="T29" s="42">
         <v>7.0075795200000002</v>
       </c>
-      <c r="U29" s="43">
+      <c r="U29" s="42">
         <v>7.6446888960000008</v>
       </c>
-      <c r="V29" s="43">
+      <c r="V29" s="42">
         <v>9.2522250239999995</v>
       </c>
-      <c r="W29" s="43">
+      <c r="W29" s="42">
         <v>9.8861740800000018</v>
       </c>
-      <c r="X29" s="43">
+      <c r="X29" s="42">
         <v>10.167006336</v>
       </c>
-      <c r="Y29" s="43">
+      <c r="Y29" s="42">
         <v>10.284390143999998</v>
       </c>
-      <c r="Z29" s="43">
+      <c r="Z29" s="42">
         <v>10.576399104</v>
       </c>
-      <c r="AA29" s="43">
+      <c r="AA29" s="42">
         <v>10.728884735999999</v>
       </c>
-      <c r="AB29" s="43">
+      <c r="AB29" s="42">
         <v>10.728884735999999</v>
       </c>
-      <c r="AC29" s="43">
+      <c r="AC29" s="42">
         <v>10.728884735999999</v>
       </c>
-      <c r="AD29" s="43">
+      <c r="AD29" s="42">
         <v>10.728884735999999</v>
       </c>
-      <c r="AE29" s="43">
+      <c r="AE29" s="42">
         <v>10.728884735999999</v>
       </c>
-      <c r="AF29" s="43">
+      <c r="AF29" s="42">
         <v>10.960891391999999</v>
       </c>
-      <c r="AG29" s="43">
+      <c r="AG29" s="42">
         <v>11.167119743999999</v>
       </c>
-      <c r="AH29" s="43">
+      <c r="AH29" s="42">
         <v>11.559156864</v>
       </c>
-      <c r="AI29" s="43">
+      <c r="AI29" s="42">
         <v>11.892979584000001</v>
       </c>
-      <c r="AJ29" s="43">
+      <c r="AJ29" s="42">
         <v>14.106180095999997</v>
       </c>
-      <c r="AK29" s="43"/>
-      <c r="AL29" s="43"/>
-    </row>
-    <row r="30" spans="1:38" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="AK29" s="42"/>
+      <c r="AL29" s="42"/>
+    </row>
+    <row r="30" spans="1:38" ht="16.5">
       <c r="A30" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="M30" s="53" t="s">
+      <c r="M30" s="52" t="s">
         <v>140</v>
       </c>
-      <c r="N30" s="43">
+      <c r="N30" s="42">
         <v>1</v>
       </c>
-      <c r="O30" s="43">
+      <c r="O30" s="42">
         <v>2</v>
       </c>
-      <c r="P30" s="43">
+      <c r="P30" s="42">
         <v>3</v>
       </c>
-      <c r="Q30" s="43">
+      <c r="Q30" s="42">
         <v>4</v>
       </c>
-      <c r="R30" s="43">
+      <c r="R30" s="42">
         <v>5</v>
       </c>
-      <c r="S30" s="43">
+      <c r="S30" s="42">
         <v>6</v>
       </c>
-      <c r="T30" s="43">
+      <c r="T30" s="42">
         <v>7</v>
       </c>
-      <c r="U30" s="43">
+      <c r="U30" s="42">
         <v>8</v>
       </c>
-      <c r="V30" s="43">
+      <c r="V30" s="42">
         <v>9</v>
       </c>
-      <c r="W30" s="43">
+      <c r="W30" s="42">
         <v>10</v>
       </c>
-      <c r="X30" s="43">
+      <c r="X30" s="42">
         <v>11</v>
       </c>
-      <c r="Y30" s="43">
+      <c r="Y30" s="42">
         <v>12</v>
       </c>
-      <c r="Z30" s="43">
+      <c r="Z30" s="42">
         <v>13</v>
       </c>
-      <c r="AA30" s="43">
+      <c r="AA30" s="42">
         <v>14</v>
       </c>
-      <c r="AB30" s="43">
+      <c r="AB30" s="42">
         <v>15</v>
       </c>
-      <c r="AC30" s="43">
+      <c r="AC30" s="42">
         <v>16</v>
       </c>
-      <c r="AD30" s="43">
+      <c r="AD30" s="42">
         <v>17</v>
       </c>
-      <c r="AE30" s="43">
+      <c r="AE30" s="42">
         <v>18</v>
       </c>
-      <c r="AF30" s="43">
+      <c r="AF30" s="42">
         <v>19</v>
       </c>
-      <c r="AG30" s="43">
+      <c r="AG30" s="42">
         <v>20</v>
       </c>
-      <c r="AH30" s="43">
+      <c r="AH30" s="42">
         <v>21</v>
       </c>
-      <c r="AI30" s="43">
+      <c r="AI30" s="42">
         <v>22</v>
       </c>
-      <c r="AJ30" s="43">
+      <c r="AJ30" s="42">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:38">
       <c r="A31" t="str">
         <f>[1]膜种类实验!P15</f>
         <v>ePTFE</v>
@@ -8904,103 +8866,103 @@
         <f>[1]膜种类实验!X15</f>
         <v>10.728884735999999</v>
       </c>
-      <c r="M31" s="53" t="s">
+      <c r="M31" s="52" t="s">
         <v>142</v>
       </c>
       <c r="N31">
         <f>IF(MATCH(N29,$N29:$AN29,0)=N30, 0, 1)</f>
         <v>0</v>
       </c>
-      <c r="O31" s="43">
+      <c r="O31" s="42">
         <f t="shared" ref="O31:AJ31" si="40">IF(MATCH(O29,$N29:$AN29,0)=O30, 0, 1)</f>
         <v>0</v>
       </c>
-      <c r="P31" s="43">
+      <c r="P31" s="42">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="Q31" s="43">
+      <c r="Q31" s="42">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="R31" s="43">
+      <c r="R31" s="42">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="S31" s="43">
+      <c r="S31" s="42">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="T31" s="43">
+      <c r="T31" s="42">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="U31" s="43">
+      <c r="U31" s="42">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="V31" s="43">
+      <c r="V31" s="42">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="W31" s="43">
+      <c r="W31" s="42">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="X31" s="43">
+      <c r="X31" s="42">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="Y31" s="43">
+      <c r="Y31" s="42">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="Z31" s="43">
+      <c r="Z31" s="42">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="AA31" s="43">
+      <c r="AA31" s="42">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="AB31" s="43">
+      <c r="AB31" s="42">
         <f t="shared" si="40"/>
         <v>1</v>
       </c>
-      <c r="AC31" s="43">
+      <c r="AC31" s="42">
         <f t="shared" si="40"/>
         <v>1</v>
       </c>
-      <c r="AD31" s="43">
+      <c r="AD31" s="42">
         <f t="shared" si="40"/>
         <v>1</v>
       </c>
-      <c r="AE31" s="43">
+      <c r="AE31" s="42">
         <f t="shared" si="40"/>
         <v>1</v>
       </c>
-      <c r="AF31" s="43">
+      <c r="AF31" s="42">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="AG31" s="43">
+      <c r="AG31" s="42">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="AH31" s="43">
+      <c r="AH31" s="42">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="AI31" s="43">
+      <c r="AI31" s="42">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
-      <c r="AJ31" s="43">
+      <c r="AJ31" s="42">
         <f t="shared" si="40"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:38">
       <c r="A32" t="str">
         <f>[1]膜种类实验!P16</f>
         <v>PTFE</v>
@@ -9037,9 +8999,9 @@
         <f>[1]膜种类实验!X16</f>
         <v>3.5032684799999991</v>
       </c>
-      <c r="O32" s="43"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="O32" s="42"/>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" t="str">
         <f>[1]膜种类实验!P17</f>
         <v>PVDF</v>
@@ -9084,19 +9046,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>111</v>
       </c>
@@ -9104,12 +9066,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5">
       <c r="A3" s="21" t="s">
         <v>113</v>
       </c>
@@ -9126,12 +9088,12 @@
         <v>4.7999999999999998E-6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5">
       <c r="A5" s="21" t="s">
         <v>116</v>
       </c>
@@ -9148,7 +9110,7 @@
         <v>322.27999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5">
       <c r="A6" s="21" t="s">
         <v>115</v>
       </c>
@@ -9165,7 +9127,7 @@
         <v>297.38</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5">
       <c r="A7" s="21" t="s">
         <v>117</v>
       </c>
@@ -9182,7 +9144,7 @@
         <v>29.719899999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5">
       <c r="A8" s="21" t="s">
         <v>118</v>
       </c>
@@ -9203,7 +9165,7 @@
         <v>1.485995E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5">
       <c r="B10" s="22">
         <f>(0.003918-C8)*(C3-D3)/(C8-D8)+C3</f>
         <v>9.5687569099487663E-7</v>

</xml_diff>

<commit_message>
Collect the exp. data for varied feeding concentration
</commit_message>
<xml_diff>
--- a/bin/2d_s_cc/reorganized exp.data.xlsx
+++ b/bin/2d_s_cc/reorganized exp.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="75" windowWidth="17235" windowHeight="8955" activeTab="1"/>
+    <workbookView xWindow="2340" yWindow="75" windowWidth="17235" windowHeight="8955" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Wang&amp;Chung2008CES" sheetId="1" r:id="rId1"/>
@@ -227,7 +227,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="148">
   <si>
     <t>Wang K Y, Chung T S, Gryta M. Chem. Eng. Sci., 2008, 63: 2587-2594</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -719,6 +719,18 @@
   </si>
   <si>
     <t>Note of duplicate</t>
+  </si>
+  <si>
+    <t>进料浓度变化</t>
+  </si>
+  <si>
+    <t>浓度</t>
+  </si>
+  <si>
+    <t>进料浓度</t>
+  </si>
+  <si>
+    <t>duplicate</t>
   </si>
 </sst>
 </file>
@@ -1323,24 +1335,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="183732096"/>
-        <c:axId val="183733632"/>
+        <c:axId val="183920896"/>
+        <c:axId val="183934976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="183732096"/>
+        <c:axId val="183920896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183733632"/>
+        <c:crossAx val="183934976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="183733632"/>
+        <c:axId val="183934976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1348,20 +1359,21 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183732096"/>
+        <c:crossAx val="183920896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1420,9 +1432,9 @@
       <sheetName val="安托因方程"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
       <sheetData sheetId="3">
         <row r="12">
           <cell r="U12" t="str">
@@ -1782,7 +1794,168 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="5">
+        <row r="15">
+          <cell r="P15" t="str">
+            <v>ePTFE</v>
+          </cell>
+          <cell r="Q15">
+            <v>46.813272232415727</v>
+          </cell>
+          <cell r="R15">
+            <v>45.115007004655496</v>
+          </cell>
+          <cell r="S15">
+            <v>19.965192717598594</v>
+          </cell>
+          <cell r="T15">
+            <v>21.428861307302665</v>
+          </cell>
+          <cell r="U15">
+            <v>25.234077623592736</v>
+          </cell>
+          <cell r="V15">
+            <v>1.0575562188444444E-2</v>
+          </cell>
+          <cell r="W15">
+            <v>1.0878928809055555E-2</v>
+          </cell>
+          <cell r="X15">
+            <v>10.728884735999999</v>
+          </cell>
+          <cell r="Y15">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="P16" t="str">
+            <v>ePTFE</v>
+          </cell>
+          <cell r="Q16">
+            <v>46.848783530878762</v>
+          </cell>
+          <cell r="R16">
+            <v>45.433250155957296</v>
+          </cell>
+          <cell r="S16">
+            <v>19.989925140361731</v>
+          </cell>
+          <cell r="T16">
+            <v>21.583000623829477</v>
+          </cell>
+          <cell r="U16">
+            <v>25.324775484892648</v>
+          </cell>
+          <cell r="V16">
+            <v>1.0575562188444444E-2</v>
+          </cell>
+          <cell r="W16">
+            <v>1.0878928809055555E-2</v>
+          </cell>
+          <cell r="X16">
+            <v>6.7713711627906985</v>
+          </cell>
+          <cell r="Y16">
+            <v>6.5039999999999996</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="P17" t="str">
+            <v>ePTFE</v>
+          </cell>
+          <cell r="Q17">
+            <v>46.810284463894057</v>
+          </cell>
+          <cell r="R17">
+            <v>46.127227258519227</v>
+          </cell>
+          <cell r="S17">
+            <v>19.900375117224076</v>
+          </cell>
+          <cell r="T17">
+            <v>21.569084088778226</v>
+          </cell>
+          <cell r="U17">
+            <v>25.716106122382811</v>
+          </cell>
+          <cell r="V17">
+            <v>1.0575562188444444E-2</v>
+          </cell>
+          <cell r="W17">
+            <v>1.0878928809055555E-2</v>
+          </cell>
+          <cell r="X17">
+            <v>5.5270333439999995</v>
+          </cell>
+          <cell r="Y17">
+            <v>12.406000000000001</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="P18" t="str">
+            <v>ePTFE</v>
+          </cell>
+          <cell r="Q18">
+            <v>46.866582914572703</v>
+          </cell>
+          <cell r="R18">
+            <v>45.261652010050049</v>
+          </cell>
+          <cell r="S18">
+            <v>19.998618090452187</v>
+          </cell>
+          <cell r="T18">
+            <v>21.251664572864392</v>
+          </cell>
+          <cell r="U18">
+            <v>25.412196622905832</v>
+          </cell>
+          <cell r="V18">
+            <v>1.0575562188444444E-2</v>
+          </cell>
+          <cell r="W18">
+            <v>1.0878928809055555E-2</v>
+          </cell>
+          <cell r="X18">
+            <v>3.0934241280000001</v>
+          </cell>
+          <cell r="Y18">
+            <v>17.439</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="P19" t="str">
+            <v>ePTFE</v>
+          </cell>
+          <cell r="Q19">
+            <v>47.081704781703998</v>
+          </cell>
+          <cell r="R19">
+            <v>45.950311850311486</v>
+          </cell>
+          <cell r="S19">
+            <v>19.971794871794781</v>
+          </cell>
+          <cell r="T19">
+            <v>21.224081774082016</v>
+          </cell>
+          <cell r="U19">
+            <v>25.899790799170869</v>
+          </cell>
+          <cell r="V19">
+            <v>1.0575562188444444E-2</v>
+          </cell>
+          <cell r="W19">
+            <v>1.0878928809055555E-2</v>
+          </cell>
+          <cell r="X19">
+            <v>0.32185294698240002</v>
+          </cell>
+          <cell r="Y19">
+            <v>21.963999999999999</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="6">
         <row r="13">
           <cell r="S13" t="str">
@@ -2166,9 +2339,9 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2912,8 +3085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="O38" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="O20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="AC39" sqref="AC39"/>
@@ -6058,10 +6231,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AL33"/>
+  <dimension ref="A1:AP40"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AA8" sqref="AA8"/>
+    <sheetView tabSelected="1" topLeftCell="Y7" workbookViewId="0">
+      <selection activeCell="AK17" sqref="AK17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6069,7 +6242,7 @@
     <col min="13" max="13" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="16.5">
+    <row r="1" spans="1:42" ht="16.5">
       <c r="A1" s="1" t="s">
         <v>129</v>
       </c>
@@ -6077,7 +6250,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:42">
       <c r="A2" t="str">
         <f>[1]热侧实验!U12</f>
         <v>膜类型</v>
@@ -6199,8 +6372,24 @@
       <c r="AJ2" t="str">
         <v>PVDF</v>
       </c>
-    </row>
-    <row r="3" spans="1:36">
+      <c r="AL2" t="str">
+        <f t="array" ref="AL2:AP11">TRANSPOSE(A36:J40)</f>
+        <v>ePTFE</v>
+      </c>
+      <c r="AM2" t="str">
+        <v>ePTFE</v>
+      </c>
+      <c r="AN2" t="str">
+        <v>ePTFE</v>
+      </c>
+      <c r="AO2" t="str">
+        <v>ePTFE</v>
+      </c>
+      <c r="AP2" t="str">
+        <v>ePTFE</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42">
       <c r="A3" t="str">
         <f>[1]热侧实验!U13</f>
         <v>ePTFE</v>
@@ -6317,8 +6506,23 @@
       <c r="AJ3">
         <v>46.843521688179884</v>
       </c>
-    </row>
-    <row r="4" spans="1:36">
+      <c r="AL3">
+        <v>46.813272232415727</v>
+      </c>
+      <c r="AM3">
+        <v>46.848783530878762</v>
+      </c>
+      <c r="AN3">
+        <v>46.810284463894057</v>
+      </c>
+      <c r="AO3">
+        <v>46.866582914572703</v>
+      </c>
+      <c r="AP3">
+        <v>47.081704781703998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42">
       <c r="A4" t="str">
         <f>[1]热侧实验!U14</f>
         <v>ePTFE</v>
@@ -6435,8 +6639,23 @@
       <c r="AJ4">
         <v>44.928683240302114</v>
       </c>
-    </row>
-    <row r="5" spans="1:36">
+      <c r="AL4">
+        <v>45.115007004655496</v>
+      </c>
+      <c r="AM4">
+        <v>45.433250155957296</v>
+      </c>
+      <c r="AN4">
+        <v>46.127227258519227</v>
+      </c>
+      <c r="AO4">
+        <v>45.261652010050049</v>
+      </c>
+      <c r="AP4">
+        <v>45.950311850311486</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42">
       <c r="A5" t="str">
         <f>[1]热侧实验!U15</f>
         <v>ePTFE</v>
@@ -6553,8 +6772,23 @@
       <c r="AJ5">
         <v>19.94308391529044</v>
       </c>
-    </row>
-    <row r="6" spans="1:36">
+      <c r="AL5">
+        <v>19.965192717598594</v>
+      </c>
+      <c r="AM5">
+        <v>19.989925140361731</v>
+      </c>
+      <c r="AN5">
+        <v>19.900375117224076</v>
+      </c>
+      <c r="AO5">
+        <v>19.998618090452187</v>
+      </c>
+      <c r="AP5">
+        <v>19.971794871794781</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42">
       <c r="A6" t="str">
         <f>[1]热侧实验!U16</f>
         <v>ePTFE</v>
@@ -6671,8 +6905,23 @@
       <c r="AJ6">
         <v>21.306892948428231</v>
       </c>
-    </row>
-    <row r="7" spans="1:36">
+      <c r="AL6">
+        <v>21.428861307302665</v>
+      </c>
+      <c r="AM6">
+        <v>21.583000623829477</v>
+      </c>
+      <c r="AN6">
+        <v>21.569084088778226</v>
+      </c>
+      <c r="AO6">
+        <v>21.251664572864392</v>
+      </c>
+      <c r="AP6">
+        <v>21.224081774082016</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42">
       <c r="A7" t="str">
         <f>[1]热侧实验!U17</f>
         <v>ePTFE</v>
@@ -6789,8 +7038,23 @@
       <c r="AJ7">
         <v>25.225507365699077</v>
       </c>
-    </row>
-    <row r="8" spans="1:36">
+      <c r="AL7">
+        <v>25.234077623592736</v>
+      </c>
+      <c r="AM7">
+        <v>25.324775484892648</v>
+      </c>
+      <c r="AN7">
+        <v>25.716106122382811</v>
+      </c>
+      <c r="AO7">
+        <v>25.412196622905832</v>
+      </c>
+      <c r="AP7">
+        <v>25.899790799170869</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42">
       <c r="M8" t="str">
         <v>料液侧流速（m/s)</v>
       </c>
@@ -6863,8 +7127,23 @@
       <c r="AJ8">
         <v>1.0575562188444444E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:36" ht="16.5">
+      <c r="AL8">
+        <v>1.0575562188444444E-2</v>
+      </c>
+      <c r="AM8">
+        <v>1.0575562188444444E-2</v>
+      </c>
+      <c r="AN8">
+        <v>1.0575562188444444E-2</v>
+      </c>
+      <c r="AO8">
+        <v>1.0575562188444444E-2</v>
+      </c>
+      <c r="AP8">
+        <v>1.0575562188444444E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" ht="16.5">
       <c r="A9" s="1" t="s">
         <v>128</v>
       </c>
@@ -6940,8 +7219,23 @@
       <c r="AJ9">
         <v>1.0878928809055555E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:36">
+      <c r="AL9">
+        <v>1.0878928809055555E-2</v>
+      </c>
+      <c r="AM9">
+        <v>1.0878928809055555E-2</v>
+      </c>
+      <c r="AN9">
+        <v>1.0878928809055555E-2</v>
+      </c>
+      <c r="AO9">
+        <v>1.0878928809055555E-2</v>
+      </c>
+      <c r="AP9">
+        <v>1.0878928809055555E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42">
       <c r="A10" t="str">
         <f>[1]冷侧实验!U13</f>
         <v>ePTFE</v>
@@ -7050,8 +7344,23 @@
       <c r="AJ10">
         <v>4.8133098240000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:36">
+      <c r="AL10">
+        <v>10.728884735999999</v>
+      </c>
+      <c r="AM10">
+        <v>6.7713711627906985</v>
+      </c>
+      <c r="AN10">
+        <v>5.5270333439999995</v>
+      </c>
+      <c r="AO10">
+        <v>3.0934241280000001</v>
+      </c>
+      <c r="AP10">
+        <v>0.32185294698240002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42">
       <c r="A11" t="str">
         <f>[1]冷侧实验!U14</f>
         <v>ePTFE</v>
@@ -7106,8 +7415,26 @@
       <c r="R11">
         <v>6.5176549910266864E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:36">
+      <c r="AK11" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="AL11">
+        <v>0</v>
+      </c>
+      <c r="AM11">
+        <v>6.5039999999999996</v>
+      </c>
+      <c r="AN11">
+        <v>12.406000000000001</v>
+      </c>
+      <c r="AO11">
+        <v>17.439</v>
+      </c>
+      <c r="AP11">
+        <v>21.963999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42">
       <c r="A12" t="str">
         <f>[1]冷侧实验!U15</f>
         <v>ePTFE</v>
@@ -7163,7 +7490,7 @@
         <v>0.34642769182840333</v>
       </c>
     </row>
-    <row r="13" spans="1:36">
+    <row r="13" spans="1:42">
       <c r="A13" t="str">
         <f>[1]冷侧实验!U16</f>
         <v>ePTFE</v>
@@ -7201,7 +7528,7 @@
         <v>5.6193918719999987</v>
       </c>
     </row>
-    <row r="14" spans="1:36" ht="16.5">
+    <row r="14" spans="1:42" ht="16.5">
       <c r="A14" t="str">
         <f>[1]冷侧实验!U17</f>
         <v>ePTFE</v>
@@ -7257,7 +7584,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:36">
+    <row r="15" spans="1:42">
       <c r="M15" t="str">
         <f t="shared" ref="M15" si="0">M8</f>
         <v>料液侧流速（m/s)</v>
@@ -7354,109 +7681,149 @@
         <f t="shared" si="5"/>
         <v>1.0575562188444444E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:36" ht="16.5">
+      <c r="AL15" s="43">
+        <f t="shared" ref="AL15:AP15" si="6">AL8</f>
+        <v>1.0575562188444444E-2</v>
+      </c>
+      <c r="AM15" s="43">
+        <f t="shared" si="6"/>
+        <v>1.0575562188444444E-2</v>
+      </c>
+      <c r="AN15" s="43">
+        <f t="shared" si="6"/>
+        <v>1.0575562188444444E-2</v>
+      </c>
+      <c r="AO15" s="43">
+        <f t="shared" si="6"/>
+        <v>1.0575562188444444E-2</v>
+      </c>
+      <c r="AP15" s="43">
+        <f t="shared" si="6"/>
+        <v>1.0575562188444444E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42" ht="16.5">
       <c r="A16" s="1" t="s">
         <v>130</v>
       </c>
       <c r="M16" t="str">
-        <f t="shared" ref="M16" si="6">M3</f>
+        <f t="shared" ref="M16" si="7">M3</f>
         <v>料液侧入口温度（℃）</v>
       </c>
       <c r="N16" s="48">
-        <f t="shared" ref="N16:R16" si="7">N3</f>
+        <f t="shared" ref="N16:R16" si="8">N3</f>
         <v>32.804908589380183</v>
       </c>
       <c r="O16" s="43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>37.545921167879214</v>
       </c>
       <c r="P16" s="43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>40.462794041113561</v>
       </c>
       <c r="Q16" s="43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>46.813272232415727</v>
       </c>
       <c r="R16" s="49">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>52.28803056208195</v>
       </c>
       <c r="S16">
-        <f t="shared" ref="S16:W16" si="8">S3</f>
+        <f t="shared" ref="S16:W16" si="9">S3</f>
         <v>46.813272232415727</v>
       </c>
       <c r="T16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>46.735559551037205</v>
       </c>
       <c r="U16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>46.756376974131932</v>
       </c>
       <c r="V16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>46.759715513146396</v>
       </c>
       <c r="W16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>46.795754117384256</v>
       </c>
       <c r="X16">
-        <f t="shared" ref="X16:AB16" si="9">X3</f>
+        <f t="shared" ref="X16:AB16" si="10">X3</f>
         <v>46.765960784537164</v>
       </c>
       <c r="Y16">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>46.747797849449768</v>
       </c>
       <c r="Z16">
-        <f t="shared" si="9"/>
-        <v>46.813272232415727</v>
-      </c>
-      <c r="AA16">
-        <f t="shared" si="9"/>
-        <v>46.780135265158755</v>
-      </c>
-      <c r="AB16">
-        <f t="shared" si="9"/>
-        <v>46.785915070345858</v>
-      </c>
-      <c r="AC16">
-        <f t="shared" ref="AC16:AG16" si="10">AC3</f>
-        <v>46.831304444044484</v>
-      </c>
-      <c r="AD16">
-        <f t="shared" si="10"/>
-        <v>46.835636390276221</v>
-      </c>
-      <c r="AE16">
         <f t="shared" si="10"/>
         <v>46.813272232415727</v>
       </c>
+      <c r="AA16">
+        <f t="shared" si="10"/>
+        <v>46.780135265158755</v>
+      </c>
+      <c r="AB16">
+        <f t="shared" si="10"/>
+        <v>46.785915070345858</v>
+      </c>
+      <c r="AC16">
+        <f t="shared" ref="AC16:AG16" si="11">AC3</f>
+        <v>46.831304444044484</v>
+      </c>
+      <c r="AD16">
+        <f t="shared" si="11"/>
+        <v>46.835636390276221</v>
+      </c>
+      <c r="AE16">
+        <f t="shared" si="11"/>
+        <v>46.813272232415727</v>
+      </c>
       <c r="AF16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>46.773248419935193</v>
       </c>
       <c r="AG16">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>46.772998389800364</v>
       </c>
       <c r="AH16">
-        <f t="shared" ref="AH16:AJ16" si="11">AH3</f>
+        <f t="shared" ref="AH16:AJ16" si="12">AH3</f>
         <v>46.813272232415727</v>
       </c>
       <c r="AI16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>46.83837113278085</v>
       </c>
       <c r="AJ16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>46.843521688179884</v>
       </c>
-    </row>
-    <row r="17" spans="1:38">
+      <c r="AL16" s="43">
+        <f t="shared" ref="AL16:AP16" si="13">AL3</f>
+        <v>46.813272232415727</v>
+      </c>
+      <c r="AM16" s="43">
+        <f t="shared" si="13"/>
+        <v>46.848783530878762</v>
+      </c>
+      <c r="AN16" s="43">
+        <f t="shared" si="13"/>
+        <v>46.810284463894057</v>
+      </c>
+      <c r="AO16" s="43">
+        <f t="shared" si="13"/>
+        <v>46.866582914572703</v>
+      </c>
+      <c r="AP16" s="43">
+        <f t="shared" si="13"/>
+        <v>47.081704781703998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42">
       <c r="A17" t="str">
         <f>[1]热转速实验!S13</f>
         <v>ePTFE</v>
@@ -7498,8 +7865,13 @@
       <c r="P17" s="43"/>
       <c r="Q17" s="43"/>
       <c r="R17" s="49"/>
-    </row>
-    <row r="18" spans="1:38">
+      <c r="AL17" s="43"/>
+      <c r="AM17" s="43"/>
+      <c r="AN17" s="43"/>
+      <c r="AO17" s="43"/>
+      <c r="AP17" s="43"/>
+    </row>
+    <row r="18" spans="1:42">
       <c r="A18" t="str">
         <f>[1]热转速实验!S14</f>
         <v>ePTFE</v>
@@ -7537,103 +7909,123 @@
         <v>10.284390143999998</v>
       </c>
       <c r="M18" t="str">
-        <f t="shared" ref="M18" si="12">M9</f>
+        <f t="shared" ref="M18" si="14">M9</f>
         <v>渗透侧流速（m/s)</v>
       </c>
       <c r="N18" s="48">
-        <f t="shared" ref="N18:R18" si="13">N9</f>
+        <f t="shared" ref="N18:R18" si="15">N9</f>
         <v>1.0024555555555557E-2</v>
       </c>
       <c r="O18" s="43">
-        <f t="shared" si="13"/>
-        <v>1.0024555555555557E-2</v>
-      </c>
-      <c r="P18" s="43">
-        <f t="shared" si="13"/>
-        <v>1.0024555555555557E-2</v>
-      </c>
-      <c r="Q18" s="43">
-        <f t="shared" si="13"/>
-        <v>1.0024555555555557E-2</v>
-      </c>
-      <c r="R18" s="49">
-        <f t="shared" si="13"/>
-        <v>1.0024555555555557E-2</v>
-      </c>
-      <c r="S18">
-        <f t="shared" ref="S18:W18" si="14">S9</f>
-        <v>1.0024555555555557E-2</v>
-      </c>
-      <c r="T18">
-        <f t="shared" si="14"/>
-        <v>1.0024555555555557E-2</v>
-      </c>
-      <c r="U18">
-        <f t="shared" si="14"/>
-        <v>1.0024555555555557E-2</v>
-      </c>
-      <c r="V18">
-        <f t="shared" si="14"/>
-        <v>1.0024555555555557E-2</v>
-      </c>
-      <c r="W18">
-        <f t="shared" si="14"/>
-        <v>1.0024555555555557E-2</v>
-      </c>
-      <c r="X18">
-        <f t="shared" ref="X18:AB18" si="15">X9</f>
-        <v>1.0024555555555557E-2</v>
-      </c>
-      <c r="Y18">
         <f t="shared" si="15"/>
         <v>1.0024555555555557E-2</v>
       </c>
-      <c r="Z18">
+      <c r="P18" s="43">
         <f t="shared" si="15"/>
         <v>1.0024555555555557E-2</v>
       </c>
-      <c r="AA18">
+      <c r="Q18" s="43">
         <f t="shared" si="15"/>
         <v>1.0024555555555557E-2</v>
       </c>
-      <c r="AB18">
+      <c r="R18" s="49">
         <f t="shared" si="15"/>
-        <v>1.0024555555555571E-2</v>
-      </c>
-      <c r="AC18">
-        <f t="shared" ref="AC18:AG18" si="16">AC9</f>
-        <v>4.9995555555555557E-3</v>
-      </c>
-      <c r="AD18">
-        <f t="shared" si="16"/>
-        <v>7.5120555555555539E-3</v>
-      </c>
-      <c r="AE18">
+        <v>1.0024555555555557E-2</v>
+      </c>
+      <c r="S18">
+        <f t="shared" ref="S18:W18" si="16">S9</f>
+        <v>1.0024555555555557E-2</v>
+      </c>
+      <c r="T18">
         <f t="shared" si="16"/>
         <v>1.0024555555555557E-2</v>
       </c>
+      <c r="U18">
+        <f t="shared" si="16"/>
+        <v>1.0024555555555557E-2</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="16"/>
+        <v>1.0024555555555557E-2</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="16"/>
+        <v>1.0024555555555557E-2</v>
+      </c>
+      <c r="X18">
+        <f t="shared" ref="X18:AB18" si="17">X9</f>
+        <v>1.0024555555555557E-2</v>
+      </c>
+      <c r="Y18">
+        <f t="shared" si="17"/>
+        <v>1.0024555555555557E-2</v>
+      </c>
+      <c r="Z18">
+        <f t="shared" si="17"/>
+        <v>1.0024555555555557E-2</v>
+      </c>
+      <c r="AA18">
+        <f t="shared" si="17"/>
+        <v>1.0024555555555557E-2</v>
+      </c>
+      <c r="AB18">
+        <f t="shared" si="17"/>
+        <v>1.0024555555555571E-2</v>
+      </c>
+      <c r="AC18">
+        <f t="shared" ref="AC18:AG18" si="18">AC9</f>
+        <v>4.9995555555555557E-3</v>
+      </c>
+      <c r="AD18">
+        <f t="shared" si="18"/>
+        <v>7.5120555555555539E-3</v>
+      </c>
+      <c r="AE18">
+        <f t="shared" si="18"/>
+        <v>1.0024555555555557E-2</v>
+      </c>
       <c r="AF18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.2537055555555556E-2</v>
       </c>
       <c r="AG18">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>1.5049555555555552E-2</v>
       </c>
       <c r="AH18">
-        <f t="shared" ref="AH18:AJ18" si="17">AH9</f>
+        <f t="shared" ref="AH18:AJ18" si="19">AH9</f>
         <v>1.0878928809055555E-2</v>
       </c>
       <c r="AI18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1.0878928809055555E-2</v>
       </c>
       <c r="AJ18">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1.0878928809055555E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:38">
+      <c r="AL18" s="43">
+        <f t="shared" ref="AL18:AP18" si="20">AL9</f>
+        <v>1.0878928809055555E-2</v>
+      </c>
+      <c r="AM18" s="43">
+        <f t="shared" si="20"/>
+        <v>1.0878928809055555E-2</v>
+      </c>
+      <c r="AN18" s="43">
+        <f t="shared" si="20"/>
+        <v>1.0878928809055555E-2</v>
+      </c>
+      <c r="AO18" s="43">
+        <f t="shared" si="20"/>
+        <v>1.0878928809055555E-2</v>
+      </c>
+      <c r="AP18" s="43">
+        <f t="shared" si="20"/>
+        <v>1.0878928809055555E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42">
       <c r="A19" t="str">
         <f>[1]热转速实验!S15</f>
         <v>ePTFE</v>
@@ -7671,103 +8063,123 @@
         <v>10.728884735999999</v>
       </c>
       <c r="M19" t="str">
-        <f t="shared" ref="M19" si="18">M5</f>
+        <f t="shared" ref="M19" si="21">M5</f>
         <v>渗透侧入口温度（℃）</v>
       </c>
       <c r="N19" s="48">
-        <f t="shared" ref="N19:R19" si="19">N5</f>
+        <f t="shared" ref="N19:R19" si="22">N5</f>
         <v>20.020584823493895</v>
       </c>
       <c r="O19" s="43">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>20.013996907080195</v>
       </c>
       <c r="P19" s="43">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>20.040555205268429</v>
       </c>
       <c r="Q19" s="43">
-        <f t="shared" si="19"/>
-        <v>19.965192717598594</v>
-      </c>
-      <c r="R19" s="49">
-        <f t="shared" si="19"/>
-        <v>20.531591054442632</v>
-      </c>
-      <c r="S19">
-        <f t="shared" ref="S19:W19" si="20">S5</f>
-        <v>19.965192717598594</v>
-      </c>
-      <c r="T19">
-        <f t="shared" si="20"/>
-        <v>25.020477816258023</v>
-      </c>
-      <c r="U19">
-        <f t="shared" si="20"/>
-        <v>29.996660937349375</v>
-      </c>
-      <c r="V19">
-        <f t="shared" si="20"/>
-        <v>34.981044802983121</v>
-      </c>
-      <c r="W19">
-        <f t="shared" si="20"/>
-        <v>39.995611966534248</v>
-      </c>
-      <c r="X19">
-        <f t="shared" ref="X19:AB19" si="21">X5</f>
-        <v>19.95147626262694</v>
-      </c>
-      <c r="Y19">
-        <f t="shared" si="21"/>
-        <v>19.98472615642196</v>
-      </c>
-      <c r="Z19">
-        <f t="shared" si="21"/>
-        <v>19.965192717598594</v>
-      </c>
-      <c r="AA19">
-        <f t="shared" si="21"/>
-        <v>19.98426554012838</v>
-      </c>
-      <c r="AB19">
-        <f t="shared" si="21"/>
-        <v>20.033552339221512</v>
-      </c>
-      <c r="AC19">
-        <f t="shared" ref="AC19:AG19" si="22">AC5</f>
-        <v>19.99611427063822</v>
-      </c>
-      <c r="AD19">
-        <f t="shared" si="22"/>
-        <v>19.985256383306695</v>
-      </c>
-      <c r="AE19">
         <f t="shared" si="22"/>
         <v>19.965192717598594</v>
       </c>
+      <c r="R19" s="49">
+        <f t="shared" si="22"/>
+        <v>20.531591054442632</v>
+      </c>
+      <c r="S19">
+        <f t="shared" ref="S19:W19" si="23">S5</f>
+        <v>19.965192717598594</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="23"/>
+        <v>25.020477816258023</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="23"/>
+        <v>29.996660937349375</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="23"/>
+        <v>34.981044802983121</v>
+      </c>
+      <c r="W19">
+        <f t="shared" si="23"/>
+        <v>39.995611966534248</v>
+      </c>
+      <c r="X19">
+        <f t="shared" ref="X19:AB19" si="24">X5</f>
+        <v>19.95147626262694</v>
+      </c>
+      <c r="Y19">
+        <f t="shared" si="24"/>
+        <v>19.98472615642196</v>
+      </c>
+      <c r="Z19">
+        <f t="shared" si="24"/>
+        <v>19.965192717598594</v>
+      </c>
+      <c r="AA19">
+        <f t="shared" si="24"/>
+        <v>19.98426554012838</v>
+      </c>
+      <c r="AB19">
+        <f t="shared" si="24"/>
+        <v>20.033552339221512</v>
+      </c>
+      <c r="AC19">
+        <f t="shared" ref="AC19:AG19" si="25">AC5</f>
+        <v>19.99611427063822</v>
+      </c>
+      <c r="AD19">
+        <f t="shared" si="25"/>
+        <v>19.985256383306695</v>
+      </c>
+      <c r="AE19">
+        <f t="shared" si="25"/>
+        <v>19.965192717598594</v>
+      </c>
       <c r="AF19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>19.978884732789933</v>
       </c>
       <c r="AG19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="25"/>
         <v>19.940144584158414</v>
       </c>
       <c r="AH19">
-        <f t="shared" ref="AH19:AJ19" si="23">AH5</f>
+        <f t="shared" ref="AH19:AJ19" si="26">AH5</f>
         <v>19.965192717598594</v>
       </c>
       <c r="AI19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>19.962840387781814</v>
       </c>
       <c r="AJ19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="26"/>
         <v>19.94308391529044</v>
       </c>
-    </row>
-    <row r="20" spans="1:38">
+      <c r="AL19" s="43">
+        <f t="shared" ref="AL19:AP19" si="27">AL5</f>
+        <v>19.965192717598594</v>
+      </c>
+      <c r="AM19" s="43">
+        <f t="shared" si="27"/>
+        <v>19.989925140361731</v>
+      </c>
+      <c r="AN19" s="43">
+        <f t="shared" si="27"/>
+        <v>19.900375117224076</v>
+      </c>
+      <c r="AO19" s="43">
+        <f t="shared" si="27"/>
+        <v>19.998618090452187</v>
+      </c>
+      <c r="AP19" s="43">
+        <f t="shared" si="27"/>
+        <v>19.971794871794781</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42">
       <c r="A20" t="str">
         <f>[1]热转速实验!S16</f>
         <v>ePTFE</v>
@@ -7809,8 +8221,13 @@
       <c r="P20" s="43"/>
       <c r="Q20" s="43"/>
       <c r="R20" s="49"/>
-    </row>
-    <row r="21" spans="1:38">
+      <c r="AL20" s="43"/>
+      <c r="AM20" s="43"/>
+      <c r="AN20" s="43"/>
+      <c r="AO20" s="43"/>
+      <c r="AP20" s="43"/>
+    </row>
+    <row r="21" spans="1:42">
       <c r="A21" t="str">
         <f>[1]热转速实验!S17</f>
         <v>ePTFE</v>
@@ -7848,302 +8265,362 @@
         <v>11.167119743999999</v>
       </c>
       <c r="M21" t="str">
-        <f t="shared" ref="M21" si="24">M4</f>
+        <f t="shared" ref="M21" si="28">M4</f>
         <v>料液侧出口温度（℃）</v>
       </c>
       <c r="N21" s="48">
-        <f t="shared" ref="N21:R21" si="25">N4</f>
+        <f t="shared" ref="N21:R21" si="29">N4</f>
         <v>32.209159619805561</v>
       </c>
       <c r="O21" s="43">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>36.641882535934052</v>
       </c>
       <c r="P21" s="43">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>39.206231593240013</v>
       </c>
       <c r="Q21" s="43">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>45.115007004655496</v>
       </c>
       <c r="R21" s="49">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>50.488628590359532</v>
       </c>
       <c r="S21">
-        <f t="shared" ref="S21:W21" si="26">S4</f>
+        <f t="shared" ref="S21:W21" si="30">S4</f>
         <v>45.115007004655496</v>
       </c>
       <c r="T21">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>45.152704364084947</v>
       </c>
       <c r="U21">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>45.332937279628425</v>
       </c>
       <c r="V21">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>45.65301197436299</v>
       </c>
       <c r="W21">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>45.862899949634645</v>
       </c>
       <c r="X21">
-        <f t="shared" ref="X21:AB21" si="27">X4</f>
+        <f t="shared" ref="X21:AB21" si="31">X4</f>
         <v>46.414726050719302</v>
       </c>
       <c r="Y21">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>45.253056164715588</v>
       </c>
       <c r="Z21">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>45.115007004655496</v>
       </c>
       <c r="AA21">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>45.554121695468943</v>
       </c>
       <c r="AB21">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>45.667769594471679</v>
       </c>
       <c r="AC21">
-        <f t="shared" ref="AC21:AG21" si="28">AC4</f>
+        <f t="shared" ref="AC21:AG21" si="32">AC4</f>
         <v>45.410532556242877</v>
       </c>
       <c r="AD21">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>45.366644909743457</v>
       </c>
       <c r="AE21">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>45.115007004655496</v>
       </c>
       <c r="AF21">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>45.184878246406505</v>
       </c>
       <c r="AG21">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>45.148270505308638</v>
       </c>
       <c r="AH21">
-        <f t="shared" ref="AH21:AJ21" si="29">AH4</f>
+        <f t="shared" ref="AH21:AJ21" si="33">AH4</f>
         <v>45.115007004655496</v>
       </c>
       <c r="AI21">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>45.243818979301523</v>
       </c>
       <c r="AJ21">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>44.928683240302114</v>
       </c>
-    </row>
-    <row r="22" spans="1:38">
+      <c r="AL21" s="43">
+        <f t="shared" ref="AL21:AP21" si="34">AL4</f>
+        <v>45.115007004655496</v>
+      </c>
+      <c r="AM21" s="43">
+        <f t="shared" si="34"/>
+        <v>45.433250155957296</v>
+      </c>
+      <c r="AN21" s="43">
+        <f t="shared" si="34"/>
+        <v>46.127227258519227</v>
+      </c>
+      <c r="AO21" s="43">
+        <f t="shared" si="34"/>
+        <v>45.261652010050049</v>
+      </c>
+      <c r="AP21" s="43">
+        <f t="shared" si="34"/>
+        <v>45.950311850311486</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42">
       <c r="M22" t="str">
-        <f t="shared" ref="M22" si="30">M6</f>
+        <f t="shared" ref="M22" si="35">M6</f>
         <v>渗透侧出口温度（℃）</v>
       </c>
       <c r="N22" s="48">
-        <f t="shared" ref="N22:R22" si="31">N6</f>
+        <f t="shared" ref="N22:R22" si="36">N6</f>
         <v>21.1468268936618</v>
       </c>
       <c r="O22" s="43">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>21.066646083396979</v>
       </c>
       <c r="P22" s="43">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>21.202254882336835</v>
       </c>
       <c r="Q22" s="43">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>21.428861307302665</v>
       </c>
       <c r="R22" s="49">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>21.993250061846652</v>
       </c>
       <c r="S22">
-        <f t="shared" ref="S22:W22" si="32">S6</f>
+        <f t="shared" ref="S22:W22" si="37">S6</f>
         <v>21.428861307302665</v>
       </c>
       <c r="T22">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>26.071689439399325</v>
       </c>
       <c r="U22">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>30.76148736331346</v>
       </c>
       <c r="V22">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>35.502290509265826</v>
       </c>
       <c r="W22">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>40.423454833974333</v>
       </c>
       <c r="X22">
-        <f t="shared" ref="X22:AB22" si="33">X6</f>
+        <f t="shared" ref="X22:AB22" si="38">X6</f>
         <v>21.494944118539394</v>
       </c>
       <c r="Y22">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>21.517883020301912</v>
       </c>
       <c r="Z22">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>21.428861307302665</v>
       </c>
       <c r="AA22">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>21.595394953178555</v>
       </c>
       <c r="AB22">
-        <f t="shared" si="33"/>
+        <f t="shared" si="38"/>
         <v>21.805176462942171</v>
       </c>
       <c r="AC22">
-        <f t="shared" ref="AC22:AG22" si="34">AC6</f>
+        <f t="shared" ref="AC22:AG22" si="39">AC6</f>
         <v>21.733402276973759</v>
       </c>
       <c r="AD22">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>21.854517375313929</v>
       </c>
       <c r="AE22">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>21.428861307302665</v>
       </c>
       <c r="AF22">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>21.479081058045157</v>
       </c>
       <c r="AG22">
-        <f t="shared" si="34"/>
+        <f t="shared" si="39"/>
         <v>21.310467600503262</v>
       </c>
       <c r="AH22">
-        <f t="shared" ref="AH22:AJ22" si="35">AH6</f>
+        <f t="shared" ref="AH22:AJ22" si="40">AH6</f>
         <v>21.428861307302665</v>
       </c>
       <c r="AI22">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>21.478318390552261</v>
       </c>
       <c r="AJ22">
-        <f t="shared" si="35"/>
+        <f t="shared" si="40"/>
         <v>21.306892948428231</v>
       </c>
-    </row>
-    <row r="23" spans="1:38" ht="16.5">
+      <c r="AL22" s="43">
+        <f t="shared" ref="AL22:AP22" si="41">AL6</f>
+        <v>21.428861307302665</v>
+      </c>
+      <c r="AM22" s="43">
+        <f t="shared" si="41"/>
+        <v>21.583000623829477</v>
+      </c>
+      <c r="AN22" s="43">
+        <f t="shared" si="41"/>
+        <v>21.569084088778226</v>
+      </c>
+      <c r="AO22" s="43">
+        <f t="shared" si="41"/>
+        <v>21.251664572864392</v>
+      </c>
+      <c r="AP22" s="43">
+        <f t="shared" si="41"/>
+        <v>21.224081774082016</v>
+      </c>
+    </row>
+    <row r="23" spans="1:42" ht="16.5">
       <c r="A23" s="1" t="s">
         <v>127</v>
       </c>
       <c r="M23" t="str">
-        <f t="shared" ref="M23:R23" si="36">M10</f>
+        <f t="shared" ref="M23:R23" si="42">M10</f>
         <v>平均膜渗透通量（kg·m-2·h-1）</v>
       </c>
       <c r="N23" s="50">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>3.8848588799999995</v>
       </c>
       <c r="O23" s="44">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>5.667941375999999</v>
       </c>
       <c r="P23" s="44">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>7.0075795200000002</v>
       </c>
       <c r="Q23" s="44">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>10.728884735999999</v>
       </c>
       <c r="R23" s="51">
-        <f t="shared" si="36"/>
+        <f t="shared" si="42"/>
         <v>14.106180095999997</v>
       </c>
       <c r="S23">
-        <f t="shared" ref="S23:AJ23" si="37">S10</f>
+        <f t="shared" ref="S23:AJ23" si="43">S10</f>
         <v>10.728884735999999</v>
       </c>
       <c r="T23">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>9.2522250239999995</v>
       </c>
       <c r="U23">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>7.6446888960000008</v>
       </c>
       <c r="V23">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>5.6193918719999987</v>
       </c>
       <c r="W23">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>3.5767384319999995</v>
       </c>
       <c r="X23">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>10.576399104</v>
       </c>
       <c r="Y23">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>10.284390143999998</v>
       </c>
       <c r="Z23">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>10.728884735999999</v>
       </c>
       <c r="AA23">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>10.960891391999999</v>
       </c>
       <c r="AB23">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>11.167119743999999</v>
       </c>
       <c r="AC23">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>9.8861740800000018</v>
       </c>
       <c r="AD23">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>10.167006336</v>
       </c>
       <c r="AE23">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>10.728884735999999</v>
       </c>
       <c r="AF23">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>11.559156864</v>
       </c>
       <c r="AG23">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>11.892979584000001</v>
       </c>
       <c r="AH23">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>10.728884735999999</v>
       </c>
       <c r="AI23">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>3.5032684799999991</v>
       </c>
       <c r="AJ23">
-        <f t="shared" si="37"/>
+        <f t="shared" si="43"/>
         <v>4.8133098240000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:38" s="42" customFormat="1">
+      <c r="AL23" s="43">
+        <f t="shared" ref="AL23:AP23" si="44">AL10</f>
+        <v>10.728884735999999</v>
+      </c>
+      <c r="AM23" s="43">
+        <f t="shared" si="44"/>
+        <v>6.7713711627906985</v>
+      </c>
+      <c r="AN23" s="43">
+        <f t="shared" si="44"/>
+        <v>5.5270333439999995</v>
+      </c>
+      <c r="AO23" s="43">
+        <f t="shared" si="44"/>
+        <v>3.0934241280000001</v>
+      </c>
+      <c r="AP23" s="43">
+        <f t="shared" si="44"/>
+        <v>0.32185294698240002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:42" s="42" customFormat="1">
       <c r="A24" t="str">
         <f>[1]冷转速实验!T13</f>
         <v>ePTFE</v>
@@ -8188,95 +8665,102 @@
         <v/>
       </c>
       <c r="O24" s="43" t="str">
-        <f t="shared" ref="O24:AJ24" si="38">IF(O26=1, "duplicate","")</f>
+        <f t="shared" ref="O24:AP24" si="45">IF(O26=1, "duplicate","")</f>
         <v/>
       </c>
       <c r="P24" s="43" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="Q24" s="43" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="R24" s="43" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="S24" s="43" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>duplicate</v>
       </c>
       <c r="T24" s="43" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="U24" s="43" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="V24" s="43" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="W24" s="43" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="X24" s="43" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="Y24" s="43" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="Z24" s="43" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>duplicate</v>
       </c>
       <c r="AA24" s="43" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="AB24" s="43" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="AC24" s="43" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="AD24" s="43" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="AE24" s="43" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>duplicate</v>
       </c>
       <c r="AF24" s="43" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="AG24" s="43" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="AH24" s="43" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v>duplicate</v>
       </c>
       <c r="AI24" s="43" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="AJ24" s="43" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
-    </row>
-    <row r="25" spans="1:38">
+      <c r="AL24" s="43" t="s">
+        <v>147</v>
+      </c>
+      <c r="AM24" s="43"/>
+      <c r="AN24" s="43"/>
+      <c r="AO24" s="43"/>
+      <c r="AP24" s="43"/>
+    </row>
+    <row r="25" spans="1:42">
       <c r="A25" t="str">
         <f>[1]冷转速实验!T14</f>
         <v>ePTFE</v>
@@ -8386,7 +8870,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:38" s="42" customFormat="1">
+    <row r="26" spans="1:42" s="42" customFormat="1">
       <c r="A26" t="str">
         <f>[1]冷转速实验!T15</f>
         <v>ePTFE</v>
@@ -8428,95 +8912,95 @@
         <v>0</v>
       </c>
       <c r="O26" s="42">
-        <f t="shared" ref="O26:AJ26" si="39">HLOOKUP(O25,$N28:$AJ31,4,FALSE)</f>
+        <f t="shared" ref="O26:AJ26" si="46">HLOOKUP(O25,$N28:$AJ31,4,FALSE)</f>
         <v>0</v>
       </c>
       <c r="P26" s="42">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="Q26" s="42">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="R26" s="42">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="S26" s="42">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>1</v>
       </c>
       <c r="T26" s="42">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="U26" s="42">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="V26" s="42">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="W26" s="42">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="X26" s="42">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="Y26" s="42">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="Z26" s="42">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>1</v>
       </c>
       <c r="AA26" s="42">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="AB26" s="42">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="AC26" s="42">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="AD26" s="42">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="AE26" s="42">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>1</v>
       </c>
       <c r="AF26" s="42">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="AG26" s="42">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="AH26" s="42">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>1</v>
       </c>
       <c r="AI26" s="42">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
       <c r="AJ26" s="42">
-        <f t="shared" si="39"/>
+        <f t="shared" si="46"/>
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:38" ht="16.5">
+    <row r="27" spans="1:42" ht="16.5">
       <c r="A27" t="str">
         <f>[1]冷转速实验!T16</f>
         <v>ePTFE</v>
@@ -8566,7 +9050,7 @@
       <c r="V27" s="42"/>
       <c r="W27" s="42"/>
     </row>
-    <row r="28" spans="1:38">
+    <row r="28" spans="1:42">
       <c r="A28" t="str">
         <f>[1]冷转速实验!T17</f>
         <v>ePTFE</v>
@@ -8676,7 +9160,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:38">
+    <row r="29" spans="1:42">
       <c r="M29" s="42" t="s">
         <v>139</v>
       </c>
@@ -8752,7 +9236,7 @@
       <c r="AK29" s="42"/>
       <c r="AL29" s="42"/>
     </row>
-    <row r="30" spans="1:38" ht="16.5">
+    <row r="30" spans="1:42" ht="16.5">
       <c r="A30" s="1" t="s">
         <v>131</v>
       </c>
@@ -8829,7 +9313,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:38">
+    <row r="31" spans="1:42">
       <c r="A31" t="str">
         <f>[1]膜种类实验!P15</f>
         <v>ePTFE</v>
@@ -8874,95 +9358,95 @@
         <v>0</v>
       </c>
       <c r="O31" s="42">
-        <f t="shared" ref="O31:AJ31" si="40">IF(MATCH(O29,$N29:$AN29,0)=O30, 0, 1)</f>
+        <f t="shared" ref="O31:AJ31" si="47">IF(MATCH(O29,$N29:$AN29,0)=O30, 0, 1)</f>
         <v>0</v>
       </c>
       <c r="P31" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Q31" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="R31" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="S31" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="T31" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="U31" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="V31" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="W31" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="X31" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Y31" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="Z31" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="AA31" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="AB31" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>1</v>
       </c>
       <c r="AC31" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>1</v>
       </c>
       <c r="AD31" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>1</v>
       </c>
       <c r="AE31" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>1</v>
       </c>
       <c r="AF31" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="AG31" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="AH31" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="AI31" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="AJ31" s="42">
-        <f t="shared" si="40"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:38">
+    <row r="32" spans="1:42">
       <c r="A32" t="str">
         <f>[1]膜种类实验!P16</f>
         <v>PTFE</v>
@@ -9001,7 +9485,7 @@
       </c>
       <c r="O32" s="42"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:10">
       <c r="A33" t="str">
         <f>[1]膜种类实验!P17</f>
         <v>PVDF</v>
@@ -9037,6 +9521,224 @@
       <c r="I33">
         <f>[1]膜种类实验!X17</f>
         <v>4.8133098240000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="16.5">
+      <c r="A35" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="J35" s="42" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" t="str">
+        <f>[1]浓度实验!P15</f>
+        <v>ePTFE</v>
+      </c>
+      <c r="B36">
+        <f>[1]浓度实验!Q15</f>
+        <v>46.813272232415727</v>
+      </c>
+      <c r="C36">
+        <f>[1]浓度实验!R15</f>
+        <v>45.115007004655496</v>
+      </c>
+      <c r="D36">
+        <f>[1]浓度实验!S15</f>
+        <v>19.965192717598594</v>
+      </c>
+      <c r="E36">
+        <f>[1]浓度实验!T15</f>
+        <v>21.428861307302665</v>
+      </c>
+      <c r="F36">
+        <f>[1]浓度实验!U15</f>
+        <v>25.234077623592736</v>
+      </c>
+      <c r="G36">
+        <f>[1]浓度实验!V15</f>
+        <v>1.0575562188444444E-2</v>
+      </c>
+      <c r="H36">
+        <f>[1]浓度实验!W15</f>
+        <v>1.0878928809055555E-2</v>
+      </c>
+      <c r="I36">
+        <f>[1]浓度实验!X15</f>
+        <v>10.728884735999999</v>
+      </c>
+      <c r="J36">
+        <f>[1]浓度实验!Y15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" t="str">
+        <f>[1]浓度实验!P16</f>
+        <v>ePTFE</v>
+      </c>
+      <c r="B37">
+        <f>[1]浓度实验!Q16</f>
+        <v>46.848783530878762</v>
+      </c>
+      <c r="C37">
+        <f>[1]浓度实验!R16</f>
+        <v>45.433250155957296</v>
+      </c>
+      <c r="D37">
+        <f>[1]浓度实验!S16</f>
+        <v>19.989925140361731</v>
+      </c>
+      <c r="E37">
+        <f>[1]浓度实验!T16</f>
+        <v>21.583000623829477</v>
+      </c>
+      <c r="F37">
+        <f>[1]浓度实验!U16</f>
+        <v>25.324775484892648</v>
+      </c>
+      <c r="G37">
+        <f>[1]浓度实验!V16</f>
+        <v>1.0575562188444444E-2</v>
+      </c>
+      <c r="H37">
+        <f>[1]浓度实验!W16</f>
+        <v>1.0878928809055555E-2</v>
+      </c>
+      <c r="I37">
+        <f>[1]浓度实验!X16</f>
+        <v>6.7713711627906985</v>
+      </c>
+      <c r="J37">
+        <f>[1]浓度实验!Y16</f>
+        <v>6.5039999999999996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" t="str">
+        <f>[1]浓度实验!P17</f>
+        <v>ePTFE</v>
+      </c>
+      <c r="B38">
+        <f>[1]浓度实验!Q17</f>
+        <v>46.810284463894057</v>
+      </c>
+      <c r="C38">
+        <f>[1]浓度实验!R17</f>
+        <v>46.127227258519227</v>
+      </c>
+      <c r="D38">
+        <f>[1]浓度实验!S17</f>
+        <v>19.900375117224076</v>
+      </c>
+      <c r="E38">
+        <f>[1]浓度实验!T17</f>
+        <v>21.569084088778226</v>
+      </c>
+      <c r="F38">
+        <f>[1]浓度实验!U17</f>
+        <v>25.716106122382811</v>
+      </c>
+      <c r="G38">
+        <f>[1]浓度实验!V17</f>
+        <v>1.0575562188444444E-2</v>
+      </c>
+      <c r="H38">
+        <f>[1]浓度实验!W17</f>
+        <v>1.0878928809055555E-2</v>
+      </c>
+      <c r="I38">
+        <f>[1]浓度实验!X17</f>
+        <v>5.5270333439999995</v>
+      </c>
+      <c r="J38">
+        <f>[1]浓度实验!Y17</f>
+        <v>12.406000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" t="str">
+        <f>[1]浓度实验!P18</f>
+        <v>ePTFE</v>
+      </c>
+      <c r="B39">
+        <f>[1]浓度实验!Q18</f>
+        <v>46.866582914572703</v>
+      </c>
+      <c r="C39">
+        <f>[1]浓度实验!R18</f>
+        <v>45.261652010050049</v>
+      </c>
+      <c r="D39">
+        <f>[1]浓度实验!S18</f>
+        <v>19.998618090452187</v>
+      </c>
+      <c r="E39">
+        <f>[1]浓度实验!T18</f>
+        <v>21.251664572864392</v>
+      </c>
+      <c r="F39">
+        <f>[1]浓度实验!U18</f>
+        <v>25.412196622905832</v>
+      </c>
+      <c r="G39">
+        <f>[1]浓度实验!V18</f>
+        <v>1.0575562188444444E-2</v>
+      </c>
+      <c r="H39">
+        <f>[1]浓度实验!W18</f>
+        <v>1.0878928809055555E-2</v>
+      </c>
+      <c r="I39">
+        <f>[1]浓度实验!X18</f>
+        <v>3.0934241280000001</v>
+      </c>
+      <c r="J39">
+        <f>[1]浓度实验!Y18</f>
+        <v>17.439</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" t="str">
+        <f>[1]浓度实验!P19</f>
+        <v>ePTFE</v>
+      </c>
+      <c r="B40">
+        <f>[1]浓度实验!Q19</f>
+        <v>47.081704781703998</v>
+      </c>
+      <c r="C40">
+        <f>[1]浓度实验!R19</f>
+        <v>45.950311850311486</v>
+      </c>
+      <c r="D40">
+        <f>[1]浓度实验!S19</f>
+        <v>19.971794871794781</v>
+      </c>
+      <c r="E40">
+        <f>[1]浓度实验!T19</f>
+        <v>21.224081774082016</v>
+      </c>
+      <c r="F40">
+        <f>[1]浓度实验!U19</f>
+        <v>25.899790799170869</v>
+      </c>
+      <c r="G40">
+        <f>[1]浓度实验!V19</f>
+        <v>1.0575562188444444E-2</v>
+      </c>
+      <c r="H40">
+        <f>[1]浓度实验!W19</f>
+        <v>1.0878928809055555E-2</v>
+      </c>
+      <c r="I40">
+        <f>[1]浓度实验!X19</f>
+        <v>0.32185294698240002</v>
+      </c>
+      <c r="J40">
+        <f>[1]浓度实验!Y19</f>
+        <v>21.963999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add FLUENT case and date files to complete the CFD verification for varied feeding concentration [BUG] the influent velocities of case #12-19 in "reorganized exp.data.xlsx" have beem wrongly specified and highlight mark
</commit_message>
<xml_diff>
--- a/bin/2d_s_cc/reorganized exp.data.xlsx
+++ b/bin/2d_s_cc/reorganized exp.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="75" windowWidth="17235" windowHeight="8955" activeTab="2"/>
+    <workbookView xWindow="2340" yWindow="75" windowWidth="17235" windowHeight="8955" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Wang&amp;Chung2008CES" sheetId="1" r:id="rId1"/>
@@ -226,8 +226,42 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Guoqiang GUAN</author>
+  </authors>
+  <commentList>
+    <comment ref="AA55" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Guoqiang GUAN:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Based on 16GGQ-2-4.cas, apply the correlation of physical properties in V3.0</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="149">
   <si>
     <t>Wang K Y, Chung T S, Gryta M. Chem. Eng. Sci., 2008, 63: 2587-2594</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -732,6 +766,9 @@
   <si>
     <t>duplicate</t>
   </si>
+  <si>
+    <t>16GGQ-3-</t>
+  </si>
 </sst>
 </file>
 
@@ -740,7 +777,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -887,8 +924,21 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -933,6 +983,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1079,7 +1135,7 @@
     <xf numFmtId="0" fontId="17" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1254,6 +1310,12 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="8" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="9" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="1" xfId="8" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -1335,23 +1397,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="183920896"/>
-        <c:axId val="183934976"/>
+        <c:axId val="235652608"/>
+        <c:axId val="235654144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="183920896"/>
+        <c:axId val="235652608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183934976"/>
+        <c:crossAx val="235654144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="183934976"/>
+        <c:axId val="235654144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1359,7 +1421,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183920896"/>
+        <c:crossAx val="235652608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1373,7 +1435,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3083,13 +3145,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y64"/>
+  <dimension ref="A1:AE64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="O20" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="V34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC39" sqref="AC39"/>
+      <selection pane="bottomRight" activeCell="AE62" sqref="AE62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3099,14 +3161,14 @@
     <col min="3" max="3" width="9.28515625" style="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="17" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="9.140625" style="17"/>
+    <col min="7" max="11" width="9.140625" style="17" customWidth="1"/>
     <col min="12" max="12" width="11.28515625" style="17" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="17"/>
+    <col min="13" max="13" width="9.140625" style="17" customWidth="1"/>
     <col min="14" max="14" width="9.7109375" style="17" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="17"/>
-    <col min="16" max="19" width="10" style="17" bestFit="1" customWidth="1"/>
-    <col min="20" max="23" width="9.140625" style="17"/>
-    <col min="24" max="25" width="10.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="17" customWidth="1"/>
+    <col min="16" max="19" width="10" style="17" customWidth="1"/>
+    <col min="20" max="23" width="9.140625" style="17" customWidth="1"/>
+    <col min="24" max="25" width="10.28515625" style="17" customWidth="1"/>
     <col min="26" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
@@ -3287,7 +3349,7 @@
       <c r="D16" s="33"/>
       <c r="E16" s="33"/>
     </row>
-    <row r="17" spans="1:25" s="34" customFormat="1">
+    <row r="17" spans="1:31" s="34" customFormat="1">
       <c r="A17" s="33" t="s">
         <v>66</v>
       </c>
@@ -3300,7 +3362,7 @@
       <c r="D17" s="33"/>
       <c r="E17" s="33"/>
     </row>
-    <row r="18" spans="1:25" s="34" customFormat="1">
+    <row r="18" spans="1:31" s="34" customFormat="1">
       <c r="A18" s="33" t="s">
         <v>76</v>
       </c>
@@ -3311,7 +3373,7 @@
       <c r="D18" s="33"/>
       <c r="E18" s="33"/>
     </row>
-    <row r="19" spans="1:25" s="34" customFormat="1">
+    <row r="19" spans="1:31" s="34" customFormat="1">
       <c r="A19" s="33" t="s">
         <v>77</v>
       </c>
@@ -3322,13 +3384,33 @@
       <c r="D19" s="33"/>
       <c r="E19" s="33"/>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:31">
       <c r="A20" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C20" s="19"/>
-    </row>
-    <row r="21" spans="1:25" s="27" customFormat="1">
+      <c r="AA20" s="24">
+        <f>100-AA21</f>
+        <v>100</v>
+      </c>
+      <c r="AB20" s="24">
+        <f t="shared" ref="AB20:AE20" si="0">100-AB21</f>
+        <v>93.495999999999995</v>
+      </c>
+      <c r="AC20" s="24">
+        <f t="shared" si="0"/>
+        <v>87.593999999999994</v>
+      </c>
+      <c r="AD20" s="24">
+        <f t="shared" si="0"/>
+        <v>82.561000000000007</v>
+      </c>
+      <c r="AE20" s="24">
+        <f t="shared" si="0"/>
+        <v>78.036000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" s="27" customFormat="1">
       <c r="A21" s="26" t="s">
         <v>94</v>
       </c>
@@ -3404,8 +3486,28 @@
       <c r="Y21" s="20">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:25" s="27" customFormat="1">
+      <c r="AA21" s="53">
+        <f>ExpData!AL11</f>
+        <v>0</v>
+      </c>
+      <c r="AB21" s="53">
+        <f>ExpData!AM11</f>
+        <v>6.5039999999999996</v>
+      </c>
+      <c r="AC21" s="53">
+        <f>ExpData!AN11</f>
+        <v>12.406000000000001</v>
+      </c>
+      <c r="AD21" s="53">
+        <f>ExpData!AO11</f>
+        <v>17.439</v>
+      </c>
+      <c r="AE21" s="53">
+        <f>ExpData!AP11</f>
+        <v>21.963999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" s="27" customFormat="1">
       <c r="A22" s="28" t="s">
         <v>125</v>
       </c>
@@ -3433,8 +3535,13 @@
       <c r="W22" s="26"/>
       <c r="X22" s="26"/>
       <c r="Y22" s="26"/>
-    </row>
-    <row r="23" spans="1:25" s="27" customFormat="1">
+      <c r="AA22" s="26"/>
+      <c r="AB22" s="26"/>
+      <c r="AC22" s="26"/>
+      <c r="AD22" s="26"/>
+      <c r="AE22" s="26"/>
+    </row>
+    <row r="23" spans="1:31" s="27" customFormat="1">
       <c r="A23" s="26" t="s">
         <v>96</v>
       </c>
@@ -3510,8 +3617,23 @@
       <c r="Y23" s="20">
         <v>100</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" s="27" customFormat="1">
+      <c r="AA23" s="20">
+        <v>100</v>
+      </c>
+      <c r="AB23" s="20">
+        <v>100</v>
+      </c>
+      <c r="AC23" s="20">
+        <v>100</v>
+      </c>
+      <c r="AD23" s="20">
+        <v>100</v>
+      </c>
+      <c r="AE23" s="20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" s="27" customFormat="1">
       <c r="A24" s="29" t="s">
         <v>98</v>
       </c>
@@ -3587,8 +3709,23 @@
       <c r="Y24" s="20">
         <v>100</v>
       </c>
-    </row>
-    <row r="25" spans="1:25" s="27" customFormat="1">
+      <c r="AA24" s="20">
+        <v>100</v>
+      </c>
+      <c r="AB24" s="20">
+        <v>100</v>
+      </c>
+      <c r="AC24" s="20">
+        <v>100</v>
+      </c>
+      <c r="AD24" s="20">
+        <v>100</v>
+      </c>
+      <c r="AE24" s="20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" s="27" customFormat="1">
       <c r="A25" s="28" t="s">
         <v>126</v>
       </c>
@@ -3617,7 +3754,7 @@
       <c r="X25" s="29"/>
       <c r="Y25" s="29"/>
     </row>
-    <row r="26" spans="1:25" s="27" customFormat="1">
+    <row r="26" spans="1:31" s="27" customFormat="1">
       <c r="A26" s="26" t="s">
         <v>96</v>
       </c>
@@ -3629,19 +3766,19 @@
         <v>189.89</v>
       </c>
       <c r="D26" s="24">
-        <f t="shared" ref="D26:G26" si="0">-22.11+2.12*D23</f>
+        <f t="shared" ref="D26:G26" si="1">-22.11+2.12*D23</f>
         <v>189.89</v>
       </c>
       <c r="E26" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>189.89</v>
       </c>
       <c r="F26" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>189.89</v>
       </c>
       <c r="G26" s="24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>189.89</v>
       </c>
       <c r="H26" s="24">
@@ -3649,19 +3786,19 @@
         <v>189.89</v>
       </c>
       <c r="I26" s="24">
-        <f t="shared" ref="I26:L26" si="1">-22.11+2.12*I23</f>
+        <f t="shared" ref="I26:L26" si="2">-22.11+2.12*I23</f>
         <v>189.89</v>
       </c>
       <c r="J26" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>189.89</v>
       </c>
       <c r="K26" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>189.89</v>
       </c>
       <c r="L26" s="24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>189.89</v>
       </c>
       <c r="M26" s="24">
@@ -3669,19 +3806,19 @@
         <v>83.89</v>
       </c>
       <c r="N26" s="24">
-        <f t="shared" ref="N26:Q26" si="2">-22.11+2.12*N23</f>
+        <f t="shared" ref="N26:Q26" si="3">-22.11+2.12*N23</f>
         <v>136.88999999999999</v>
       </c>
       <c r="O26" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>189.89</v>
       </c>
       <c r="P26" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>242.89</v>
       </c>
       <c r="Q26" s="24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>295.89</v>
       </c>
       <c r="R26" s="24">
@@ -3689,19 +3826,19 @@
         <v>189.89</v>
       </c>
       <c r="S26" s="24">
-        <f t="shared" ref="S26:V26" si="3">-22.11+2.12*S23</f>
+        <f t="shared" ref="S26:V26" si="4">-22.11+2.12*S23</f>
         <v>189.89</v>
       </c>
       <c r="T26" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>189.89</v>
       </c>
       <c r="U26" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>189.89</v>
       </c>
       <c r="V26" s="24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>189.89</v>
       </c>
       <c r="W26" s="24">
@@ -3709,15 +3846,35 @@
         <v>189.89</v>
       </c>
       <c r="X26" s="24">
-        <f t="shared" ref="X26:Y26" si="4">-22.11+2.12*X23</f>
+        <f t="shared" ref="X26:Y26" si="5">-22.11+2.12*X23</f>
         <v>189.89</v>
       </c>
       <c r="Y26" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>189.89</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" s="27" customFormat="1">
+      <c r="AA26" s="24">
+        <f t="shared" ref="AA26:AD26" si="6">-22.11+2.12*AA23</f>
+        <v>189.89</v>
+      </c>
+      <c r="AB26" s="24">
+        <f t="shared" si="6"/>
+        <v>189.89</v>
+      </c>
+      <c r="AC26" s="24">
+        <f>-22.11+2.12*AC23</f>
+        <v>189.89</v>
+      </c>
+      <c r="AD26" s="24">
+        <f t="shared" ref="AD26:AE26" si="7">-22.11+2.12*AD23</f>
+        <v>189.89</v>
+      </c>
+      <c r="AE26" s="24">
+        <f t="shared" si="7"/>
+        <v>189.89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" s="27" customFormat="1">
       <c r="A27" s="29" t="s">
         <v>98</v>
       </c>
@@ -3729,19 +3886,19 @@
         <v>196.76</v>
       </c>
       <c r="D27" s="24">
-        <f t="shared" ref="D27:G27" si="5">-7.24+2.04*D24</f>
+        <f t="shared" ref="D27:G27" si="8">-7.24+2.04*D24</f>
         <v>196.76</v>
       </c>
       <c r="E27" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>196.76</v>
       </c>
       <c r="F27" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>196.76</v>
       </c>
       <c r="G27" s="24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>196.76</v>
       </c>
       <c r="H27" s="24">
@@ -3749,19 +3906,19 @@
         <v>196.76</v>
       </c>
       <c r="I27" s="24">
-        <f t="shared" ref="I27:L27" si="6">-7.24+2.04*I24</f>
+        <f t="shared" ref="I27:L27" si="9">-7.24+2.04*I24</f>
         <v>196.76</v>
       </c>
       <c r="J27" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>196.76</v>
       </c>
       <c r="K27" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>196.76</v>
       </c>
       <c r="L27" s="24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>196.76</v>
       </c>
       <c r="M27" s="24">
@@ -3769,19 +3926,19 @@
         <v>196.76</v>
       </c>
       <c r="N27" s="24">
-        <f t="shared" ref="N27:Q27" si="7">-7.24+2.04*N24</f>
+        <f t="shared" ref="N27:Q27" si="10">-7.24+2.04*N24</f>
         <v>196.76</v>
       </c>
       <c r="O27" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>196.76</v>
       </c>
       <c r="P27" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>196.76</v>
       </c>
       <c r="Q27" s="24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>196.76</v>
       </c>
       <c r="R27" s="24">
@@ -3789,19 +3946,19 @@
         <v>94.76</v>
       </c>
       <c r="S27" s="24">
-        <f t="shared" ref="S27:V27" si="8">-7.24+2.04*S24</f>
+        <f t="shared" ref="S27:V27" si="11">-7.24+2.04*S24</f>
         <v>145.76</v>
       </c>
       <c r="T27" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>196.76</v>
       </c>
       <c r="U27" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>247.76</v>
       </c>
       <c r="V27" s="24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>298.76</v>
       </c>
       <c r="W27" s="24">
@@ -3809,15 +3966,35 @@
         <v>196.76</v>
       </c>
       <c r="X27" s="24">
-        <f t="shared" ref="X27:Y27" si="9">-7.24+2.04*X24</f>
+        <f t="shared" ref="X27:Y27" si="12">-7.24+2.04*X24</f>
         <v>196.76</v>
       </c>
       <c r="Y27" s="24">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>196.76</v>
       </c>
-    </row>
-    <row r="28" spans="1:25" s="27" customFormat="1">
+      <c r="AA27" s="24">
+        <f t="shared" ref="AA27:AD27" si="13">-7.24+2.04*AA24</f>
+        <v>196.76</v>
+      </c>
+      <c r="AB27" s="24">
+        <f t="shared" si="13"/>
+        <v>196.76</v>
+      </c>
+      <c r="AC27" s="24">
+        <f>-7.24+2.04*AC24</f>
+        <v>196.76</v>
+      </c>
+      <c r="AD27" s="24">
+        <f t="shared" ref="AD27:AE27" si="14">-7.24+2.04*AD24</f>
+        <v>196.76</v>
+      </c>
+      <c r="AE27" s="24">
+        <f t="shared" si="14"/>
+        <v>196.76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" s="27" customFormat="1">
       <c r="A28" s="28" t="s">
         <v>96</v>
       </c>
@@ -3840,7 +4017,7 @@
       <c r="X28" s="26"/>
       <c r="Y28" s="26"/>
     </row>
-    <row r="29" spans="1:25" s="27" customFormat="1">
+    <row r="29" spans="1:31" s="27" customFormat="1">
       <c r="A29" s="26" t="s">
         <v>85</v>
       </c>
@@ -3939,8 +4116,28 @@
         <f>ExpData!AJ15</f>
         <v>1.0575562188444444E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:25" s="27" customFormat="1">
+      <c r="AA29" s="58">
+        <f>ExpData!AL15</f>
+        <v>1.0575562188444444E-2</v>
+      </c>
+      <c r="AB29" s="58">
+        <f>ExpData!AM15</f>
+        <v>1.0575562188444444E-2</v>
+      </c>
+      <c r="AC29" s="58">
+        <f>ExpData!AN15</f>
+        <v>1.0575562188444444E-2</v>
+      </c>
+      <c r="AD29" s="58">
+        <f>ExpData!AO15</f>
+        <v>1.0575562188444444E-2</v>
+      </c>
+      <c r="AE29" s="58">
+        <f>ExpData!AP15</f>
+        <v>1.0575562188444444E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" s="27" customFormat="1">
       <c r="A30" s="26" t="s">
         <v>97</v>
       </c>
@@ -4039,8 +4236,28 @@
         <f>ExpData!AJ16</f>
         <v>46.843521688179884</v>
       </c>
-    </row>
-    <row r="31" spans="1:25" s="27" customFormat="1">
+      <c r="AA30" s="58">
+        <f>ExpData!AL16</f>
+        <v>46.813272232415727</v>
+      </c>
+      <c r="AB30" s="58">
+        <f>ExpData!AM16</f>
+        <v>46.848783530878762</v>
+      </c>
+      <c r="AC30" s="58">
+        <f>ExpData!AN16</f>
+        <v>46.810284463894057</v>
+      </c>
+      <c r="AD30" s="58">
+        <f>ExpData!AO16</f>
+        <v>46.866582914572703</v>
+      </c>
+      <c r="AE30" s="58">
+        <f>ExpData!AP16</f>
+        <v>47.081704781703998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" s="27" customFormat="1">
       <c r="A31" s="28" t="s">
         <v>98</v>
       </c>
@@ -4069,7 +4286,7 @@
       <c r="X31" s="41"/>
       <c r="Y31" s="41"/>
     </row>
-    <row r="32" spans="1:25" s="27" customFormat="1">
+    <row r="32" spans="1:31" s="27" customFormat="1">
       <c r="A32" s="26" t="s">
         <v>85</v>
       </c>
@@ -4168,8 +4385,28 @@
         <f>ExpData!AJ18</f>
         <v>1.0878928809055555E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:25" s="27" customFormat="1">
+      <c r="AA32" s="58">
+        <f>ExpData!AL18</f>
+        <v>1.0878928809055555E-2</v>
+      </c>
+      <c r="AB32" s="58">
+        <f>ExpData!AM18</f>
+        <v>1.0878928809055555E-2</v>
+      </c>
+      <c r="AC32" s="58">
+        <f>ExpData!AN18</f>
+        <v>1.0878928809055555E-2</v>
+      </c>
+      <c r="AD32" s="58">
+        <f>ExpData!AO18</f>
+        <v>1.0878928809055555E-2</v>
+      </c>
+      <c r="AE32" s="58">
+        <f>ExpData!AP18</f>
+        <v>1.0878928809055555E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" s="27" customFormat="1">
       <c r="A33" s="26" t="s">
         <v>97</v>
       </c>
@@ -4268,8 +4505,28 @@
         <f>ExpData!AJ19</f>
         <v>19.94308391529044</v>
       </c>
-    </row>
-    <row r="34" spans="1:25">
+      <c r="AA33" s="58">
+        <f>ExpData!AL19</f>
+        <v>19.965192717598594</v>
+      </c>
+      <c r="AB33" s="58">
+        <f>ExpData!AM19</f>
+        <v>19.989925140361731</v>
+      </c>
+      <c r="AC33" s="58">
+        <f>ExpData!AN19</f>
+        <v>19.900375117224076</v>
+      </c>
+      <c r="AD33" s="58">
+        <f>ExpData!AO19</f>
+        <v>19.998618090452187</v>
+      </c>
+      <c r="AE33" s="58">
+        <f>ExpData!AP19</f>
+        <v>19.971794871794781</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31">
       <c r="A34" s="18" t="s">
         <v>70</v>
       </c>
@@ -4297,7 +4554,7 @@
       <c r="X34" s="19"/>
       <c r="Y34" s="19"/>
     </row>
-    <row r="35" spans="1:25" s="25" customFormat="1">
+    <row r="35" spans="1:31" s="25" customFormat="1">
       <c r="A35" s="25" t="s">
         <v>73</v>
       </c>
@@ -4396,8 +4653,28 @@
         <f>ExpData!AJ21</f>
         <v>44.928683240302114</v>
       </c>
-    </row>
-    <row r="36" spans="1:25" s="25" customFormat="1">
+      <c r="AA35" s="58">
+        <f>ExpData!AL21</f>
+        <v>45.115007004655496</v>
+      </c>
+      <c r="AB35" s="58">
+        <f>ExpData!AM21</f>
+        <v>45.433250155957296</v>
+      </c>
+      <c r="AC35" s="58">
+        <f>ExpData!AN21</f>
+        <v>46.127227258519227</v>
+      </c>
+      <c r="AD35" s="58">
+        <f>ExpData!AO21</f>
+        <v>45.261652010050049</v>
+      </c>
+      <c r="AE35" s="58">
+        <f>ExpData!AP21</f>
+        <v>45.950311850311486</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" s="25" customFormat="1">
       <c r="A36" s="25" t="s">
         <v>75</v>
       </c>
@@ -4496,8 +4773,28 @@
         <f>ExpData!AJ22</f>
         <v>21.306892948428231</v>
       </c>
-    </row>
-    <row r="37" spans="1:25" s="25" customFormat="1">
+      <c r="AA36" s="58">
+        <f>ExpData!AL22</f>
+        <v>21.428861307302665</v>
+      </c>
+      <c r="AB36" s="58">
+        <f>ExpData!AM22</f>
+        <v>21.583000623829477</v>
+      </c>
+      <c r="AC36" s="58">
+        <f>ExpData!AN22</f>
+        <v>21.569084088778226</v>
+      </c>
+      <c r="AD36" s="58">
+        <f>ExpData!AO22</f>
+        <v>21.251664572864392</v>
+      </c>
+      <c r="AE36" s="58">
+        <f>ExpData!AP22</f>
+        <v>21.224081774082016</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" s="25" customFormat="1">
       <c r="A37" s="25" t="s">
         <v>71</v>
       </c>
@@ -4596,8 +4893,28 @@
         <f>ExpData!AJ23</f>
         <v>4.8133098240000001</v>
       </c>
-    </row>
-    <row r="38" spans="1:25">
+      <c r="AA37" s="58">
+        <f>ExpData!AL23</f>
+        <v>10.728884735999999</v>
+      </c>
+      <c r="AB37" s="58">
+        <f>ExpData!AM23</f>
+        <v>6.7713711627906985</v>
+      </c>
+      <c r="AC37" s="58">
+        <f>ExpData!AN23</f>
+        <v>5.5270333439999995</v>
+      </c>
+      <c r="AD37" s="58">
+        <f>ExpData!AO23</f>
+        <v>3.0934241280000001</v>
+      </c>
+      <c r="AE37" s="58">
+        <f>ExpData!AP23</f>
+        <v>0.32185294698240002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31">
       <c r="A38" s="18" t="s">
         <v>68</v>
       </c>
@@ -4693,13 +5010,21 @@
         <f>ExpData!AJ24</f>
         <v/>
       </c>
-    </row>
-    <row r="39" spans="1:25">
+      <c r="AA38" s="53" t="str">
+        <f>ExpData!AL24</f>
+        <v>duplicate</v>
+      </c>
+      <c r="AB38" s="53"/>
+      <c r="AC38" s="53"/>
+      <c r="AD38" s="53"/>
+      <c r="AE38" s="53"/>
+    </row>
+    <row r="39" spans="1:31">
       <c r="A39" s="18" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="1:25">
+    <row r="40" spans="1:31">
       <c r="A40" s="18" t="s">
         <v>100</v>
       </c>
@@ -4722,7 +5047,7 @@
       <c r="X40" s="42"/>
       <c r="Y40" s="42"/>
     </row>
-    <row r="41" spans="1:25" s="56" customFormat="1">
+    <row r="41" spans="1:31" s="56" customFormat="1">
       <c r="A41" s="56" t="s">
         <v>87</v>
       </c>
@@ -4730,99 +5055,119 @@
         <v>86</v>
       </c>
       <c r="C41" s="57">
-        <f t="shared" ref="C41:O41" si="10">C26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <f t="shared" ref="C41:Y41" si="15">C26/1000000/60/(MOD1W*MOD1H/10000)</f>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="D41" s="57">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="E41" s="57">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="F41" s="57">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="G41" s="57">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="H41" s="57">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="I41" s="57">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="J41" s="57">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="K41" s="57">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="L41" s="57">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>8.4395555555555543E-3</v>
       </c>
       <c r="M41" s="57">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>3.7284444444444444E-3</v>
       </c>
       <c r="N41" s="57">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>6.084E-3</v>
       </c>
       <c r="O41" s="57">
-        <f t="shared" si="10"/>
+        <f t="shared" si="15"/>
         <v>8.4395555555555543E-3</v>
       </c>
-      <c r="P41" s="57">
-        <f>P29</f>
-        <v>1.321588888888889E-2</v>
-      </c>
-      <c r="Q41" s="57">
-        <f t="shared" ref="Q41:Y41" si="11">Q29</f>
-        <v>1.5861722222222222E-2</v>
-      </c>
-      <c r="R41" s="57">
-        <f t="shared" si="11"/>
-        <v>1.0570055555555555E-2</v>
-      </c>
-      <c r="S41" s="57">
-        <f t="shared" si="11"/>
-        <v>1.0570055555555555E-2</v>
-      </c>
-      <c r="T41" s="57">
-        <f t="shared" si="11"/>
-        <v>1.0570055555555555E-2</v>
-      </c>
-      <c r="U41" s="57">
-        <f t="shared" si="11"/>
-        <v>1.0570055555555555E-2</v>
-      </c>
-      <c r="V41" s="57">
-        <f t="shared" si="11"/>
-        <v>1.0570055555555555E-2</v>
-      </c>
-      <c r="W41" s="57">
-        <f t="shared" si="11"/>
-        <v>1.0575562188444444E-2</v>
-      </c>
-      <c r="X41" s="57">
-        <f t="shared" si="11"/>
-        <v>1.0575562188444444E-2</v>
-      </c>
-      <c r="Y41" s="57">
-        <f t="shared" si="11"/>
-        <v>1.0575562188444444E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:25" s="56" customFormat="1">
+      <c r="P41" s="59">
+        <f t="shared" si="15"/>
+        <v>1.0795111111111109E-2</v>
+      </c>
+      <c r="Q41" s="59">
+        <f t="shared" si="15"/>
+        <v>1.3150666666666666E-2</v>
+      </c>
+      <c r="R41" s="59">
+        <f t="shared" si="15"/>
+        <v>8.4395555555555543E-3</v>
+      </c>
+      <c r="S41" s="59">
+        <f t="shared" si="15"/>
+        <v>8.4395555555555543E-3</v>
+      </c>
+      <c r="T41" s="59">
+        <f t="shared" si="15"/>
+        <v>8.4395555555555543E-3</v>
+      </c>
+      <c r="U41" s="59">
+        <f t="shared" si="15"/>
+        <v>8.4395555555555543E-3</v>
+      </c>
+      <c r="V41" s="59">
+        <f t="shared" si="15"/>
+        <v>8.4395555555555543E-3</v>
+      </c>
+      <c r="W41" s="59">
+        <f t="shared" si="15"/>
+        <v>8.4395555555555543E-3</v>
+      </c>
+      <c r="X41" s="59">
+        <f t="shared" si="15"/>
+        <v>8.4395555555555543E-3</v>
+      </c>
+      <c r="Y41" s="59">
+        <f t="shared" si="15"/>
+        <v>8.4395555555555543E-3</v>
+      </c>
+      <c r="AA41" s="57">
+        <f t="shared" ref="AA41:AE41" si="16">AA26/1000000/60/(MOD1W*MOD1H/10000)</f>
+        <v>8.4395555555555543E-3</v>
+      </c>
+      <c r="AB41" s="57">
+        <f t="shared" si="16"/>
+        <v>8.4395555555555543E-3</v>
+      </c>
+      <c r="AC41" s="57">
+        <f t="shared" si="16"/>
+        <v>8.4395555555555543E-3</v>
+      </c>
+      <c r="AD41" s="57">
+        <f t="shared" si="16"/>
+        <v>8.4395555555555543E-3</v>
+      </c>
+      <c r="AE41" s="57">
+        <f t="shared" si="16"/>
+        <v>8.4395555555555543E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31" s="56" customFormat="1">
       <c r="A42" s="56" t="s">
         <v>102</v>
       </c>
@@ -4830,99 +5175,119 @@
         <v>90</v>
       </c>
       <c r="C42" s="57">
-        <f t="shared" ref="C42:Y42" si="12">C30+273.15</f>
+        <f t="shared" ref="C42:Y42" si="17">C30+273.15</f>
         <v>305.95490858938018</v>
       </c>
       <c r="D42" s="57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>310.69592116787919</v>
       </c>
       <c r="E42" s="57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>313.61279404111355</v>
       </c>
       <c r="F42" s="57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>319.9632722324157</v>
       </c>
       <c r="G42" s="57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>325.43803056208191</v>
       </c>
       <c r="H42" s="57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>319.9632722324157</v>
       </c>
       <c r="I42" s="57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>319.8855595510372</v>
       </c>
       <c r="J42" s="57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>319.90637697413189</v>
       </c>
       <c r="K42" s="57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>319.90971551314635</v>
       </c>
       <c r="L42" s="57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>319.94575411738424</v>
       </c>
       <c r="M42" s="57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>319.91596078453716</v>
       </c>
       <c r="N42" s="57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>319.89779784944972</v>
       </c>
       <c r="O42" s="57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>319.9632722324157</v>
       </c>
       <c r="P42" s="57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>319.93013526515875</v>
       </c>
       <c r="Q42" s="57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>319.93591507034586</v>
       </c>
       <c r="R42" s="57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>319.98130444404444</v>
       </c>
       <c r="S42" s="57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>319.98563639027623</v>
       </c>
       <c r="T42" s="57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>319.9632722324157</v>
       </c>
       <c r="U42" s="57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>319.92324841993519</v>
       </c>
       <c r="V42" s="57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>319.92299838980034</v>
       </c>
       <c r="W42" s="57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>319.9632722324157</v>
       </c>
       <c r="X42" s="57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>319.9883711327808</v>
       </c>
       <c r="Y42" s="57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>319.99352168817984</v>
       </c>
-    </row>
-    <row r="43" spans="1:25" s="56" customFormat="1">
+      <c r="AA42" s="57">
+        <f t="shared" ref="AA42" si="18">AA30+273.15</f>
+        <v>319.9632722324157</v>
+      </c>
+      <c r="AB42" s="57">
+        <f t="shared" ref="AA42:AE42" si="19">AB30+273.15</f>
+        <v>319.99878353087877</v>
+      </c>
+      <c r="AC42" s="57">
+        <f t="shared" si="19"/>
+        <v>319.96028446389403</v>
+      </c>
+      <c r="AD42" s="57">
+        <f t="shared" si="19"/>
+        <v>320.01658291457267</v>
+      </c>
+      <c r="AE42" s="57">
+        <f t="shared" si="19"/>
+        <v>320.23170478170397</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31" s="56" customFormat="1">
       <c r="A43" s="56" t="s">
         <v>101</v>
       </c>
@@ -4930,104 +5295,124 @@
         <v>90</v>
       </c>
       <c r="C43" s="57">
-        <f t="shared" ref="C43:Y43" si="13">C35+273.15</f>
+        <f t="shared" ref="C43:Y43" si="20">C35+273.15</f>
         <v>305.35915961980555</v>
       </c>
       <c r="D43" s="57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>309.79188253593401</v>
       </c>
       <c r="E43" s="57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>312.35623159324001</v>
       </c>
       <c r="F43" s="57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>318.26500700465544</v>
       </c>
       <c r="G43" s="57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>323.63862859035953</v>
       </c>
       <c r="H43" s="57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>318.26500700465544</v>
       </c>
       <c r="I43" s="57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>318.30270436408495</v>
       </c>
       <c r="J43" s="57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>318.4829372796284</v>
       </c>
       <c r="K43" s="57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>318.80301197436296</v>
       </c>
       <c r="L43" s="57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>319.01289994963463</v>
       </c>
       <c r="M43" s="57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>319.56472605071929</v>
       </c>
       <c r="N43" s="57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>318.40305616471557</v>
       </c>
       <c r="O43" s="57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>318.26500700465544</v>
       </c>
       <c r="P43" s="57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>318.70412169546893</v>
       </c>
       <c r="Q43" s="57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>318.81776959447166</v>
       </c>
       <c r="R43" s="57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>318.56053255624283</v>
       </c>
       <c r="S43" s="57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>318.51664490974343</v>
       </c>
       <c r="T43" s="57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>318.26500700465544</v>
       </c>
       <c r="U43" s="57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>318.3348782464065</v>
       </c>
       <c r="V43" s="57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>318.29827050530861</v>
       </c>
       <c r="W43" s="57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>318.26500700465544</v>
       </c>
       <c r="X43" s="57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>318.3938189793015</v>
       </c>
       <c r="Y43" s="57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="20"/>
         <v>318.0786832403021</v>
       </c>
-    </row>
-    <row r="44" spans="1:25" s="56" customFormat="1">
+      <c r="AA43" s="57">
+        <f t="shared" ref="AA43" si="21">AA35+273.15</f>
+        <v>318.26500700465544</v>
+      </c>
+      <c r="AB43" s="57">
+        <f t="shared" ref="AA43:AE43" si="22">AB35+273.15</f>
+        <v>318.58325015595727</v>
+      </c>
+      <c r="AC43" s="57">
+        <f t="shared" si="22"/>
+        <v>319.27722725851919</v>
+      </c>
+      <c r="AD43" s="57">
+        <f t="shared" si="22"/>
+        <v>318.41165201005003</v>
+      </c>
+      <c r="AE43" s="57">
+        <f t="shared" si="22"/>
+        <v>319.10031185031147</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31" s="56" customFormat="1">
       <c r="A44" s="32" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="45" spans="1:25" s="56" customFormat="1">
+    <row r="45" spans="1:31" s="56" customFormat="1">
       <c r="A45" s="56" t="s">
         <v>87</v>
       </c>
@@ -5035,99 +5420,119 @@
         <v>86</v>
       </c>
       <c r="C45" s="57">
-        <f t="shared" ref="C45:O45" si="14">C27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <f t="shared" ref="C45:Y45" si="23">C27/1000000/60/(MOD1H*MOD1W/10000)</f>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="D45" s="57">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="E45" s="57">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="F45" s="57">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="G45" s="57">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="H45" s="57">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="I45" s="57">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="J45" s="57">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="K45" s="57">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="L45" s="57">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="M45" s="57">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="N45" s="57">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>8.7448888888888889E-3</v>
       </c>
       <c r="O45" s="57">
-        <f t="shared" si="14"/>
+        <f t="shared" si="23"/>
         <v>8.7448888888888889E-3</v>
       </c>
-      <c r="P45" s="57">
-        <f>P32</f>
-        <v>1.0024555555555557E-2</v>
-      </c>
-      <c r="Q45" s="57">
-        <f t="shared" ref="Q45:Y45" si="15">Q32</f>
-        <v>1.0024555555555571E-2</v>
-      </c>
-      <c r="R45" s="57">
-        <f t="shared" si="15"/>
-        <v>4.9995555555555557E-3</v>
-      </c>
-      <c r="S45" s="57">
-        <f t="shared" si="15"/>
-        <v>7.5120555555555539E-3</v>
-      </c>
-      <c r="T45" s="57">
-        <f t="shared" si="15"/>
-        <v>1.0024555555555557E-2</v>
-      </c>
-      <c r="U45" s="57">
-        <f t="shared" si="15"/>
-        <v>1.2537055555555556E-2</v>
-      </c>
-      <c r="V45" s="57">
-        <f t="shared" si="15"/>
-        <v>1.5049555555555552E-2</v>
-      </c>
-      <c r="W45" s="57">
-        <f t="shared" si="15"/>
-        <v>1.0878928809055555E-2</v>
-      </c>
-      <c r="X45" s="57">
-        <f t="shared" si="15"/>
-        <v>1.0878928809055555E-2</v>
-      </c>
-      <c r="Y45" s="57">
-        <f t="shared" si="15"/>
-        <v>1.0878928809055555E-2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:25" s="56" customFormat="1">
+      <c r="P45" s="59">
+        <f t="shared" si="23"/>
+        <v>8.7448888888888889E-3</v>
+      </c>
+      <c r="Q45" s="59">
+        <f t="shared" si="23"/>
+        <v>8.7448888888888889E-3</v>
+      </c>
+      <c r="R45" s="59">
+        <f t="shared" si="23"/>
+        <v>4.2115555555555561E-3</v>
+      </c>
+      <c r="S45" s="59">
+        <f t="shared" si="23"/>
+        <v>6.478222222222222E-3</v>
+      </c>
+      <c r="T45" s="59">
+        <f t="shared" si="23"/>
+        <v>8.7448888888888889E-3</v>
+      </c>
+      <c r="U45" s="59">
+        <f t="shared" si="23"/>
+        <v>1.1011555555555554E-2</v>
+      </c>
+      <c r="V45" s="59">
+        <f t="shared" si="23"/>
+        <v>1.3278222222222219E-2</v>
+      </c>
+      <c r="W45" s="59">
+        <f t="shared" si="23"/>
+        <v>8.7448888888888889E-3</v>
+      </c>
+      <c r="X45" s="59">
+        <f t="shared" si="23"/>
+        <v>8.7448888888888889E-3</v>
+      </c>
+      <c r="Y45" s="59">
+        <f t="shared" si="23"/>
+        <v>8.7448888888888889E-3</v>
+      </c>
+      <c r="AA45" s="57">
+        <f t="shared" ref="AA45:AE45" si="24">AA27/1000000/60/(MOD1H*MOD1W/10000)</f>
+        <v>8.7448888888888889E-3</v>
+      </c>
+      <c r="AB45" s="57">
+        <f t="shared" si="24"/>
+        <v>8.7448888888888889E-3</v>
+      </c>
+      <c r="AC45" s="57">
+        <f t="shared" si="24"/>
+        <v>8.7448888888888889E-3</v>
+      </c>
+      <c r="AD45" s="57">
+        <f t="shared" si="24"/>
+        <v>8.7448888888888889E-3</v>
+      </c>
+      <c r="AE45" s="57">
+        <f t="shared" si="24"/>
+        <v>8.7448888888888889E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31" s="56" customFormat="1">
       <c r="A46" s="56" t="s">
         <v>102</v>
       </c>
@@ -5135,99 +5540,119 @@
         <v>90</v>
       </c>
       <c r="C46" s="57">
-        <f t="shared" ref="C46:Y46" si="16">C33+273.15</f>
+        <f t="shared" ref="C46:Y46" si="25">C33+273.15</f>
         <v>293.17058482349387</v>
       </c>
       <c r="D46" s="57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>293.16399690708016</v>
       </c>
       <c r="E46" s="57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>293.19055520526842</v>
       </c>
       <c r="F46" s="57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>293.11519271759857</v>
       </c>
       <c r="G46" s="57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>293.68159105444261</v>
       </c>
       <c r="H46" s="57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>293.11519271759857</v>
       </c>
       <c r="I46" s="57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>298.17047781625797</v>
       </c>
       <c r="J46" s="57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>303.14666093734934</v>
       </c>
       <c r="K46" s="57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>308.13104480298307</v>
       </c>
       <c r="L46" s="57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>313.1456119665342</v>
       </c>
       <c r="M46" s="57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>293.10147626262693</v>
       </c>
       <c r="N46" s="57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>293.13472615642195</v>
       </c>
       <c r="O46" s="57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>293.11519271759857</v>
       </c>
       <c r="P46" s="57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>293.13426554012835</v>
       </c>
       <c r="Q46" s="57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>293.18355233922148</v>
       </c>
       <c r="R46" s="57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>293.14611427063818</v>
       </c>
       <c r="S46" s="57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>293.13525638330668</v>
       </c>
       <c r="T46" s="57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>293.11519271759857</v>
       </c>
       <c r="U46" s="57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>293.12888473278991</v>
       </c>
       <c r="V46" s="57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>293.09014458415839</v>
       </c>
       <c r="W46" s="57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>293.11519271759857</v>
       </c>
       <c r="X46" s="57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>293.11284038778177</v>
       </c>
       <c r="Y46" s="57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>293.09308391529044</v>
       </c>
-    </row>
-    <row r="47" spans="1:25" s="56" customFormat="1">
+      <c r="AA46" s="57">
+        <f t="shared" ref="AA46" si="26">AA33+273.15</f>
+        <v>293.11519271759857</v>
+      </c>
+      <c r="AB46" s="57">
+        <f t="shared" ref="AA46:AE46" si="27">AB33+273.15</f>
+        <v>293.1399251403617</v>
+      </c>
+      <c r="AC46" s="57">
+        <f t="shared" si="27"/>
+        <v>293.05037511722406</v>
+      </c>
+      <c r="AD46" s="57">
+        <f t="shared" si="27"/>
+        <v>293.14861809045215</v>
+      </c>
+      <c r="AE46" s="57">
+        <f t="shared" si="27"/>
+        <v>293.12179487179475</v>
+      </c>
+    </row>
+    <row r="47" spans="1:31" s="56" customFormat="1">
       <c r="A47" s="56" t="s">
         <v>101</v>
       </c>
@@ -5235,99 +5660,119 @@
         <v>90</v>
       </c>
       <c r="C47" s="57">
-        <f t="shared" ref="C47:Y47" si="17">C36+273.15</f>
+        <f t="shared" ref="C47:Y47" si="28">C36+273.15</f>
         <v>294.29682689366177</v>
       </c>
       <c r="D47" s="57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="28"/>
         <v>294.21664608339694</v>
       </c>
       <c r="E47" s="57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="28"/>
         <v>294.35225488233681</v>
       </c>
       <c r="F47" s="57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="28"/>
         <v>294.57886130730265</v>
       </c>
       <c r="G47" s="57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="28"/>
         <v>295.14325006184663</v>
       </c>
       <c r="H47" s="57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="28"/>
         <v>294.57886130730265</v>
       </c>
       <c r="I47" s="57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="28"/>
         <v>299.22168943939931</v>
       </c>
       <c r="J47" s="57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="28"/>
         <v>303.91148736331343</v>
       </c>
       <c r="K47" s="57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="28"/>
         <v>308.65229050926581</v>
       </c>
       <c r="L47" s="57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="28"/>
         <v>313.57345483397432</v>
       </c>
       <c r="M47" s="57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="28"/>
         <v>294.64494411853934</v>
       </c>
       <c r="N47" s="57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="28"/>
         <v>294.66788302030187</v>
       </c>
       <c r="O47" s="57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="28"/>
         <v>294.57886130730265</v>
       </c>
       <c r="P47" s="57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="28"/>
         <v>294.74539495317856</v>
       </c>
       <c r="Q47" s="57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="28"/>
         <v>294.95517646294218</v>
       </c>
       <c r="R47" s="57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="28"/>
         <v>294.88340227697375</v>
       </c>
       <c r="S47" s="57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="28"/>
         <v>295.00451737531392</v>
       </c>
       <c r="T47" s="57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="28"/>
         <v>294.57886130730265</v>
       </c>
       <c r="U47" s="57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="28"/>
         <v>294.62908105804513</v>
       </c>
       <c r="V47" s="57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="28"/>
         <v>294.46046760050325</v>
       </c>
       <c r="W47" s="57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="28"/>
         <v>294.57886130730265</v>
       </c>
       <c r="X47" s="57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="28"/>
         <v>294.62831839055224</v>
       </c>
       <c r="Y47" s="57">
-        <f t="shared" si="17"/>
+        <f t="shared" si="28"/>
         <v>294.45689294842822</v>
       </c>
-    </row>
-    <row r="48" spans="1:25" s="56" customFormat="1">
+      <c r="AA47" s="57">
+        <f t="shared" ref="AA47" si="29">AA36+273.15</f>
+        <v>294.57886130730265</v>
+      </c>
+      <c r="AB47" s="57">
+        <f t="shared" ref="AA47:AE47" si="30">AB36+273.15</f>
+        <v>294.73300062382947</v>
+      </c>
+      <c r="AC47" s="57">
+        <f t="shared" si="30"/>
+        <v>294.71908408877823</v>
+      </c>
+      <c r="AD47" s="57">
+        <f t="shared" si="30"/>
+        <v>294.40166457286438</v>
+      </c>
+      <c r="AE47" s="57">
+        <f t="shared" si="30"/>
+        <v>294.37408177408201</v>
+      </c>
+    </row>
+    <row r="48" spans="1:31" s="56" customFormat="1">
       <c r="A48" s="32" t="s">
         <v>71</v>
       </c>
@@ -5335,99 +5780,119 @@
         <v>89</v>
       </c>
       <c r="C48" s="57">
-        <f t="shared" ref="C48:Y48" si="18">C37/3600</f>
+        <f t="shared" ref="C48:Y48" si="31">C37/3600</f>
         <v>1.0791274666666665E-3</v>
       </c>
       <c r="D48" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="31"/>
         <v>1.5744281599999997E-3</v>
       </c>
       <c r="E48" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="31"/>
         <v>1.9465498666666667E-3</v>
       </c>
       <c r="F48" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="31"/>
         <v>2.9802457599999999E-3</v>
       </c>
       <c r="G48" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="31"/>
         <v>3.9183833599999995E-3</v>
       </c>
       <c r="H48" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="31"/>
         <v>2.9802457599999999E-3</v>
       </c>
       <c r="I48" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="31"/>
         <v>2.5700625066666666E-3</v>
       </c>
       <c r="J48" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="31"/>
         <v>2.1235246933333334E-3</v>
       </c>
       <c r="K48" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="31"/>
         <v>1.5609421866666663E-3</v>
       </c>
       <c r="L48" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="31"/>
         <v>9.935384533333333E-4</v>
       </c>
       <c r="M48" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="31"/>
         <v>2.9378886400000001E-3</v>
       </c>
       <c r="N48" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="31"/>
         <v>2.8567750399999996E-3</v>
       </c>
       <c r="O48" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="31"/>
         <v>2.9802457599999999E-3</v>
       </c>
       <c r="P48" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="31"/>
         <v>3.0446920533333329E-3</v>
       </c>
       <c r="Q48" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="31"/>
         <v>3.1019777066666663E-3</v>
       </c>
       <c r="R48" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="31"/>
         <v>2.7461594666666673E-3</v>
       </c>
       <c r="S48" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="31"/>
         <v>2.8241684266666666E-3</v>
       </c>
       <c r="T48" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="31"/>
         <v>2.9802457599999999E-3</v>
       </c>
       <c r="U48" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="31"/>
         <v>3.2108769066666668E-3</v>
       </c>
       <c r="V48" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="31"/>
         <v>3.3036054400000002E-3</v>
       </c>
       <c r="W48" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="31"/>
         <v>2.9802457599999999E-3</v>
       </c>
       <c r="X48" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="31"/>
         <v>9.7313013333333309E-4</v>
       </c>
       <c r="Y48" s="57">
-        <f t="shared" si="18"/>
+        <f t="shared" si="31"/>
         <v>1.3370305066666666E-3</v>
       </c>
-    </row>
-    <row r="49" spans="1:25" customFormat="1">
+      <c r="AA48" s="57">
+        <f t="shared" ref="AA48" si="32">AA37/3600</f>
+        <v>2.9802457599999999E-3</v>
+      </c>
+      <c r="AB48" s="57">
+        <f t="shared" ref="AA48:AE48" si="33">AB37/3600</f>
+        <v>1.8809364341085273E-3</v>
+      </c>
+      <c r="AC48" s="57">
+        <f t="shared" si="33"/>
+        <v>1.5352870399999998E-3</v>
+      </c>
+      <c r="AD48" s="57">
+        <f t="shared" si="33"/>
+        <v>8.5928448000000001E-4</v>
+      </c>
+      <c r="AE48" s="57">
+        <f t="shared" si="33"/>
+        <v>8.9403596384000003E-5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:31" customFormat="1">
       <c r="A49" s="18" t="s">
         <v>88</v>
       </c>
@@ -5437,7 +5902,7 @@
       <c r="K49" s="35"/>
       <c r="L49" s="35"/>
     </row>
-    <row r="50" spans="1:25" s="35" customFormat="1">
+    <row r="50" spans="1:31" s="35" customFormat="1" hidden="1">
       <c r="A50" s="36" t="s">
         <v>136</v>
       </c>
@@ -5457,7 +5922,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:25" s="35" customFormat="1">
+    <row r="51" spans="1:31" s="35" customFormat="1" hidden="1">
       <c r="A51" s="36" t="s">
         <v>104</v>
       </c>
@@ -5477,7 +5942,7 @@
         <v>317.02</v>
       </c>
     </row>
-    <row r="52" spans="1:25" s="35" customFormat="1">
+    <row r="52" spans="1:31" s="35" customFormat="1" hidden="1">
       <c r="A52" s="36" t="s">
         <v>105</v>
       </c>
@@ -5497,7 +5962,7 @@
         <v>296.02</v>
       </c>
     </row>
-    <row r="53" spans="1:25" s="35" customFormat="1">
+    <row r="53" spans="1:31" s="35" customFormat="1" hidden="1">
       <c r="A53" s="35" t="s">
         <v>71</v>
       </c>
@@ -5523,7 +5988,7 @@
       <c r="K53" s="27"/>
       <c r="L53" s="27"/>
     </row>
-    <row r="54" spans="1:25" s="27" customFormat="1">
+    <row r="54" spans="1:31" s="27" customFormat="1" hidden="1">
       <c r="E54" s="38"/>
       <c r="H54" s="39"/>
       <c r="I54" s="39"/>
@@ -5531,7 +5996,7 @@
       <c r="K54" s="39"/>
       <c r="L54" s="39"/>
     </row>
-    <row r="55" spans="1:25" s="39" customFormat="1">
+    <row r="55" spans="1:31" s="39" customFormat="1">
       <c r="A55" s="39" t="s">
         <v>136</v>
       </c>
@@ -5595,8 +6060,26 @@
       <c r="Y55" s="39">
         <v>19</v>
       </c>
-    </row>
-    <row r="56" spans="1:25" s="39" customFormat="1">
+      <c r="Z55" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA55" s="39">
+        <v>20</v>
+      </c>
+      <c r="AB55" s="39">
+        <v>21</v>
+      </c>
+      <c r="AC55" s="39">
+        <v>22</v>
+      </c>
+      <c r="AD55" s="39">
+        <v>23</v>
+      </c>
+      <c r="AE55" s="39">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:31" s="39" customFormat="1">
       <c r="A56" s="39" t="s">
         <v>108</v>
       </c>
@@ -5661,8 +6144,23 @@
       <c r="Y56" s="39">
         <v>318.00878999999998</v>
       </c>
-    </row>
-    <row r="57" spans="1:25" s="39" customFormat="1">
+      <c r="AA56" s="39">
+        <v>317.47500000000002</v>
+      </c>
+      <c r="AB56" s="39">
+        <v>317.59199999999998</v>
+      </c>
+      <c r="AC56" s="39">
+        <v>317.73099999999999</v>
+      </c>
+      <c r="AD56" s="39">
+        <v>317.86700000000002</v>
+      </c>
+      <c r="AE56" s="39">
+        <v>317.99400000000003</v>
+      </c>
+    </row>
+    <row r="57" spans="1:31" s="39" customFormat="1">
       <c r="A57" s="39" t="s">
         <v>109</v>
       </c>
@@ -5727,8 +6225,23 @@
       <c r="Y57" s="39">
         <v>295.12842000000001</v>
       </c>
-    </row>
-    <row r="58" spans="1:25" s="39" customFormat="1">
+      <c r="AA57" s="39">
+        <v>295.42500000000001</v>
+      </c>
+      <c r="AB57" s="39">
+        <v>295.40800000000002</v>
+      </c>
+      <c r="AC57" s="39">
+        <v>295.36700000000002</v>
+      </c>
+      <c r="AD57" s="39">
+        <v>295.315</v>
+      </c>
+      <c r="AE57" s="39">
+        <v>295.26</v>
+      </c>
+    </row>
+    <row r="58" spans="1:31" s="39" customFormat="1">
       <c r="A58" s="39" t="s">
         <v>117</v>
       </c>
@@ -5793,8 +6306,23 @@
       <c r="Y58" s="39">
         <v>6.2292604000000003</v>
       </c>
-    </row>
-    <row r="59" spans="1:25" s="39" customFormat="1">
+      <c r="AA58" s="39">
+        <v>6.1228699999999998</v>
+      </c>
+      <c r="AB58" s="39">
+        <v>5.88544</v>
+      </c>
+      <c r="AC58" s="39">
+        <v>5.5725600000000002</v>
+      </c>
+      <c r="AD58" s="39">
+        <v>5.2153600000000004</v>
+      </c>
+      <c r="AE58" s="39">
+        <v>4.8068</v>
+      </c>
+    </row>
+    <row r="59" spans="1:31" s="39" customFormat="1">
       <c r="A59" s="39" t="s">
         <v>71</v>
       </c>
@@ -5823,66 +6351,86 @@
       </c>
       <c r="H59" s="17"/>
       <c r="I59" s="24">
-        <f t="shared" ref="I59:N59" si="19">I58*0.0005</f>
+        <f t="shared" ref="I59:N59" si="34">I58*0.0005</f>
         <v>2.51885E-3</v>
       </c>
       <c r="J59" s="24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="34"/>
         <v>2.0999450000000002E-3</v>
       </c>
       <c r="K59" s="24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="34"/>
         <v>1.4890823500000002E-3</v>
       </c>
       <c r="L59" s="24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="34"/>
         <v>1.0682052500000001E-3</v>
       </c>
       <c r="M59" s="24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="34"/>
         <v>2.8806469500000003E-3</v>
       </c>
       <c r="N59" s="24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="34"/>
         <v>2.8756708999999997E-3</v>
       </c>
       <c r="O59" s="24"/>
       <c r="P59" s="24">
-        <f t="shared" ref="P59:Q59" si="20">P58*0.0005</f>
+        <f t="shared" ref="P59:Q59" si="35">P58*0.0005</f>
         <v>3.2439937500000002E-3</v>
       </c>
       <c r="Q59" s="24">
-        <f t="shared" si="20"/>
+        <f t="shared" si="35"/>
         <v>3.3747971000000002E-3</v>
       </c>
       <c r="R59" s="24">
-        <f t="shared" ref="R59:S59" si="21">R58*0.0005</f>
+        <f t="shared" ref="R59:S59" si="36">R58*0.0005</f>
         <v>2.8682699E-3</v>
       </c>
       <c r="S59" s="24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="36"/>
         <v>3.0008037E-3</v>
       </c>
       <c r="T59" s="24"/>
       <c r="U59" s="24">
-        <f t="shared" ref="U59" si="22">U58*0.0005</f>
+        <f t="shared" ref="U59" si="37">U58*0.0005</f>
         <v>3.13639785E-3</v>
       </c>
       <c r="V59" s="24">
-        <f t="shared" ref="V59:X59" si="23">V58*0.0005</f>
+        <f t="shared" ref="V59:X59" si="38">V58*0.0005</f>
         <v>3.1832208500000001E-3</v>
       </c>
       <c r="W59" s="24"/>
       <c r="X59" s="24">
-        <f t="shared" si="23"/>
+        <f t="shared" si="38"/>
         <v>3.1122703500000002E-3</v>
       </c>
       <c r="Y59" s="24">
-        <f t="shared" ref="Y59" si="24">Y58*0.0005</f>
+        <f t="shared" ref="Y59:AA59" si="39">Y58*0.0005</f>
         <v>3.1146302000000002E-3</v>
       </c>
-    </row>
-    <row r="60" spans="1:25">
+      <c r="AA59" s="24">
+        <f t="shared" si="39"/>
+        <v>3.0614349999999999E-3</v>
+      </c>
+      <c r="AB59" s="24">
+        <f t="shared" ref="AB59:AD59" si="40">AB58*0.0005</f>
+        <v>2.9427200000000002E-3</v>
+      </c>
+      <c r="AC59" s="24">
+        <f t="shared" si="40"/>
+        <v>2.7862800000000004E-3</v>
+      </c>
+      <c r="AD59" s="24">
+        <f t="shared" si="40"/>
+        <v>2.6076800000000002E-3</v>
+      </c>
+      <c r="AE59" s="24">
+        <f t="shared" ref="AE59" si="41">AE58*0.0005</f>
+        <v>2.4034E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:31">
       <c r="A60" s="39" t="s">
         <v>121</v>
       </c>
@@ -5895,78 +6443,98 @@
         <v>1.2004269863037987E-3</v>
       </c>
       <c r="E60" s="24">
-        <f t="shared" ref="E60:G60" si="25">(E43-E56)/E43</f>
+        <f t="shared" ref="E60:G60" si="42">(E43-E56)/E43</f>
         <v>9.4837740783661011E-4</v>
       </c>
       <c r="F60" s="24">
-        <f t="shared" si="25"/>
+        <f t="shared" si="42"/>
         <v>1.5239093019371039E-3</v>
       </c>
       <c r="G60" s="24">
-        <f t="shared" si="25"/>
+        <f t="shared" si="42"/>
         <v>2.7766419425072604E-3</v>
       </c>
       <c r="I60" s="24">
-        <f t="shared" ref="I60:J60" si="26">(I43-I56)/I43</f>
+        <f t="shared" ref="I60:J60" si="43">(I43-I56)/I43</f>
         <v>5.4257900331065141E-4</v>
       </c>
       <c r="J60" s="24">
-        <f t="shared" si="26"/>
+        <f t="shared" si="43"/>
         <v>-3.047658414628378E-4</v>
       </c>
       <c r="K60" s="24">
-        <f t="shared" ref="K60:L60" si="27">(K43-K56)/K43</f>
+        <f t="shared" ref="K60:L60" si="44">(K43-K56)/K43</f>
         <v>-6.289088186317677E-4</v>
       </c>
       <c r="L60" s="24">
-        <f t="shared" si="27"/>
+        <f t="shared" si="44"/>
         <v>-8.3745845515194241E-4</v>
       </c>
       <c r="M60" s="24">
-        <f t="shared" ref="M60:N60" si="28">(M43-M56)/M43</f>
+        <f t="shared" ref="M60:N60" si="45">(M43-M56)/M43</f>
         <v>5.727340665342434E-3</v>
       </c>
       <c r="N60" s="24">
-        <f t="shared" si="28"/>
+        <f t="shared" si="45"/>
         <v>2.1438115982229866E-3</v>
       </c>
       <c r="O60" s="24"/>
       <c r="P60" s="24">
-        <f t="shared" ref="P60" si="29">(P43-P56)/P43</f>
+        <f t="shared" ref="P60" si="46">(P43-P56)/P43</f>
         <v>1.3842986815541562E-3</v>
       </c>
       <c r="Q60" s="24">
-        <f t="shared" ref="Q60:R60" si="30">(Q43-Q56)/Q43</f>
+        <f t="shared" ref="Q60:R60" si="47">(Q43-Q56)/Q43</f>
         <v>1.0586285541768043E-3</v>
       </c>
       <c r="R60" s="24">
-        <f t="shared" si="30"/>
+        <f t="shared" si="47"/>
         <v>4.606426134000754E-4</v>
       </c>
       <c r="S60" s="24">
-        <f t="shared" ref="S60:U60" si="31">(S43-S56)/S43</f>
+        <f t="shared" ref="S60:U60" si="48">(S43-S56)/S43</f>
         <v>1.0571344233480612E-3</v>
       </c>
       <c r="T60" s="24"/>
       <c r="U60" s="24">
-        <f t="shared" si="31"/>
+        <f t="shared" si="48"/>
         <v>1.3903856493660976E-3</v>
       </c>
       <c r="V60" s="24">
-        <f t="shared" ref="V60:X60" si="32">(V43-V56)/V43</f>
+        <f t="shared" ref="V60:X60" si="49">(V43-V56)/V43</f>
         <v>1.458162196645917E-3</v>
       </c>
       <c r="W60" s="24"/>
       <c r="X60" s="24">
-        <f t="shared" si="32"/>
+        <f t="shared" si="49"/>
         <v>1.2226964095895161E-3</v>
       </c>
       <c r="Y60" s="24">
-        <f t="shared" ref="Y60" si="33">(Y43-Y56)/Y43</f>
+        <f t="shared" ref="Y60:AA60" si="50">(Y43-Y56)/Y43</f>
         <v>2.1973569429460568E-4</v>
       </c>
-    </row>
-    <row r="61" spans="1:25">
+      <c r="AA60" s="24">
+        <f t="shared" si="50"/>
+        <v>2.4822301769539686E-3</v>
+      </c>
+      <c r="AB60" s="24">
+        <f t="shared" ref="AB60:AD60" si="51">(AB43-AB56)/AB43</f>
+        <v>3.1114321153796953E-3</v>
+      </c>
+      <c r="AC60" s="24">
+        <f t="shared" si="51"/>
+        <v>4.8428986677061473E-3</v>
+      </c>
+      <c r="AD60" s="24">
+        <f t="shared" si="51"/>
+        <v>1.7105278861868545E-3</v>
+      </c>
+      <c r="AE60" s="24">
+        <f t="shared" ref="AE60" si="52">(AE43-AE56)/AE43</f>
+        <v>3.4669720123319979E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:31">
       <c r="A61" s="39" t="s">
         <v>122</v>
       </c>
@@ -5979,78 +6547,98 @@
         <v>-7.9313634938556589E-4</v>
       </c>
       <c r="E61" s="24">
-        <f t="shared" ref="E61:G61" si="34">(E47-E57)/E47</f>
+        <f t="shared" ref="E61:G61" si="53">(E47-E57)/E47</f>
         <v>-1.3512555486357143E-3</v>
       </c>
       <c r="F61" s="24">
-        <f t="shared" si="34"/>
+        <f t="shared" si="53"/>
         <v>-2.5838197938558632E-3</v>
       </c>
       <c r="G61" s="24">
-        <f t="shared" si="34"/>
+        <f t="shared" si="53"/>
         <v>-4.4952745416857081E-3</v>
       </c>
       <c r="I61" s="24">
-        <f t="shared" ref="I61:J61" si="35">(I47-I57)/I47</f>
+        <f t="shared" ref="I61:J61" si="54">(I47-I57)/I47</f>
         <v>-2.4340166047628E-3</v>
       </c>
       <c r="J61" s="24">
-        <f t="shared" si="35"/>
+        <f t="shared" si="54"/>
         <v>-1.9035563338051613E-3</v>
       </c>
       <c r="K61" s="24">
-        <f t="shared" ref="K61:L61" si="36">(K47-K57)/K47</f>
+        <f t="shared" ref="K61:L61" si="55">(K47-K57)/K47</f>
         <v>-1.2512121329052266E-3</v>
       </c>
       <c r="L61" s="24">
-        <f t="shared" si="36"/>
+        <f t="shared" si="55"/>
         <v>-5.7847742922529646E-4</v>
       </c>
       <c r="M61" s="24">
-        <f t="shared" ref="M61:N61" si="37">(M47-M57)/M47</f>
+        <f t="shared" ref="M61:N61" si="56">(M47-M57)/M47</f>
         <v>-2.3153490160897345E-3</v>
       </c>
       <c r="N61" s="24">
-        <f t="shared" si="37"/>
+        <f t="shared" si="56"/>
         <v>-2.3381814558007786E-3</v>
       </c>
       <c r="O61" s="24"/>
       <c r="P61" s="24">
-        <f t="shared" ref="P61" si="38">(P47-P57)/P47</f>
+        <f t="shared" ref="P61" si="57">(P47-P57)/P47</f>
         <v>-2.2733011551473695E-3</v>
       </c>
       <c r="Q61" s="24">
-        <f t="shared" ref="Q61:R61" si="39">(Q47-Q57)/Q47</f>
+        <f t="shared" ref="Q61:R61" si="58">(Q47-Q57)/Q47</f>
         <v>-2.0176405926973472E-3</v>
       </c>
       <c r="R61" s="24">
-        <f t="shared" si="39"/>
+        <f t="shared" si="58"/>
         <v>-5.5541875547402255E-3</v>
       </c>
       <c r="S61" s="24">
-        <f t="shared" ref="S61:U61" si="40">(S47-S57)/S47</f>
+        <f t="shared" ref="S61:U61" si="59">(S47-S57)/S47</f>
         <v>-2.601901257361215E-3</v>
       </c>
       <c r="T61" s="24"/>
       <c r="U61" s="24">
-        <f t="shared" si="40"/>
+        <f t="shared" si="59"/>
         <v>-1.076129147931664E-3</v>
       </c>
       <c r="V61" s="24">
-        <f t="shared" ref="V61:X61" si="41">(V47-V57)/V47</f>
+        <f t="shared" ref="V61:X61" si="60">(V47-V57)/V47</f>
         <v>-6.877744953237417E-4</v>
       </c>
       <c r="W61" s="24"/>
       <c r="X61" s="24">
-        <f t="shared" si="41"/>
+        <f t="shared" si="60"/>
         <v>-1.7589334666764701E-3</v>
       </c>
       <c r="Y61" s="24">
-        <f t="shared" ref="Y61" si="42">(Y47-Y57)/Y47</f>
+        <f t="shared" ref="Y61:AA61" si="61">(Y47-Y57)/Y47</f>
         <v>-2.2805614935609564E-3</v>
       </c>
-    </row>
-    <row r="62" spans="1:25">
+      <c r="AA61" s="24">
+        <f t="shared" si="61"/>
+        <v>-2.8723673142815225E-3</v>
+      </c>
+      <c r="AB61" s="24">
+        <f t="shared" ref="AB61:AD61" si="62">(AB47-AB57)/AB47</f>
+        <v>-2.290206304492027E-3</v>
+      </c>
+      <c r="AC61" s="24">
+        <f t="shared" si="62"/>
+        <v>-2.198418582987369E-3</v>
+      </c>
+      <c r="AD61" s="24">
+        <f t="shared" si="62"/>
+        <v>-3.1023446435357051E-3</v>
+      </c>
+      <c r="AE61" s="24">
+        <f t="shared" ref="AE61" si="63">(AE47-AE57)/AE47</f>
+        <v>-3.0094980528818289E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:31">
       <c r="A62" s="39" t="s">
         <v>123</v>
       </c>
@@ -6063,28 +6651,28 @@
         <v>-6.5537445671729399E-4</v>
       </c>
       <c r="E62" s="55">
-        <f t="shared" ref="E62:G62" si="43">(E48-E59)/E48</f>
+        <f t="shared" ref="E62:G62" si="64">(E48-E59)/E48</f>
         <v>4.4822209880538222E-3</v>
       </c>
       <c r="F62" s="55">
-        <f t="shared" si="43"/>
+        <f t="shared" si="64"/>
         <v>3.1125204922697346E-2</v>
       </c>
       <c r="G62" s="55">
-        <f t="shared" si="43"/>
+        <f t="shared" si="64"/>
         <v>1.7975106958396075E-2</v>
       </c>
       <c r="H62" s="19"/>
       <c r="I62" s="55">
-        <f t="shared" ref="I62:J62" si="44">(I48-I59)/I48</f>
+        <f t="shared" ref="I62:J62" si="65">(I48-I59)/I48</f>
         <v>1.9926560748551023E-2</v>
       </c>
       <c r="J62" s="55">
-        <f t="shared" si="44"/>
+        <f t="shared" si="65"/>
         <v>1.1104035383887956E-2</v>
       </c>
       <c r="K62" s="55">
-        <f t="shared" ref="K62" si="45">(K48-K59)/K48</f>
+        <f t="shared" ref="K62" si="66">(K48-K59)/K48</f>
         <v>4.6036193576214461E-2</v>
       </c>
       <c r="L62" s="55">
@@ -6101,41 +6689,61 @@
       </c>
       <c r="O62" s="55"/>
       <c r="P62" s="55">
-        <f t="shared" ref="P62" si="46">(P48-P59)/P48</f>
+        <f t="shared" ref="P62" si="67">(P48-P59)/P48</f>
         <v>-6.545873709903488E-2</v>
       </c>
       <c r="Q62" s="55">
-        <f t="shared" ref="Q62:R62" si="47">(Q48-Q59)/Q48</f>
+        <f t="shared" ref="Q62:R62" si="68">(Q48-Q59)/Q48</f>
         <v>-8.7950146368556942E-2</v>
       </c>
       <c r="R62" s="55">
-        <f t="shared" si="47"/>
+        <f t="shared" si="68"/>
         <v>-4.446589311929227E-2</v>
       </c>
       <c r="S62" s="55">
-        <f t="shared" ref="S62:U62" si="48">(S48-S59)/S48</f>
+        <f t="shared" ref="S62:U62" si="69">(S48-S59)/S48</f>
         <v>-6.2544171114402705E-2</v>
       </c>
       <c r="T62" s="55"/>
       <c r="U62" s="55">
-        <f t="shared" si="48"/>
+        <f t="shared" si="69"/>
         <v>2.3195861701215525E-2</v>
       </c>
       <c r="V62" s="55">
-        <f t="shared" ref="V62:X62" si="49">(V48-V59)/V48</f>
+        <f t="shared" ref="V62:X62" si="70">(V48-V59)/V48</f>
         <v>3.6440365590389663E-2</v>
       </c>
       <c r="W62" s="55"/>
       <c r="X62" s="55">
-        <f t="shared" si="49"/>
+        <f t="shared" si="70"/>
         <v>-2.1982057110278923</v>
       </c>
       <c r="Y62" s="55">
-        <f t="shared" ref="Y62" si="50">(Y48-Y59)/Y48</f>
+        <f t="shared" ref="Y62:AA62" si="71">(Y48-Y59)/Y48</f>
         <v>-1.3295131894671905</v>
       </c>
-    </row>
-    <row r="63" spans="1:25">
+      <c r="AA62" s="55">
+        <f t="shared" si="71"/>
+        <v>-2.7242464728814877E-2</v>
+      </c>
+      <c r="AB62" s="55">
+        <f t="shared" ref="AB62:AD62" si="72">(AB48-AB59)/AB48</f>
+        <v>-0.5644973145489135</v>
+      </c>
+      <c r="AC62" s="55">
+        <f t="shared" si="72"/>
+        <v>-0.81482675708641472</v>
+      </c>
+      <c r="AD62" s="55">
+        <f t="shared" si="72"/>
+        <v>-2.0347109260020622</v>
+      </c>
+      <c r="AE62" s="55">
+        <f t="shared" ref="AE62" si="73">(AE48-AE59)/AE48</f>
+        <v>-25.882587470833794</v>
+      </c>
+    </row>
+    <row r="63" spans="1:31">
       <c r="A63" s="39" t="s">
         <v>120</v>
       </c>
@@ -6148,84 +6756,105 @@
         <v>1.5810141987599514E-3</v>
       </c>
       <c r="E63" s="24">
-        <f t="shared" ref="E63:G63" si="51">SQRT(E60^2+E61^2+E62^2)</f>
+        <f t="shared" ref="E63:G63" si="74">SQRT(E60^2+E61^2+E62^2)</f>
         <v>4.7765695065772754E-3</v>
       </c>
       <c r="F63" s="24">
-        <f t="shared" si="51"/>
+        <f t="shared" si="74"/>
         <v>3.1269422856323316E-2</v>
       </c>
       <c r="G63" s="24">
-        <f t="shared" si="51"/>
+        <f t="shared" si="74"/>
         <v>1.8735573219087726E-2</v>
       </c>
       <c r="I63" s="24">
-        <f t="shared" ref="I63:J63" si="52">SQRT(I60^2+I61^2+I62^2)</f>
+        <f t="shared" ref="I63:J63" si="75">SQRT(I60^2+I61^2+I62^2)</f>
         <v>2.0081998209162077E-2</v>
       </c>
       <c r="J63" s="24">
-        <f t="shared" si="52"/>
+        <f t="shared" si="75"/>
         <v>1.1270138008947718E-2</v>
       </c>
       <c r="K63" s="24">
-        <f t="shared" ref="K63:L63" si="53">SQRT(K60^2+K61^2+K62^2)</f>
+        <f t="shared" ref="K63:L63" si="76">SQRT(K60^2+K61^2+K62^2)</f>
         <v>4.6057487741846835E-2</v>
       </c>
       <c r="L63" s="24">
-        <f t="shared" si="53"/>
+        <f t="shared" si="76"/>
         <v>7.5159289553528977E-2</v>
       </c>
       <c r="M63" s="24">
-        <f t="shared" ref="M63:N63" si="54">SQRT(M60^2+M61^2+M62^2)</f>
+        <f t="shared" ref="M63:N63" si="77">SQRT(M60^2+M61^2+M62^2)</f>
         <v>2.0439857481210747E-2</v>
       </c>
       <c r="N63" s="24">
-        <f t="shared" si="54"/>
+        <f t="shared" si="77"/>
         <v>7.3357577165551E-3</v>
       </c>
       <c r="O63" s="24"/>
       <c r="P63" s="24">
-        <f t="shared" ref="P63" si="55">SQRT(P60^2+P61^2+P62^2)</f>
+        <f t="shared" ref="P63" si="78">SQRT(P60^2+P61^2+P62^2)</f>
         <v>6.5512826557723128E-2</v>
       </c>
       <c r="Q63" s="24">
-        <f t="shared" ref="Q63:R63" si="56">SQRT(Q60^2+Q61^2+Q62^2)</f>
+        <f t="shared" ref="Q63:R63" si="79">SQRT(Q60^2+Q61^2+Q62^2)</f>
         <v>8.7979655683729563E-2</v>
       </c>
       <c r="R63" s="24">
-        <f t="shared" si="56"/>
+        <f t="shared" si="79"/>
         <v>4.481380191310301E-2</v>
       </c>
       <c r="S63" s="24">
-        <f t="shared" ref="S63:U63" si="57">SQRT(S60^2+S61^2+S62^2)</f>
+        <f t="shared" ref="S63:U63" si="80">SQRT(S60^2+S61^2+S62^2)</f>
         <v>6.2607194185091627E-2</v>
       </c>
       <c r="T63" s="24"/>
       <c r="U63" s="24">
-        <f t="shared" si="57"/>
+        <f t="shared" si="80"/>
         <v>2.3262399408893929E-2</v>
       </c>
       <c r="V63" s="24">
-        <f t="shared" ref="V63:X63" si="58">SQRT(V60^2+V61^2+V62^2)</f>
+        <f t="shared" ref="V63:X63" si="81">SQRT(V60^2+V61^2+V62^2)</f>
         <v>3.647601287297448E-2</v>
       </c>
       <c r="W63" s="24"/>
       <c r="X63" s="24">
-        <f t="shared" si="58"/>
+        <f t="shared" si="81"/>
         <v>2.1982067547956201</v>
       </c>
       <c r="Y63" s="24">
-        <f t="shared" ref="Y63" si="59">SQRT(Y60^2+Y61^2+Y62^2)</f>
+        <f t="shared" ref="Y63:AA63" si="82">SQRT(Y60^2+Y61^2+Y62^2)</f>
         <v>1.3295151635884876</v>
       </c>
-    </row>
-    <row r="64" spans="1:25">
+      <c r="AA63" s="24">
+        <f t="shared" si="82"/>
+        <v>2.7505705683371524E-2</v>
+      </c>
+      <c r="AB63" s="24">
+        <f t="shared" ref="AB63:AD63" si="83">SQRT(AB60^2+AB61^2+AB62^2)</f>
+        <v>0.56451053505462656</v>
+      </c>
+      <c r="AC63" s="24">
+        <f t="shared" si="83"/>
+        <v>0.81484411440209514</v>
+      </c>
+      <c r="AD63" s="24">
+        <f t="shared" si="83"/>
+        <v>2.0347140100859646</v>
+      </c>
+      <c r="AE63" s="24">
+        <f t="shared" ref="AE63" si="84">SQRT(AE60^2+AE61^2+AE62^2)</f>
+        <v>25.882587877998905</v>
+      </c>
+    </row>
+    <row r="64" spans="1:31">
       <c r="L64" s="54"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.11811023622047245" right="0.11811023622047245" top="0.23622047244094491" bottom="0.23622047244094491" header="0.11811023622047245" footer="0.11811023622047245"/>
   <pageSetup paperSize="9" scale="55" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6233,8 +6862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AP40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y7" workbookViewId="0">
-      <selection activeCell="AK17" sqref="AK17"/>
+    <sheetView topLeftCell="Y4" workbookViewId="0">
+      <selection activeCell="AL11" sqref="AL11:AP11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8665,7 +9294,7 @@
         <v/>
       </c>
       <c r="O24" s="43" t="str">
-        <f t="shared" ref="O24:AP24" si="45">IF(O26=1, "duplicate","")</f>
+        <f t="shared" ref="O24:AJ24" si="45">IF(O26=1, "duplicate","")</f>
         <v/>
       </c>
       <c r="P24" s="43" t="str">
@@ -9751,7 +10380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adjust the md coefficient as 2.23e-7 Redo FLUENT case 18 by using the v3.0 UDF (16GGQ-3-18.cas&dat)
</commit_message>
<xml_diff>
--- a/bin/2d_s_cc/reorganized exp.data.xlsx
+++ b/bin/2d_s_cc/reorganized exp.data.xlsx
@@ -4,16 +4,17 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="75" windowWidth="17235" windowHeight="8955" activeTab="1"/>
+    <workbookView xWindow="2340" yWindow="75" windowWidth="17235" windowHeight="8955" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Wang&amp;Chung2008CES" sheetId="1" r:id="rId1"/>
     <sheet name="Yao2016(preparing)" sheetId="2" r:id="rId2"/>
     <sheet name="ExpData" sheetId="3" r:id="rId3"/>
     <sheet name="SimRecords" sheetId="4" r:id="rId4"/>
+    <sheet name="Origin exporter" sheetId="5" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
     <definedName name="MOD1H">'Yao2016(preparing)'!$C$17</definedName>
@@ -261,7 +262,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="157">
   <si>
     <t>Wang K Y, Chung T S, Gryta M. Chem. Eng. Sci., 2008, 63: 2587-2594</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -768,6 +769,30 @@
   </si>
   <si>
     <t>16GGQ-3-</t>
+  </si>
+  <si>
+    <t>JM_EXP</t>
+  </si>
+  <si>
+    <t>JM_SIM</t>
+  </si>
+  <si>
+    <t>T0O_SIM</t>
+  </si>
+  <si>
+    <t>T1O_SIM</t>
+  </si>
+  <si>
+    <t>T0O_EXP</t>
+  </si>
+  <si>
+    <t>T1O_EXP</t>
+  </si>
+  <si>
+    <t>transpose</t>
+  </si>
+  <si>
+    <t>16GGQ-3-18</t>
   </si>
 </sst>
 </file>
@@ -1397,23 +1422,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="235652608"/>
-        <c:axId val="235654144"/>
+        <c:axId val="178368512"/>
+        <c:axId val="178370816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="235652608"/>
+        <c:axId val="178368512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235654144"/>
+        <c:crossAx val="178370816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="235654144"/>
+        <c:axId val="178370816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1421,7 +1446,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235652608"/>
+        <c:crossAx val="178368512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1435,7 +1460,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3147,11 +3172,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="V34" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="T42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE62" sqref="AE62"/>
+      <selection pane="bottomRight" activeCell="X56" sqref="X56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3854,7 +3879,7 @@
         <v>189.89</v>
       </c>
       <c r="AA26" s="24">
-        <f t="shared" ref="AA26:AD26" si="6">-22.11+2.12*AA23</f>
+        <f t="shared" ref="AA26:AB26" si="6">-22.11+2.12*AA23</f>
         <v>189.89</v>
       </c>
       <c r="AB26" s="24">
@@ -3974,7 +3999,7 @@
         <v>196.76</v>
       </c>
       <c r="AA27" s="24">
-        <f t="shared" ref="AA27:AD27" si="13">-7.24+2.04*AA24</f>
+        <f t="shared" ref="AA27:AB27" si="13">-7.24+2.04*AA24</f>
         <v>196.76</v>
       </c>
       <c r="AB27" s="24">
@@ -5271,7 +5296,7 @@
         <v>319.9632722324157</v>
       </c>
       <c r="AB42" s="57">
-        <f t="shared" ref="AA42:AE42" si="19">AB30+273.15</f>
+        <f t="shared" ref="AB42:AE42" si="19">AB30+273.15</f>
         <v>319.99878353087877</v>
       </c>
       <c r="AC42" s="57">
@@ -5391,7 +5416,7 @@
         <v>318.26500700465544</v>
       </c>
       <c r="AB43" s="57">
-        <f t="shared" ref="AA43:AE43" si="22">AB35+273.15</f>
+        <f t="shared" ref="AB43:AE43" si="22">AB35+273.15</f>
         <v>318.58325015595727</v>
       </c>
       <c r="AC43" s="57">
@@ -5636,7 +5661,7 @@
         <v>293.11519271759857</v>
       </c>
       <c r="AB46" s="57">
-        <f t="shared" ref="AA46:AE46" si="27">AB33+273.15</f>
+        <f t="shared" ref="AB46:AE46" si="27">AB33+273.15</f>
         <v>293.1399251403617</v>
       </c>
       <c r="AC46" s="57">
@@ -5756,7 +5781,7 @@
         <v>294.57886130730265</v>
       </c>
       <c r="AB47" s="57">
-        <f t="shared" ref="AA47:AE47" si="30">AB36+273.15</f>
+        <f t="shared" ref="AB47:AE47" si="30">AB36+273.15</f>
         <v>294.73300062382947</v>
       </c>
       <c r="AC47" s="57">
@@ -5876,7 +5901,7 @@
         <v>2.9802457599999999E-3</v>
       </c>
       <c r="AB48" s="57">
-        <f t="shared" ref="AA48:AE48" si="33">AB37/3600</f>
+        <f t="shared" ref="AB48:AE48" si="33">AB37/3600</f>
         <v>1.8809364341085273E-3</v>
       </c>
       <c r="AC48" s="57">
@@ -6054,8 +6079,8 @@
       <c r="V55" s="39">
         <v>17</v>
       </c>
-      <c r="X55" s="39">
-        <v>18</v>
+      <c r="X55" s="39" t="s">
+        <v>156</v>
       </c>
       <c r="Y55" s="39">
         <v>19</v>
@@ -6138,8 +6163,8 @@
       <c r="V56" s="39">
         <v>317.83413999999999</v>
       </c>
-      <c r="X56" s="39">
-        <v>318.00452000000001</v>
+      <c r="X56" s="42">
+        <v>318.14089999999999</v>
       </c>
       <c r="Y56" s="39">
         <v>318.00878999999998</v>
@@ -6219,8 +6244,8 @@
       <c r="V57" s="39">
         <v>294.66298999999998</v>
       </c>
-      <c r="X57" s="39">
-        <v>295.14654999999999</v>
+      <c r="X57" s="42">
+        <v>294.798</v>
       </c>
       <c r="Y57" s="39">
         <v>295.12842000000001</v>
@@ -6300,8 +6325,8 @@
       <c r="V58" s="39">
         <v>6.3664417000000002</v>
       </c>
-      <c r="X58" s="39">
-        <v>6.2245407000000004</v>
+      <c r="X58" s="42">
+        <v>1.9314100000000001</v>
       </c>
       <c r="Y58" s="39">
         <v>6.2292604000000003</v>
@@ -6402,11 +6427,11 @@
       </c>
       <c r="W59" s="24"/>
       <c r="X59" s="24">
-        <f t="shared" si="38"/>
-        <v>3.1122703500000002E-3</v>
+        <f t="shared" ref="X59:AA59" si="39">X58*0.0005</f>
+        <v>9.6570500000000008E-4</v>
       </c>
       <c r="Y59" s="24">
-        <f t="shared" ref="Y59:AA59" si="39">Y58*0.0005</f>
+        <f t="shared" si="39"/>
         <v>3.1146302000000002E-3</v>
       </c>
       <c r="AA59" s="24">
@@ -6507,7 +6532,7 @@
       <c r="W60" s="24"/>
       <c r="X60" s="24">
         <f t="shared" si="49"/>
-        <v>1.2226964095895161E-3</v>
+        <v>7.9435894865143128E-4</v>
       </c>
       <c r="Y60" s="24">
         <f t="shared" ref="Y60:AA60" si="50">(Y43-Y56)/Y43</f>
@@ -6611,7 +6636,7 @@
       <c r="W61" s="24"/>
       <c r="X61" s="24">
         <f t="shared" si="60"/>
-        <v>-1.7589334666764701E-3</v>
+        <v>-5.7591751660082495E-4</v>
       </c>
       <c r="Y61" s="24">
         <f t="shared" ref="Y61:AA61" si="61">(Y47-Y57)/Y47</f>
@@ -6716,7 +6741,7 @@
       <c r="W62" s="55"/>
       <c r="X62" s="55">
         <f t="shared" si="70"/>
-        <v>-2.1982057110278923</v>
+        <v>7.6301545692549523E-3</v>
       </c>
       <c r="Y62" s="55">
         <f t="shared" ref="Y62:AA62" si="71">(Y48-Y59)/Y48</f>
@@ -6820,7 +6845,7 @@
       <c r="W63" s="24"/>
       <c r="X63" s="24">
         <f t="shared" si="81"/>
-        <v>2.1982067547956201</v>
+        <v>7.692980298684802E-3</v>
       </c>
       <c r="Y63" s="24">
         <f t="shared" ref="Y63:AA63" si="82">SQRT(Y60^2+Y61^2+Y62^2)</f>
@@ -10378,10 +10403,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10502,9 +10527,1486 @@
         <v>9.5687569099487663E-7</v>
       </c>
     </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12" s="42" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="42" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="22">
+        <v>2.23E-7</v>
+      </c>
+      <c r="D14" s="22">
+        <v>3.4999999999999998E-7</v>
+      </c>
+      <c r="E14" s="22">
+        <v>2.4999999999999999E-7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="B15" s="42"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="C16">
+        <v>318.14089999999999</v>
+      </c>
+      <c r="D16">
+        <v>317.97539999999998</v>
+      </c>
+      <c r="E16">
+        <v>318.10550000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="C17">
+        <v>294.798</v>
+      </c>
+      <c r="D17">
+        <v>294.95639999999997</v>
+      </c>
+      <c r="E17">
+        <v>294.83249999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="21"/>
+      <c r="C18">
+        <v>1.9314100000000001</v>
+      </c>
+      <c r="D18">
+        <v>2.8276400000000002</v>
+      </c>
+      <c r="E18">
+        <v>2.1318199999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19" s="21"/>
+      <c r="C19" s="42">
+        <f>C18*0.0005</f>
+        <v>9.6570500000000008E-4</v>
+      </c>
+      <c r="D19" s="42">
+        <f>D18*0.0005</f>
+        <v>1.4138200000000001E-3</v>
+      </c>
+      <c r="E19" s="42">
+        <f>E18*0.0005</f>
+        <v>1.06591E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" s="42"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="B21" s="22">
+        <f>(0.001337-C19)*(C14-D14)/(C19-D19)+C14</f>
+        <v>3.2822849045445922E-7</v>
+      </c>
+      <c r="C21" s="22">
+        <f>(0.0009731-D19)*(D14-E14)/(D19-E19)+D14</f>
+        <v>2.2332356069098329E-7</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AA36"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:G36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:27" s="42" customFormat="1">
+      <c r="B1" s="42">
+        <v>1</v>
+      </c>
+      <c r="C1" s="42">
+        <v>2</v>
+      </c>
+      <c r="D1" s="42">
+        <v>3</v>
+      </c>
+      <c r="E1" s="42">
+        <v>4</v>
+      </c>
+      <c r="F1" s="42">
+        <v>5</v>
+      </c>
+      <c r="G1" s="42">
+        <v>6</v>
+      </c>
+      <c r="H1" s="42">
+        <v>7</v>
+      </c>
+      <c r="I1" s="42">
+        <v>8</v>
+      </c>
+      <c r="J1" s="42">
+        <v>9</v>
+      </c>
+      <c r="K1" s="42">
+        <v>10</v>
+      </c>
+      <c r="L1" s="42">
+        <v>11</v>
+      </c>
+      <c r="M1" s="42">
+        <v>12</v>
+      </c>
+      <c r="N1" s="42">
+        <v>13</v>
+      </c>
+      <c r="O1" s="42">
+        <v>14</v>
+      </c>
+      <c r="P1" s="42">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="42">
+        <v>16</v>
+      </c>
+      <c r="R1" s="42">
+        <v>17</v>
+      </c>
+      <c r="S1" s="42">
+        <v>18</v>
+      </c>
+      <c r="T1" s="42">
+        <v>19</v>
+      </c>
+      <c r="U1" s="42">
+        <v>20</v>
+      </c>
+      <c r="V1" s="42">
+        <v>21</v>
+      </c>
+      <c r="W1" s="42">
+        <v>22</v>
+      </c>
+      <c r="X1" s="42">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="42">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="42">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="42">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
+      <c r="A2" s="42">
+        <v>1</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" t="str">
+        <f>'Yao2016(preparing)'!B43</f>
+        <v>K</v>
+      </c>
+      <c r="D2">
+        <f>'Yao2016(preparing)'!C43</f>
+        <v>305.35915961980555</v>
+      </c>
+      <c r="E2">
+        <f>'Yao2016(preparing)'!D43</f>
+        <v>309.79188253593401</v>
+      </c>
+      <c r="F2">
+        <f>'Yao2016(preparing)'!E43</f>
+        <v>312.35623159324001</v>
+      </c>
+      <c r="G2">
+        <f>'Yao2016(preparing)'!F43</f>
+        <v>318.26500700465544</v>
+      </c>
+      <c r="H2">
+        <f>'Yao2016(preparing)'!G43</f>
+        <v>323.63862859035953</v>
+      </c>
+      <c r="I2">
+        <f>'Yao2016(preparing)'!I43</f>
+        <v>318.30270436408495</v>
+      </c>
+      <c r="J2">
+        <f>'Yao2016(preparing)'!J43</f>
+        <v>318.4829372796284</v>
+      </c>
+      <c r="K2">
+        <f>'Yao2016(preparing)'!K43</f>
+        <v>318.80301197436296</v>
+      </c>
+      <c r="L2">
+        <f>'Yao2016(preparing)'!L43</f>
+        <v>319.01289994963463</v>
+      </c>
+      <c r="M2">
+        <f>'Yao2016(preparing)'!M43</f>
+        <v>319.56472605071929</v>
+      </c>
+      <c r="N2">
+        <f>'Yao2016(preparing)'!N43</f>
+        <v>318.40305616471557</v>
+      </c>
+      <c r="O2">
+        <f>'Yao2016(preparing)'!P43</f>
+        <v>318.70412169546893</v>
+      </c>
+      <c r="P2">
+        <f>'Yao2016(preparing)'!Q43</f>
+        <v>318.81776959447166</v>
+      </c>
+      <c r="Q2">
+        <f>'Yao2016(preparing)'!R43</f>
+        <v>318.56053255624283</v>
+      </c>
+      <c r="R2">
+        <f>'Yao2016(preparing)'!S43</f>
+        <v>318.51664490974343</v>
+      </c>
+      <c r="S2">
+        <f>'Yao2016(preparing)'!U43</f>
+        <v>318.3348782464065</v>
+      </c>
+      <c r="T2">
+        <f>'Yao2016(preparing)'!V43</f>
+        <v>318.29827050530861</v>
+      </c>
+      <c r="U2">
+        <f>'Yao2016(preparing)'!X43</f>
+        <v>318.3938189793015</v>
+      </c>
+      <c r="V2">
+        <f>'Yao2016(preparing)'!Y43</f>
+        <v>318.0786832403021</v>
+      </c>
+      <c r="W2">
+        <f>'Yao2016(preparing)'!AA43</f>
+        <v>318.26500700465544</v>
+      </c>
+      <c r="X2">
+        <f>'Yao2016(preparing)'!AB43</f>
+        <v>318.58325015595727</v>
+      </c>
+      <c r="Y2">
+        <f>'Yao2016(preparing)'!AC43</f>
+        <v>319.27722725851919</v>
+      </c>
+      <c r="Z2">
+        <f>'Yao2016(preparing)'!AD43</f>
+        <v>318.41165201005003</v>
+      </c>
+      <c r="AA2">
+        <f>'Yao2016(preparing)'!AE43</f>
+        <v>319.10031185031147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27">
+      <c r="A3" s="42">
+        <v>2</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" t="str">
+        <f>'Yao2016(preparing)'!B56</f>
+        <v>K</v>
+      </c>
+      <c r="D3">
+        <f>'Yao2016(preparing)'!C56</f>
+        <v>305.07</v>
+      </c>
+      <c r="E3">
+        <f>'Yao2016(preparing)'!D56</f>
+        <v>309.42</v>
+      </c>
+      <c r="F3">
+        <f>'Yao2016(preparing)'!E56</f>
+        <v>312.06</v>
+      </c>
+      <c r="G3">
+        <f>'Yao2016(preparing)'!F56</f>
+        <v>317.77999999999997</v>
+      </c>
+      <c r="H3">
+        <f>'Yao2016(preparing)'!G56</f>
+        <v>322.74</v>
+      </c>
+      <c r="I3">
+        <f>'Yao2016(preparing)'!I56</f>
+        <v>318.13</v>
+      </c>
+      <c r="J3">
+        <f>'Yao2016(preparing)'!J56</f>
+        <v>318.58</v>
+      </c>
+      <c r="K3">
+        <f>'Yao2016(preparing)'!K56</f>
+        <v>319.00351000000001</v>
+      </c>
+      <c r="L3">
+        <f>'Yao2016(preparing)'!L56</f>
+        <v>319.28005999999999</v>
+      </c>
+      <c r="M3">
+        <f>'Yao2016(preparing)'!M56</f>
+        <v>317.73446999999999</v>
+      </c>
+      <c r="N3">
+        <f>'Yao2016(preparing)'!N56</f>
+        <v>317.72046</v>
+      </c>
+      <c r="O3">
+        <f>'Yao2016(preparing)'!P56</f>
+        <v>318.26294000000001</v>
+      </c>
+      <c r="P3">
+        <f>'Yao2016(preparing)'!Q56</f>
+        <v>318.48025999999999</v>
+      </c>
+      <c r="Q3">
+        <f>'Yao2016(preparing)'!R56</f>
+        <v>318.41379000000001</v>
+      </c>
+      <c r="R3">
+        <f>'Yao2016(preparing)'!S56</f>
+        <v>318.17993000000001</v>
+      </c>
+      <c r="S3">
+        <f>'Yao2016(preparing)'!U56</f>
+        <v>317.89227</v>
+      </c>
+      <c r="T3">
+        <f>'Yao2016(preparing)'!V56</f>
+        <v>317.83413999999999</v>
+      </c>
+      <c r="U3">
+        <f>'Yao2016(preparing)'!X56</f>
+        <v>318.14089999999999</v>
+      </c>
+      <c r="V3">
+        <f>'Yao2016(preparing)'!Y56</f>
+        <v>318.00878999999998</v>
+      </c>
+      <c r="W3">
+        <f>'Yao2016(preparing)'!AA56</f>
+        <v>317.47500000000002</v>
+      </c>
+      <c r="X3">
+        <f>'Yao2016(preparing)'!AB56</f>
+        <v>317.59199999999998</v>
+      </c>
+      <c r="Y3">
+        <f>'Yao2016(preparing)'!AC56</f>
+        <v>317.73099999999999</v>
+      </c>
+      <c r="Z3">
+        <f>'Yao2016(preparing)'!AD56</f>
+        <v>317.86700000000002</v>
+      </c>
+      <c r="AA3">
+        <f>'Yao2016(preparing)'!AE56</f>
+        <v>317.99400000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
+      <c r="A4" s="42">
+        <v>3</v>
+      </c>
+      <c r="B4" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" t="str">
+        <f>'Yao2016(preparing)'!B47</f>
+        <v>K</v>
+      </c>
+      <c r="D4">
+        <f>'Yao2016(preparing)'!C47</f>
+        <v>294.29682689366177</v>
+      </c>
+      <c r="E4">
+        <f>'Yao2016(preparing)'!D47</f>
+        <v>294.21664608339694</v>
+      </c>
+      <c r="F4">
+        <f>'Yao2016(preparing)'!E47</f>
+        <v>294.35225488233681</v>
+      </c>
+      <c r="G4">
+        <f>'Yao2016(preparing)'!F47</f>
+        <v>294.57886130730265</v>
+      </c>
+      <c r="H4">
+        <f>'Yao2016(preparing)'!G47</f>
+        <v>295.14325006184663</v>
+      </c>
+      <c r="I4">
+        <f>'Yao2016(preparing)'!I47</f>
+        <v>299.22168943939931</v>
+      </c>
+      <c r="J4">
+        <f>'Yao2016(preparing)'!J47</f>
+        <v>303.91148736331343</v>
+      </c>
+      <c r="K4">
+        <f>'Yao2016(preparing)'!K47</f>
+        <v>308.65229050926581</v>
+      </c>
+      <c r="L4">
+        <f>'Yao2016(preparing)'!L47</f>
+        <v>313.57345483397432</v>
+      </c>
+      <c r="M4">
+        <f>'Yao2016(preparing)'!M47</f>
+        <v>294.64494411853934</v>
+      </c>
+      <c r="N4">
+        <f>'Yao2016(preparing)'!N47</f>
+        <v>294.66788302030187</v>
+      </c>
+      <c r="O4">
+        <f>'Yao2016(preparing)'!P47</f>
+        <v>294.74539495317856</v>
+      </c>
+      <c r="P4">
+        <f>'Yao2016(preparing)'!Q47</f>
+        <v>294.95517646294218</v>
+      </c>
+      <c r="Q4">
+        <f>'Yao2016(preparing)'!R47</f>
+        <v>294.88340227697375</v>
+      </c>
+      <c r="R4">
+        <f>'Yao2016(preparing)'!S47</f>
+        <v>295.00451737531392</v>
+      </c>
+      <c r="S4">
+        <f>'Yao2016(preparing)'!U47</f>
+        <v>294.62908105804513</v>
+      </c>
+      <c r="T4">
+        <f>'Yao2016(preparing)'!V47</f>
+        <v>294.46046760050325</v>
+      </c>
+      <c r="U4">
+        <f>'Yao2016(preparing)'!X47</f>
+        <v>294.62831839055224</v>
+      </c>
+      <c r="V4">
+        <f>'Yao2016(preparing)'!Y47</f>
+        <v>294.45689294842822</v>
+      </c>
+      <c r="W4">
+        <f>'Yao2016(preparing)'!AA47</f>
+        <v>294.57886130730265</v>
+      </c>
+      <c r="X4">
+        <f>'Yao2016(preparing)'!AB47</f>
+        <v>294.73300062382947</v>
+      </c>
+      <c r="Y4">
+        <f>'Yao2016(preparing)'!AC47</f>
+        <v>294.71908408877823</v>
+      </c>
+      <c r="Z4">
+        <f>'Yao2016(preparing)'!AD47</f>
+        <v>294.40166457286438</v>
+      </c>
+      <c r="AA4">
+        <f>'Yao2016(preparing)'!AE47</f>
+        <v>294.37408177408201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27">
+      <c r="A5" s="42">
+        <v>4</v>
+      </c>
+      <c r="B5" s="42" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" t="str">
+        <f>'Yao2016(preparing)'!B57</f>
+        <v>K</v>
+      </c>
+      <c r="D5">
+        <f>'Yao2016(preparing)'!C57</f>
+        <v>294.04000000000002</v>
+      </c>
+      <c r="E5">
+        <f>'Yao2016(preparing)'!D57</f>
+        <v>294.45</v>
+      </c>
+      <c r="F5">
+        <f>'Yao2016(preparing)'!E57</f>
+        <v>294.75</v>
+      </c>
+      <c r="G5">
+        <f>'Yao2016(preparing)'!F57</f>
+        <v>295.33999999999997</v>
+      </c>
+      <c r="H5">
+        <f>'Yao2016(preparing)'!G57</f>
+        <v>296.47000000000003</v>
+      </c>
+      <c r="I5">
+        <f>'Yao2016(preparing)'!I57</f>
+        <v>299.95</v>
+      </c>
+      <c r="J5">
+        <f>'Yao2016(preparing)'!J57</f>
+        <v>304.49</v>
+      </c>
+      <c r="K5">
+        <f>'Yao2016(preparing)'!K57</f>
+        <v>309.03847999999999</v>
+      </c>
+      <c r="L5">
+        <f>'Yao2016(preparing)'!L57</f>
+        <v>313.75484999999998</v>
+      </c>
+      <c r="M5">
+        <f>'Yao2016(preparing)'!M57</f>
+        <v>295.32715000000002</v>
+      </c>
+      <c r="N5">
+        <f>'Yao2016(preparing)'!N57</f>
+        <v>295.35687000000001</v>
+      </c>
+      <c r="O5">
+        <f>'Yao2016(preparing)'!P57</f>
+        <v>295.41543999999999</v>
+      </c>
+      <c r="P5">
+        <f>'Yao2016(preparing)'!Q57</f>
+        <v>295.55029000000002</v>
+      </c>
+      <c r="Q5">
+        <f>'Yao2016(preparing)'!R57</f>
+        <v>296.52123999999998</v>
+      </c>
+      <c r="R5">
+        <f>'Yao2016(preparing)'!S57</f>
+        <v>295.77208999999999</v>
+      </c>
+      <c r="S5">
+        <f>'Yao2016(preparing)'!U57</f>
+        <v>294.94614000000001</v>
+      </c>
+      <c r="T5">
+        <f>'Yao2016(preparing)'!V57</f>
+        <v>294.66298999999998</v>
+      </c>
+      <c r="U5">
+        <f>'Yao2016(preparing)'!X57</f>
+        <v>294.798</v>
+      </c>
+      <c r="V5">
+        <f>'Yao2016(preparing)'!Y57</f>
+        <v>295.12842000000001</v>
+      </c>
+      <c r="W5">
+        <f>'Yao2016(preparing)'!AA57</f>
+        <v>295.42500000000001</v>
+      </c>
+      <c r="X5">
+        <f>'Yao2016(preparing)'!AB57</f>
+        <v>295.40800000000002</v>
+      </c>
+      <c r="Y5">
+        <f>'Yao2016(preparing)'!AC57</f>
+        <v>295.36700000000002</v>
+      </c>
+      <c r="Z5">
+        <f>'Yao2016(preparing)'!AD57</f>
+        <v>295.315</v>
+      </c>
+      <c r="AA5">
+        <f>'Yao2016(preparing)'!AE57</f>
+        <v>295.26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27">
+      <c r="A6" s="42">
+        <v>5</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" t="str">
+        <f>'Yao2016(preparing)'!B48</f>
+        <v>kg/m2-s</v>
+      </c>
+      <c r="D6">
+        <f>'Yao2016(preparing)'!C48</f>
+        <v>1.0791274666666665E-3</v>
+      </c>
+      <c r="E6">
+        <f>'Yao2016(preparing)'!D48</f>
+        <v>1.5744281599999997E-3</v>
+      </c>
+      <c r="F6">
+        <f>'Yao2016(preparing)'!E48</f>
+        <v>1.9465498666666667E-3</v>
+      </c>
+      <c r="G6">
+        <f>'Yao2016(preparing)'!F48</f>
+        <v>2.9802457599999999E-3</v>
+      </c>
+      <c r="H6">
+        <f>'Yao2016(preparing)'!G48</f>
+        <v>3.9183833599999995E-3</v>
+      </c>
+      <c r="I6">
+        <f>'Yao2016(preparing)'!I48</f>
+        <v>2.5700625066666666E-3</v>
+      </c>
+      <c r="J6">
+        <f>'Yao2016(preparing)'!J48</f>
+        <v>2.1235246933333334E-3</v>
+      </c>
+      <c r="K6">
+        <f>'Yao2016(preparing)'!K48</f>
+        <v>1.5609421866666663E-3</v>
+      </c>
+      <c r="L6">
+        <f>'Yao2016(preparing)'!L48</f>
+        <v>9.935384533333333E-4</v>
+      </c>
+      <c r="M6">
+        <f>'Yao2016(preparing)'!M48</f>
+        <v>2.9378886400000001E-3</v>
+      </c>
+      <c r="N6">
+        <f>'Yao2016(preparing)'!N48</f>
+        <v>2.8567750399999996E-3</v>
+      </c>
+      <c r="O6">
+        <f>'Yao2016(preparing)'!P48</f>
+        <v>3.0446920533333329E-3</v>
+      </c>
+      <c r="P6">
+        <f>'Yao2016(preparing)'!Q48</f>
+        <v>3.1019777066666663E-3</v>
+      </c>
+      <c r="Q6">
+        <f>'Yao2016(preparing)'!R48</f>
+        <v>2.7461594666666673E-3</v>
+      </c>
+      <c r="R6">
+        <f>'Yao2016(preparing)'!S48</f>
+        <v>2.8241684266666666E-3</v>
+      </c>
+      <c r="S6">
+        <f>'Yao2016(preparing)'!U48</f>
+        <v>3.2108769066666668E-3</v>
+      </c>
+      <c r="T6">
+        <f>'Yao2016(preparing)'!V48</f>
+        <v>3.3036054400000002E-3</v>
+      </c>
+      <c r="U6">
+        <f>'Yao2016(preparing)'!X48</f>
+        <v>9.7313013333333309E-4</v>
+      </c>
+      <c r="V6">
+        <f>'Yao2016(preparing)'!Y48</f>
+        <v>1.3370305066666666E-3</v>
+      </c>
+      <c r="W6">
+        <f>'Yao2016(preparing)'!AA48</f>
+        <v>2.9802457599999999E-3</v>
+      </c>
+      <c r="X6">
+        <f>'Yao2016(preparing)'!AB48</f>
+        <v>1.8809364341085273E-3</v>
+      </c>
+      <c r="Y6">
+        <f>'Yao2016(preparing)'!AC48</f>
+        <v>1.5352870399999998E-3</v>
+      </c>
+      <c r="Z6">
+        <f>'Yao2016(preparing)'!AD48</f>
+        <v>8.5928448000000001E-4</v>
+      </c>
+      <c r="AA6">
+        <f>'Yao2016(preparing)'!AE48</f>
+        <v>8.9403596384000003E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27">
+      <c r="A7" s="42">
+        <v>6</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" t="str">
+        <f>'Yao2016(preparing)'!B59</f>
+        <v>kg/m2-s</v>
+      </c>
+      <c r="D7">
+        <f>'Yao2016(preparing)'!C59</f>
+        <v>1.0750550000000001E-3</v>
+      </c>
+      <c r="E7">
+        <f>'Yao2016(preparing)'!D59</f>
+        <v>1.5754600000000001E-3</v>
+      </c>
+      <c r="F7">
+        <f>'Yao2016(preparing)'!E59</f>
+        <v>1.937825E-3</v>
+      </c>
+      <c r="G7">
+        <f>'Yao2016(preparing)'!F59</f>
+        <v>2.887485E-3</v>
+      </c>
+      <c r="H7">
+        <f>'Yao2016(preparing)'!G59</f>
+        <v>3.8479500000000002E-3</v>
+      </c>
+      <c r="I7">
+        <f>'Yao2016(preparing)'!I59</f>
+        <v>2.51885E-3</v>
+      </c>
+      <c r="J7">
+        <f>'Yao2016(preparing)'!J59</f>
+        <v>2.0999450000000002E-3</v>
+      </c>
+      <c r="K7">
+        <f>'Yao2016(preparing)'!K59</f>
+        <v>1.4890823500000002E-3</v>
+      </c>
+      <c r="L7">
+        <f>'Yao2016(preparing)'!L59</f>
+        <v>1.0682052500000001E-3</v>
+      </c>
+      <c r="M7">
+        <f>'Yao2016(preparing)'!M59</f>
+        <v>2.8806469500000003E-3</v>
+      </c>
+      <c r="N7">
+        <f>'Yao2016(preparing)'!N59</f>
+        <v>2.8756708999999997E-3</v>
+      </c>
+      <c r="O7">
+        <f>'Yao2016(preparing)'!P59</f>
+        <v>3.2439937500000002E-3</v>
+      </c>
+      <c r="P7">
+        <f>'Yao2016(preparing)'!Q59</f>
+        <v>3.3747971000000002E-3</v>
+      </c>
+      <c r="Q7">
+        <f>'Yao2016(preparing)'!R59</f>
+        <v>2.8682699E-3</v>
+      </c>
+      <c r="R7">
+        <f>'Yao2016(preparing)'!S59</f>
+        <v>3.0008037E-3</v>
+      </c>
+      <c r="S7">
+        <f>'Yao2016(preparing)'!U59</f>
+        <v>3.13639785E-3</v>
+      </c>
+      <c r="T7">
+        <f>'Yao2016(preparing)'!V59</f>
+        <v>3.1832208500000001E-3</v>
+      </c>
+      <c r="U7">
+        <f>'Yao2016(preparing)'!X59</f>
+        <v>9.6570500000000008E-4</v>
+      </c>
+      <c r="V7">
+        <f>'Yao2016(preparing)'!Y59</f>
+        <v>3.1146302000000002E-3</v>
+      </c>
+      <c r="W7">
+        <f>'Yao2016(preparing)'!AA59</f>
+        <v>3.0614349999999999E-3</v>
+      </c>
+      <c r="X7">
+        <f>'Yao2016(preparing)'!AB59</f>
+        <v>2.9427200000000002E-3</v>
+      </c>
+      <c r="Y7">
+        <f>'Yao2016(preparing)'!AC59</f>
+        <v>2.7862800000000004E-3</v>
+      </c>
+      <c r="Z7">
+        <f>'Yao2016(preparing)'!AD59</f>
+        <v>2.6076800000000002E-3</v>
+      </c>
+      <c r="AA7">
+        <f>'Yao2016(preparing)'!AE59</f>
+        <v>2.4034E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="16.5">
+      <c r="A9" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27">
+      <c r="B10" s="42">
+        <v>1</v>
+      </c>
+      <c r="C10" s="42">
+        <v>2</v>
+      </c>
+      <c r="D10" s="42">
+        <v>3</v>
+      </c>
+      <c r="E10" s="42">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="array" ref="B11:G36">TRANSPOSE(B2:AA7)</f>
+        <v>T0O_EXP</v>
+      </c>
+      <c r="C11" t="str">
+        <v>T0O_SIM</v>
+      </c>
+      <c r="D11" t="str">
+        <v>T1O_EXP</v>
+      </c>
+      <c r="E11" t="str">
+        <v>T1O_SIM</v>
+      </c>
+      <c r="F11" t="str">
+        <v>JM_EXP</v>
+      </c>
+      <c r="G11" t="str">
+        <v>JM_SIM</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="str">
+        <v>K</v>
+      </c>
+      <c r="C12" t="str">
+        <v>K</v>
+      </c>
+      <c r="D12" t="str">
+        <v>K</v>
+      </c>
+      <c r="E12" t="str">
+        <v>K</v>
+      </c>
+      <c r="F12" t="str">
+        <v>kg/m2-s</v>
+      </c>
+      <c r="G12" t="str">
+        <v>kg/m2-s</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27">
+      <c r="A13" s="42">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>305.35915961980555</v>
+      </c>
+      <c r="C13">
+        <v>305.07</v>
+      </c>
+      <c r="D13">
+        <v>294.29682689366177</v>
+      </c>
+      <c r="E13">
+        <v>294.04000000000002</v>
+      </c>
+      <c r="F13">
+        <v>1.0791274666666665E-3</v>
+      </c>
+      <c r="G13">
+        <v>1.0750550000000001E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27">
+      <c r="A14" s="42">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>309.79188253593401</v>
+      </c>
+      <c r="C14">
+        <v>309.42</v>
+      </c>
+      <c r="D14">
+        <v>294.21664608339694</v>
+      </c>
+      <c r="E14">
+        <v>294.45</v>
+      </c>
+      <c r="F14">
+        <v>1.5744281599999997E-3</v>
+      </c>
+      <c r="G14">
+        <v>1.5754600000000001E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27">
+      <c r="A15" s="42">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>312.35623159324001</v>
+      </c>
+      <c r="C15">
+        <v>312.06</v>
+      </c>
+      <c r="D15">
+        <v>294.35225488233681</v>
+      </c>
+      <c r="E15">
+        <v>294.75</v>
+      </c>
+      <c r="F15">
+        <v>1.9465498666666667E-3</v>
+      </c>
+      <c r="G15">
+        <v>1.937825E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27">
+      <c r="A16" s="42">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>318.26500700465544</v>
+      </c>
+      <c r="C16">
+        <v>317.77999999999997</v>
+      </c>
+      <c r="D16">
+        <v>294.57886130730265</v>
+      </c>
+      <c r="E16">
+        <v>295.33999999999997</v>
+      </c>
+      <c r="F16">
+        <v>2.9802457599999999E-3</v>
+      </c>
+      <c r="G16">
+        <v>2.887485E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="42">
+        <v>7</v>
+      </c>
+      <c r="B17">
+        <v>323.63862859035953</v>
+      </c>
+      <c r="C17">
+        <v>322.74</v>
+      </c>
+      <c r="D17">
+        <v>295.14325006184663</v>
+      </c>
+      <c r="E17">
+        <v>296.47000000000003</v>
+      </c>
+      <c r="F17">
+        <v>3.9183833599999995E-3</v>
+      </c>
+      <c r="G17">
+        <v>3.8479500000000002E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="42">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>318.30270436408495</v>
+      </c>
+      <c r="C18">
+        <v>318.13</v>
+      </c>
+      <c r="D18">
+        <v>299.22168943939931</v>
+      </c>
+      <c r="E18">
+        <v>299.95</v>
+      </c>
+      <c r="F18">
+        <v>2.5700625066666666E-3</v>
+      </c>
+      <c r="G18">
+        <v>2.51885E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="42">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>318.4829372796284</v>
+      </c>
+      <c r="C19">
+        <v>318.58</v>
+      </c>
+      <c r="D19">
+        <v>303.91148736331343</v>
+      </c>
+      <c r="E19">
+        <v>304.49</v>
+      </c>
+      <c r="F19">
+        <v>2.1235246933333334E-3</v>
+      </c>
+      <c r="G19">
+        <v>2.0999450000000002E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="42">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>318.80301197436296</v>
+      </c>
+      <c r="C20">
+        <v>319.00351000000001</v>
+      </c>
+      <c r="D20">
+        <v>308.65229050926581</v>
+      </c>
+      <c r="E20">
+        <v>309.03847999999999</v>
+      </c>
+      <c r="F20">
+        <v>1.5609421866666663E-3</v>
+      </c>
+      <c r="G20">
+        <v>1.4890823500000002E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="42">
+        <v>11</v>
+      </c>
+      <c r="B21">
+        <v>319.01289994963463</v>
+      </c>
+      <c r="C21">
+        <v>319.28005999999999</v>
+      </c>
+      <c r="D21">
+        <v>313.57345483397432</v>
+      </c>
+      <c r="E21">
+        <v>313.75484999999998</v>
+      </c>
+      <c r="F21">
+        <v>9.935384533333333E-4</v>
+      </c>
+      <c r="G21">
+        <v>1.0682052500000001E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="42">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <v>319.56472605071929</v>
+      </c>
+      <c r="C22">
+        <v>317.73446999999999</v>
+      </c>
+      <c r="D22">
+        <v>294.64494411853934</v>
+      </c>
+      <c r="E22">
+        <v>295.32715000000002</v>
+      </c>
+      <c r="F22">
+        <v>2.9378886400000001E-3</v>
+      </c>
+      <c r="G22">
+        <v>2.8806469500000003E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="42">
+        <v>13</v>
+      </c>
+      <c r="B23">
+        <v>318.40305616471557</v>
+      </c>
+      <c r="C23">
+        <v>317.72046</v>
+      </c>
+      <c r="D23">
+        <v>294.66788302030187</v>
+      </c>
+      <c r="E23">
+        <v>295.35687000000001</v>
+      </c>
+      <c r="F23">
+        <v>2.8567750399999996E-3</v>
+      </c>
+      <c r="G23">
+        <v>2.8756708999999997E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="42">
+        <v>14</v>
+      </c>
+      <c r="B24">
+        <v>318.70412169546893</v>
+      </c>
+      <c r="C24">
+        <v>318.26294000000001</v>
+      </c>
+      <c r="D24">
+        <v>294.74539495317856</v>
+      </c>
+      <c r="E24">
+        <v>295.41543999999999</v>
+      </c>
+      <c r="F24">
+        <v>3.0446920533333329E-3</v>
+      </c>
+      <c r="G24">
+        <v>3.2439937500000002E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="42">
+        <v>15</v>
+      </c>
+      <c r="B25">
+        <v>318.81776959447166</v>
+      </c>
+      <c r="C25">
+        <v>318.48025999999999</v>
+      </c>
+      <c r="D25">
+        <v>294.95517646294218</v>
+      </c>
+      <c r="E25">
+        <v>295.55029000000002</v>
+      </c>
+      <c r="F25">
+        <v>3.1019777066666663E-3</v>
+      </c>
+      <c r="G25">
+        <v>3.3747971000000002E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="42">
+        <v>16</v>
+      </c>
+      <c r="B26">
+        <v>318.56053255624283</v>
+      </c>
+      <c r="C26">
+        <v>318.41379000000001</v>
+      </c>
+      <c r="D26">
+        <v>294.88340227697375</v>
+      </c>
+      <c r="E26">
+        <v>296.52123999999998</v>
+      </c>
+      <c r="F26">
+        <v>2.7461594666666673E-3</v>
+      </c>
+      <c r="G26">
+        <v>2.8682699E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="42">
+        <v>17</v>
+      </c>
+      <c r="B27">
+        <v>318.51664490974343</v>
+      </c>
+      <c r="C27">
+        <v>318.17993000000001</v>
+      </c>
+      <c r="D27">
+        <v>295.00451737531392</v>
+      </c>
+      <c r="E27">
+        <v>295.77208999999999</v>
+      </c>
+      <c r="F27">
+        <v>2.8241684266666666E-3</v>
+      </c>
+      <c r="G27">
+        <v>3.0008037E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="42">
+        <v>18</v>
+      </c>
+      <c r="B28">
+        <v>318.3348782464065</v>
+      </c>
+      <c r="C28">
+        <v>317.89227</v>
+      </c>
+      <c r="D28">
+        <v>294.62908105804513</v>
+      </c>
+      <c r="E28">
+        <v>294.94614000000001</v>
+      </c>
+      <c r="F28">
+        <v>3.2108769066666668E-3</v>
+      </c>
+      <c r="G28">
+        <v>3.13639785E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="42">
+        <v>19</v>
+      </c>
+      <c r="B29">
+        <v>318.29827050530861</v>
+      </c>
+      <c r="C29">
+        <v>317.83413999999999</v>
+      </c>
+      <c r="D29">
+        <v>294.46046760050325</v>
+      </c>
+      <c r="E29">
+        <v>294.66298999999998</v>
+      </c>
+      <c r="F29">
+        <v>3.3036054400000002E-3</v>
+      </c>
+      <c r="G29">
+        <v>3.1832208500000001E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="42">
+        <v>20</v>
+      </c>
+      <c r="B30">
+        <v>318.3938189793015</v>
+      </c>
+      <c r="C30">
+        <v>318.14089999999999</v>
+      </c>
+      <c r="D30">
+        <v>294.62831839055224</v>
+      </c>
+      <c r="E30">
+        <v>294.798</v>
+      </c>
+      <c r="F30">
+        <v>9.7313013333333309E-4</v>
+      </c>
+      <c r="G30">
+        <v>9.6570500000000008E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="42">
+        <v>21</v>
+      </c>
+      <c r="B31">
+        <v>318.0786832403021</v>
+      </c>
+      <c r="C31">
+        <v>318.00878999999998</v>
+      </c>
+      <c r="D31">
+        <v>294.45689294842822</v>
+      </c>
+      <c r="E31">
+        <v>295.12842000000001</v>
+      </c>
+      <c r="F31">
+        <v>1.3370305066666666E-3</v>
+      </c>
+      <c r="G31">
+        <v>3.1146302000000002E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="42">
+        <v>22</v>
+      </c>
+      <c r="B32">
+        <v>318.26500700465544</v>
+      </c>
+      <c r="C32">
+        <v>317.47500000000002</v>
+      </c>
+      <c r="D32">
+        <v>294.57886130730265</v>
+      </c>
+      <c r="E32">
+        <v>295.42500000000001</v>
+      </c>
+      <c r="F32">
+        <v>2.9802457599999999E-3</v>
+      </c>
+      <c r="G32">
+        <v>3.0614349999999999E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="42">
+        <v>23</v>
+      </c>
+      <c r="B33">
+        <v>318.58325015595727</v>
+      </c>
+      <c r="C33">
+        <v>317.59199999999998</v>
+      </c>
+      <c r="D33">
+        <v>294.73300062382947</v>
+      </c>
+      <c r="E33">
+        <v>295.40800000000002</v>
+      </c>
+      <c r="F33">
+        <v>1.8809364341085273E-3</v>
+      </c>
+      <c r="G33">
+        <v>2.9427200000000002E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="42">
+        <v>24</v>
+      </c>
+      <c r="B34">
+        <v>319.27722725851919</v>
+      </c>
+      <c r="C34">
+        <v>317.73099999999999</v>
+      </c>
+      <c r="D34">
+        <v>294.71908408877823</v>
+      </c>
+      <c r="E34">
+        <v>295.36700000000002</v>
+      </c>
+      <c r="F34">
+        <v>1.5352870399999998E-3</v>
+      </c>
+      <c r="G34">
+        <v>2.7862800000000004E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="42">
+        <v>25</v>
+      </c>
+      <c r="B35">
+        <v>318.41165201005003</v>
+      </c>
+      <c r="C35">
+        <v>317.86700000000002</v>
+      </c>
+      <c r="D35">
+        <v>294.40166457286438</v>
+      </c>
+      <c r="E35">
+        <v>295.315</v>
+      </c>
+      <c r="F35">
+        <v>8.5928448000000001E-4</v>
+      </c>
+      <c r="G35">
+        <v>2.6076800000000002E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="42">
+        <v>26</v>
+      </c>
+      <c r="B36">
+        <v>319.10031185031147</v>
+      </c>
+      <c r="C36">
+        <v>317.99400000000003</v>
+      </c>
+      <c r="D36">
+        <v>294.37408177408201</v>
+      </c>
+      <c r="E36">
+        <v>295.26</v>
+      </c>
+      <c r="F36">
+        <v>8.9403596384000003E-5</v>
+      </c>
+      <c r="G36">
+        <v>2.4034E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Complete the case 19 with md coefficient of 3.28e-7 Add FLUENT files 16GGQ-3-19.cas & dat
</commit_message>
<xml_diff>
--- a/bin/2d_s_cc/reorganized exp.data.xlsx
+++ b/bin/2d_s_cc/reorganized exp.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="75" windowWidth="17235" windowHeight="8955" activeTab="3"/>
+    <workbookView xWindow="2340" yWindow="75" windowWidth="17235" windowHeight="8955" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Wang&amp;Chung2008CES" sheetId="1" r:id="rId1"/>
@@ -262,7 +262,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="158">
   <si>
     <t>Wang K Y, Chung T S, Gryta M. Chem. Eng. Sci., 2008, 63: 2587-2594</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -793,6 +793,9 @@
   </si>
   <si>
     <t>16GGQ-3-18</t>
+  </si>
+  <si>
+    <t>16GGQ-3-19</t>
   </si>
 </sst>
 </file>
@@ -1422,23 +1425,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="178368512"/>
-        <c:axId val="178370816"/>
+        <c:axId val="139702656"/>
+        <c:axId val="139704192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="178368512"/>
+        <c:axId val="139702656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="178370816"/>
+        <c:crossAx val="139704192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="178370816"/>
+        <c:axId val="139704192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1446,7 +1449,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="178368512"/>
+        <c:crossAx val="139702656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1460,7 +1463,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3172,11 +3175,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="T42" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="X42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X56" sqref="X56"/>
+      <selection pane="bottomRight" activeCell="Y56" sqref="Y56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -6082,8 +6085,8 @@
       <c r="X55" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="Y55" s="39">
-        <v>19</v>
+      <c r="Y55" s="39" t="s">
+        <v>157</v>
       </c>
       <c r="Z55" s="39" t="s">
         <v>148</v>
@@ -6166,8 +6169,8 @@
       <c r="X56" s="42">
         <v>318.14089999999999</v>
       </c>
-      <c r="Y56" s="39">
-        <v>318.00878999999998</v>
+      <c r="Y56" s="21">
+        <v>317.99880000000002</v>
       </c>
       <c r="AA56" s="39">
         <v>317.47500000000002</v>
@@ -6247,8 +6250,8 @@
       <c r="X57" s="42">
         <v>294.798</v>
       </c>
-      <c r="Y57" s="39">
-        <v>295.12842000000001</v>
+      <c r="Y57" s="21">
+        <v>294.93329999999997</v>
       </c>
       <c r="AA57" s="39">
         <v>295.42500000000001</v>
@@ -6328,8 +6331,8 @@
       <c r="X58" s="42">
         <v>1.9314100000000001</v>
       </c>
-      <c r="Y58" s="39">
-        <v>6.2292604000000003</v>
+      <c r="Y58" s="21">
+        <v>2.67977</v>
       </c>
       <c r="AA58" s="39">
         <v>6.1228699999999998</v>
@@ -6422,7 +6425,7 @@
         <v>3.13639785E-3</v>
       </c>
       <c r="V59" s="24">
-        <f t="shared" ref="V59:X59" si="38">V58*0.0005</f>
+        <f t="shared" ref="V59" si="38">V58*0.0005</f>
         <v>3.1832208500000001E-3</v>
       </c>
       <c r="W59" s="24"/>
@@ -6432,7 +6435,7 @@
       </c>
       <c r="Y59" s="24">
         <f t="shared" si="39"/>
-        <v>3.1146302000000002E-3</v>
+        <v>1.3398850000000001E-3</v>
       </c>
       <c r="AA59" s="24">
         <f t="shared" si="39"/>
@@ -6536,7 +6539,7 @@
       </c>
       <c r="Y60" s="24">
         <f t="shared" ref="Y60:AA60" si="50">(Y43-Y56)/Y43</f>
-        <v>2.1973569429460568E-4</v>
+        <v>2.511430174707145E-4</v>
       </c>
       <c r="AA60" s="24">
         <f t="shared" si="50"/>
@@ -6640,7 +6643,7 @@
       </c>
       <c r="Y61" s="24">
         <f t="shared" ref="Y61:AA61" si="61">(Y47-Y57)/Y47</f>
-        <v>-2.2805614935609564E-3</v>
+        <v>-1.6179178106562233E-3</v>
       </c>
       <c r="AA61" s="24">
         <f t="shared" si="61"/>
@@ -6745,7 +6748,7 @@
       </c>
       <c r="Y62" s="55">
         <f t="shared" ref="Y62:AA62" si="71">(Y48-Y59)/Y48</f>
-        <v>-1.3295131894671905</v>
+        <v>-2.1349500397339002E-3</v>
       </c>
       <c r="AA62" s="55">
         <f t="shared" si="71"/>
@@ -6849,7 +6852,7 @@
       </c>
       <c r="Y63" s="24">
         <f t="shared" ref="Y63:AA63" si="82">SQRT(Y60^2+Y61^2+Y62^2)</f>
-        <v>1.3295151635884876</v>
+        <v>2.6904911316379962E-3</v>
       </c>
       <c r="AA63" s="24">
         <f t="shared" si="82"/>
@@ -10405,8 +10408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10544,7 +10547,9 @@
       <c r="A14" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="B14" s="21"/>
+      <c r="B14" s="23">
+        <v>3.2800000000000003E-7</v>
+      </c>
       <c r="C14" s="22">
         <v>2.23E-7</v>
       </c>
@@ -10565,7 +10570,9 @@
       <c r="A16" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="B16" s="21"/>
+      <c r="B16" s="21">
+        <v>317.99880000000002</v>
+      </c>
       <c r="C16">
         <v>318.14089999999999</v>
       </c>
@@ -10580,7 +10587,9 @@
       <c r="A17" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="B17" s="21"/>
+      <c r="B17" s="21">
+        <v>294.93329999999997</v>
+      </c>
       <c r="C17">
         <v>294.798</v>
       </c>
@@ -10595,7 +10604,9 @@
       <c r="A18" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="B18" s="21"/>
+      <c r="B18" s="21">
+        <v>2.67977</v>
+      </c>
       <c r="C18">
         <v>1.9314100000000001</v>
       </c>
@@ -10610,7 +10621,10 @@
       <c r="A19" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="B19" s="21"/>
+      <c r="B19" s="42">
+        <f>B18*0.0005</f>
+        <v>1.3398850000000001E-3</v>
+      </c>
       <c r="C19" s="42">
         <f>C18*0.0005</f>
         <v>9.6570500000000008E-4</v>
@@ -10927,7 +10941,7 @@
       </c>
       <c r="V3">
         <f>'Yao2016(preparing)'!Y56</f>
-        <v>318.00878999999998</v>
+        <v>317.99880000000002</v>
       </c>
       <c r="W3">
         <f>'Yao2016(preparing)'!AA56</f>
@@ -11143,7 +11157,7 @@
       </c>
       <c r="V5">
         <f>'Yao2016(preparing)'!Y57</f>
-        <v>295.12842000000001</v>
+        <v>294.93329999999997</v>
       </c>
       <c r="W5">
         <f>'Yao2016(preparing)'!AA57</f>
@@ -11359,7 +11373,7 @@
       </c>
       <c r="V7">
         <f>'Yao2016(preparing)'!Y59</f>
-        <v>3.1146302000000002E-3</v>
+        <v>1.3398850000000001E-3</v>
       </c>
       <c r="W7">
         <f>'Yao2016(preparing)'!AA59</f>
@@ -11876,19 +11890,19 @@
         <v>318.0786832403021</v>
       </c>
       <c r="C31">
-        <v>318.00878999999998</v>
+        <v>317.99880000000002</v>
       </c>
       <c r="D31">
         <v>294.45689294842822</v>
       </c>
       <c r="E31">
-        <v>295.12842000000001</v>
+        <v>294.93329999999997</v>
       </c>
       <c r="F31">
         <v>1.3370305066666666E-3</v>
       </c>
       <c r="G31">
-        <v>3.1146302000000002E-3</v>
+        <v>1.3398850000000001E-3</v>
       </c>
     </row>
     <row r="32" spans="1:7">

</xml_diff>

<commit_message>
Remove the folder of /case_20160831_yao.cl/ Remove base.cas & dat The sim results have a great difference while new UDFs are applied. Optimize the md coefficient as 8.88e-7 and add the FLUENT case and date file for v3.2 (16GGQ-3.2-20 and 16GGQ-3.2-24)
</commit_message>
<xml_diff>
--- a/bin/2d_s_cc/reorganized exp.data.xlsx
+++ b/bin/2d_s_cc/reorganized exp.data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="75" windowWidth="17235" windowHeight="8955" activeTab="1"/>
+    <workbookView xWindow="2340" yWindow="75" windowWidth="17235" windowHeight="8955" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Wang&amp;Chung2008CES" sheetId="1" r:id="rId1"/>
@@ -262,7 +262,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="161">
   <si>
     <t>Wang K Y, Chung T S, Gryta M. Chem. Eng. Sci., 2008, 63: 2587-2594</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -796,6 +796,15 @@
   </si>
   <si>
     <t>16GGQ-3-19</t>
+  </si>
+  <si>
+    <t>16GGQ-3.2-20</t>
+  </si>
+  <si>
+    <t>Exp. JM</t>
+  </si>
+  <si>
+    <t>Linearly corr. MDC</t>
   </si>
 </sst>
 </file>
@@ -1425,23 +1434,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="139702656"/>
-        <c:axId val="139704192"/>
+        <c:axId val="204928896"/>
+        <c:axId val="204930432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="139702656"/>
+        <c:axId val="204928896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139704192"/>
+        <c:crossAx val="204930432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="139704192"/>
+        <c:axId val="204930432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1449,7 +1458,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139702656"/>
+        <c:crossAx val="204928896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1463,7 +1472,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3179,7 +3188,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="X42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y56" sqref="Y56"/>
+      <selection pane="bottomRight" activeCell="AA48" sqref="AA48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -10406,10 +10415,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:B18"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10649,6 +10658,117 @@
       <c r="C21" s="22">
         <f>(0.0009731-D19)*(D14-E14)/(D19-E19)+D14</f>
         <v>2.2332356069098329E-7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="B23" s="42" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="B24" s="42"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" s="22">
+        <v>8.8800000000000001E-7</v>
+      </c>
+      <c r="C25" s="23">
+        <v>3.2800000000000003E-7</v>
+      </c>
+      <c r="D25" s="22">
+        <v>6.9999999999999997E-7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" s="42"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="B27">
+        <v>317.49423000000002</v>
+      </c>
+      <c r="C27" s="21">
+        <v>317.97573999999997</v>
+      </c>
+      <c r="D27">
+        <v>317.62227999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28">
+        <v>295.37509</v>
+      </c>
+      <c r="C28" s="21">
+        <v>294.91201999999998</v>
+      </c>
+      <c r="D28">
+        <v>295.25033999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="B29">
+        <v>5.7986893999999998</v>
+      </c>
+      <c r="C29" s="21">
+        <v>2.6637732999999999</v>
+      </c>
+      <c r="D29">
+        <v>4.8526243999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" s="42">
+        <f>B29*0.0005</f>
+        <v>2.8993447000000001E-3</v>
+      </c>
+      <c r="C30" s="42">
+        <f>C29*0.0005</f>
+        <v>1.33188665E-3</v>
+      </c>
+      <c r="D30" s="42">
+        <f>D29*0.0005</f>
+        <v>2.4263122E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="B31">
+        <f>'Yao2016(preparing)'!AA48</f>
+        <v>2.9802457599999999E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="B32" s="22">
+        <f>(B31-C30)*(C25-D25)/(C30-D30)+C25</f>
+        <v>8.8828442402500554E-7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>